<commit_message>
fix data & add grade.py
</commit_message>
<xml_diff>
--- a/repo/topic_list.xlsx
+++ b/repo/topic_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,21 +465,21 @@
         <v>-1</v>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-1_台北市_市府_高雄_路面</t>
+          <t>-1_台北市_信義區_地層下陷_坑洞</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['台北市', '市府', '高雄', '路面', '四川', '道路', '台北', '坍塌', '鄉', '下陷']</t>
+          <t>['台北市', '信義區', '地層下陷', '坑洞', '路面', '道路', '坍塌', '北市', '下陷', '當地']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['張信 哲杜拜 站 演唱 會 原定 2 月 登場   後 來 撞 上 極端 氣候 出現 冰雹   淹水 災害   因而 延期 至 端午 假期 6 月 9 日舉行   他 笑 說     很 開心   差點 變成 不是 第一 個     透露 目前 已經 很多 歌手   陸續 安排 開唱 計畫   原本 很 擔心 阿拉伯 國家 演出 會 很多 限制   像是 有些 景點 不能 比 出 特定 手勢   演唱 會太過 喧鬧   後 來 才 發現 他們 對 外國人 很 禮遇   很 支持 娛樂 活動     第一次 得知 邀請 時   張信哲 心想     真的假 啦   有人 要 聽     過往 都 只有 杜拜 轉機 經驗   從 未 入境 過旅遊 他 說     他們 來 邀 請 時 就 說   以中 東來 說 這邊 是 華人 最 多 地方   30 萬人     杜拜位 處國際 航班 交通 樞紐   因此 有來 自 歐洲   俄羅斯 華人 歌迷   特地 飛來 欣賞 演唱 會   因為 天災 延期 開唱   歌迷 們 沒 太 多 抱怨 問題   把 票 留著 就 為 了 等到 正式 演出 這 一天 朝聖     首次 前進 沙漠 開唱   張信哲 歌喉 完全 沒有 受 影響     還好   場館 冷氣 很足   我 提前 4 天來   杜拜   調時 差     本來 就 沒 計畫 要 衝場 次 演出   1 週 1 場已 是 最大 限度     未來式   巡演 開唱 6 年   亞洲 站 預計 至 2024 年底 結束   前進 海外 開唱   他 最 想 攻 佔 場館 是 英國倫敦 皇家 阿爾伯特 音樂廳   Royal   Albert   Hall       張信 哲新 專輯 已經 籌備 中   下半年 會釋 出 更 多 新歌   台北 小 巨蛋   高雄 巨蛋 演唱 會   則要 排到 2025 年 才能 開唱     第一 個 要 搶 時間   現在 場館 太難 搶 了     記者 提議 大 巨蛋 開唱   張信哲 卻 謙虛回     大 巨蛋 周董   周杰倫   都 還排 不到   哪 還輪 到 我   等 別人 有空 給我用   我 再 用 就 好       歌神 張學友 因為 身體 不適   日前 取消 台北 站 演唱 會   張信哲 關注 此事     好 害怕   我 吃 增強 免疫力 的藥   醫生開     即將 前進 海拔 2000 多 公尺 青海 西寧站 開唱   張信哲 提到   前輩   薛之謙唱 到 吸氧 氣   私下 還嚇 他     一定 不要 亂動   不要 突然 爆衝    ', '台北市 信義區 崇德 街一處 新建 工地 旁 道路   13 日 發生 地層下陷   晚間 緊急 灌漿 搶 救   晚間 11 時 坑洞 初步 填平 完成   附近 住戶 一 早就 跑 來 關心 自己 攤位   擔心會 再次 坍塌   北市 都 發局 長 王玉芬 視察 表示   初步 判斷 道路 塌陷 原因 是   因 工地 地下 連續 壁 約 11 至 12 公尺 處有 破口   水 與 砂往 地下室 流 造成 坑洞   未來 一周 將會 同三大技師 公會 全面 檢查 地下室 開挖 工地   避免 類似 意外 再度 發生   台北市 信義區 崇德 街一處 新建 工地 旁 巷道   13 日 下午 突然 發生 地層下陷   坑洞 長 約 15 公尺   寬 3 公尺   深度 3 公尺   北市 勒令 工地 停工   附近 住戶 一 早就 跑 來 關心 自己 攤位   擔心會 再次 坍塌   周邊 住戶 說     昨晚 11   12 點還 沒 睡覺   早上 5   6 點又趕 快 跑 出來 看   是 要 關心 一下 我 自己 攤位   希望 說 沒 下 一次 啦     信義區 區長 陳 冠伶 表示     安置 了 5 戶   一共 是 10 位   那現 我們 把 他們 都 安置 我們 信義區 旅館裡     台北 市長 蔣萬安 上午 前往 旅館 探視 安置 戶   致贈慰 問金 以及 康乃馨   報告 工程 搶修 進度   蔣萬安 提及     接下 來 我們 還是 要 持續 監測   第二 個 我們 會 請 土木 技師 來 整體 評估     初步 了解   因連續 壁體 滲水 造成 地下水 湧入 引發 道路 坍陷   現場 隨即 進行 緊急 處置   基地 外 道路 下陷 處 進行 灌漿 回填   基地 內採 填砂 灌水 以 平衡 水壓   北市 府 都 發局 長 王玉芬 解釋     初步 判斷 是 工地 裡面 地下 連續 壁   大約 11 到 12 公尺 之間 破口   所以 它 水 跟 砂會 往 地下室 裡面 流   才 造成 這個 坑洞     為 了 避免 類 似的 工地 意外 再度 發生   蔣萬安 指出   已責成 相關局 處針 對 北市 工地 全面 清查   目前 建築 工地 正在 開挖 階段 102 件   將由三大 專業 公會 逐案 現場 勘查   於 一週 內檢 查完 畢   屆 時 安全 疑慮者將 下令 停工   改善  ', '台北市 信義區 崇德 街今   13   日 下午 3 點 13 分   傳出 一處 新建 案 工地 旁 道路   地層下陷     馬 路上 出現 一個 長 15 公尺   寬 3 公尺   深度 約 4 公尺 天坑   摩托 車   腳踏車 都 掉入 坑洞   一旁 住戶 家門口 更是 危險   懸空     而 台北 市長 蔣萬安 稍早 前往 現場 勘查   受訪 時 表示   第一 時間 就 即刻 派員前 來   相關 單位 了 緊急 疏散   強調   當這次 事件 緊急 處置 告一段落 之 後   會 台北市 相關 工地 全面 清查   了解 是否 有類 似 這次 地面 坍塌 原因   積極 相關 處置   目前 對廠 商及 建築師 各 開罰 9 萬元   工地 勒令停工   蔣萬安 表示   初步 了解   聽 了 相關 單位 說明   我們 下午 3 點 13 分   消防局 接收 到 地方 反應 這邊 地層下陷   第一 時間 就 即刻 派員前 來   趕快 連絡 了 警察局   新工處   建管處   區 公所   自來 水處   瓦斯 公司   台電 等 相關 單位   了 緊急 疏散   蔣萬安 指出   跟 指揮官   相關 單位 來 說明   第一   人員 安全 最 重要   所以 相關 緊急 應變 處置 必須 盡速 完成   包括 疏散   安置 等等   將這次 地面 坍塌 可能 造成 損害 降到 最低   第二   就 旁邊 工地   目前 了解 可能 是 連續 壁 滲水 問題   已經 趕快 了 處理   盡速 找出 坍塌 原因   然後盡 快 排除   避免 坍塌 面積 持續 擴大   第三   會 就 這次 地面 坍塌 事件 進行 調查   當然 包括 工地 實施者   營造 商過 去 相關 紀錄   第四   當這次 事件 緊急 處置 告一段落 之 後   要 台北市 相關 工地 全面 清查   了解 是否 有類 似 這次 地面 坍塌 原因   要積 極來 相關 處置   蔣萬安 表示     我們 現在 已經 非常 努力 緊急 應變   處置   第一 時間 盡快 疏散 了 住戶   我 想 市民 朋友 安全 是 最 重要   目前 還在 緊急 處置   我 想 必要 話 我們 還是 希望 預防性 疏散     而 台北市 土木 技師 公會 理事 長 莊均緯 指出   還要 再 把 崩塌 孔洞 填補 完成   現在 還在 灌水 當中   水頭 差會 慢慢 達到 平衡   而 因 地質 條件屬 於 沙 跟 水   因此 擔心 擋 土 設施 破洞   只要 衝破 連續 壁 洞   勢必 擋 土 牆後面 會 崩塌   目前 要 把 崩塌 部分 用 混 泥土 灌足外   開 挖面 水平衡   只要 水 與 地下水位 一 平衡   土沙 部分 就 會靜止   就 不會 往開 挖面 流動   防止 二次 下陷   目前 搶救 可控 範圍   莊均緯 表示   通常 會 發生 這狀況   是 地面 本來 就 下陷   只是 下陷 又 再 造成 第二 崩塌   灌漿 部分 還是 從 最 底下 往上 灌   表層 部分 基本上 還是 有些 鬆 動   需要 等 水位 平衡 後   才能 達到 搶災 最終 停止 狀態   估計 應該 都 要 到 凌晨  ']</t>
+          <t>['北市 近日 連續 出現 天坑   市長 蔣萬安 昨天下午 公安 會報 中   指示 工務局 邀集 都 發   建管 等 相關 單位   針對 道路 塌陷   制定 通案 性處 理機 制外   應 全面 檢視   清查 地下 老舊 管線   下 一步 再針 對 其他 地方   避免 再 發生 地層下陷 情形       北市 建管處 昨天下午 公安 會報   針對 今年 5 月 13 日 信義區 崇德 街 60 巷道 路 塌陷 案 進行 專題 報告   北市 開挖 中 建築 工地 計有 102 件   已委 託 台北市 土木 技師 公會   台北市 建築師 公會   台北市 結構 工程 工業 技師 公會   從 5 月 15 日起 逐案 現勘   包括 觀測 項目 是否 設置   是否 按計畫 觀測   以及 施工 計畫   例如 是否 抽水 計畫 等   已 全數檢 查完 畢   針對 檢查 項目 不 符合 建築 工地   要求 停工 釐 清 改善                             為 加強 建築 工地 開挖 階段 安全 管理   6 月 起委 託 三 大公 會 不定期 現勘   並就 建築 工地 因違 反建築法 公共安全   公共交通 受裁罰 或 勒令停工 案件   同步 於 建管處 網站 揭露 裁處訊息       建管處 表示   已 函告 工地   若 發生 公安 意外   應 於 第一 時間 主動 通報 原因 緊急 應變 處理 情形   未通 報者   將依建築 法相 關規定 加重 裁罰   最高 處 9 萬元 罰款   情節 嚴重 時 還會 勒令停工       最近 常發 生午 後 雷雨   市長 蔣萬安 副 市長 李 四川 都 強調 要 注意   李 四川 提醒 建管處   開挖 中 工地 要 加強 宣導 防範       蔣萬安說   信義區 案例   主因 為 建案 開 挖 造成 地層下陷   最近 許多 下午 暴雨   可能 造成 地層下陷   請 建管處 加強 工地 管理 查核       蔣萬安 指示   針對 有些 地方 老舊 管線   像是 汙水 管等   主管 機關加 強督導   另環 保局 進行 清疏 時   或是 新工處 地面 上 施工   發現 相關 管線 鬆 脫 或 破裂 情形   要 即 時 通報 相關 單位 處理       建管處 指出   地下 管線 一旦 老舊 可能 鬆 脫   造成 漏水   淘空 地基   導致 地層下陷 隱憂  ', '北市 信義區 崇德 街 60 巷鄰近 一處 新建 工地   今天下午 3 點多 路面 突然 下陷   出現 一個 大 天坑   台北市 副 市長 李 四川   都 發局 長 王玉芬 傍晚 抵達 了解 現況   王 說 明處理 進度   住戶 方面 已 撤離 16 戶   工程 則在 坑洞 灌漿   建案 基地 灌水       都 發局 長 王玉芬 到場 表示   馬 路上 坑洞 約 10 幾 公尺 長   3 公尺 寬   深度 判斷 達 到 3 公尺   以 灌漿 方式 處理   建築 基地 開挖 地下室 部分   是 用 消防 水車 拉水線 灌水   使內外 壓力 可以 平衡   已拉 兩條 水線   再 請 消防局 再拉一條   加快 灌水 速度                             王玉芬 說 明住 戶 部分   已經 撤離 16 戶   10 人 需要 安置 且 安置 妥當 某 一家 旅館   所有 住宿   日常 開銷 都 會 由 營造 單位 負責   其餘住 戶 由 台北市 結構 技師 公會 判斷 沒有 危險   因 居民 擔心   請里長 逐戶 安撫   現場 分為 撤離區 監測區   除了 天坑 之外   轉角 一戶 地下室   技師 下去 看   目前 還沒有 任何 影響   會持續 監測       黃 住 當地 20 多年   他 提到 走路 經過 時   看到 裂一個 小洞   下午 2 點多 就 一直 下陷   從 22 號先 坍 下去   住戶 鄭 表示   他 姊姊 騎車 來 時   突然 聽到   砰   一聲 被 嚇到   那時 就 一個 小洞   自己 走 出去 看   前 後 不到 一分 鐘出 現好 大一個 洞 就 停住 了   沒 多久 警察 到場 就 要求 不要 過去   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影', '台北市 信義區 崇德 街一處 新建 工地 旁 道路   13 日 發生 地層下陷   晚間 緊急 灌漿 搶 救   晚間 11 時 坑洞 初步 填平 完成   附近 住戶 一 早就 跑 來 關心 自己 攤位   擔心會 再次 坍塌   北市 都 發局 長 王玉芬 視察 表示   初步 判斷 道路 塌陷 原因 是   因 工地 地下 連續 壁 約 11 至 12 公尺 處有 破口   水 與 砂往 地下室 流 造成 坑洞   未來 一周 將會 同三大技師 公會 全面 檢查 地下室 開挖 工地   避免 類似 意外 再度 發生   台北市 信義區 崇德 街一處 新建 工地 旁 巷道   13 日 下午 突然 發生 地層下陷   坑洞 長 約 15 公尺   寬 3 公尺   深度 3 公尺   北市 勒令 工地 停工   附近 住戶 一 早就 跑 來 關心 自己 攤位   擔心會 再次 坍塌   周邊 住戶 說     昨晚 11   12 點還 沒 睡覺   早上 5   6 點又趕 快 跑 出來 看   是 要 關心 一下 我 自己 攤位   希望 說 沒 下 一次 啦     信義區 區長 陳 冠伶 表示     安置 了 5 戶   一共 是 10 位   那現 我們 把 他們 都 安置 我們 信義區 旅館裡     台北 市長 蔣萬安 上午 前往 旅館 探視 安置 戶   致贈慰 問金 以及 康乃馨   報告 工程 搶修 進度   蔣萬安 提及     接下 來 我們 還是 要 持續 監測   第二 個 我們 會 請 土木 技師 來 整體 評估     初步 了解   因連續 壁體 滲水 造成 地下水 湧入 引發 道路 坍陷   現場 隨即 進行 緊急 處置   基地 外 道路 下陷 處 進行 灌漿 回填   基地 內採 填砂 灌水 以 平衡 水壓   北市 府 都 發局 長 王玉芬 解釋     初步 判斷 是 工地 裡面 地下 連續 壁   大約 11 到 12 公尺 之間 破口   所以 它 水 跟 砂會 往 地下室 裡面 流   才 造成 這個 坑洞     為 了 避免 類 似的 工地 意外 再度 發生   蔣萬安 指出   已責成 相關局 處針 對 北市 工地 全面 清查   目前 建築 工地 正在 開挖 階段 102 件   將由三大 專業 公會 逐案 現場 勘查   於 一週 內檢 查完 畢   屆 時 安全 疑慮者將 下令 停工   改善  ']</t>
         </is>
       </c>
     </row>
@@ -488,21 +488,21 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0_台北市_鄰損_大樓_建物</t>
+          <t>0_台北市_消防局_巷道_市府</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['台北市', '鄰損', '大樓', '建物', '市府', '損鄰', '台北', '中山', '建設', '高雄']</t>
+          <t>['台北市', '消防局', '巷道', '市府', '街', '信義區', '地層下陷', '坑洞', '鄰近', '巷']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['基泰 建設位 台北市 大直 新建 案 去   2023   年 9 月 7 日 晚間 突然 發生 崩塌   導致 附近 5 樓 民宅 下陷 成 4 樓   台北 地檢署 偵查 終結   將 工地 邱姓 負責人   基泰 公司 工程部 人員 張姓 工地 主任   王姓 劉姓 建築師   姜姓 專案 人員 等 5 人   依涉 犯 違背 建築術 成規   偽造 文書 等 罪 起訴   檢方 查出   大直 基泰 建案 坍塌 後   所幸 住戶 時 撤離   無人 傷亡   檢方 發現 建案 商未 依圖 施工   應該 60 公分 厚 連續 壁   只施作 50 公分   此外   建商 為 了 趕工   改變 施工 順序   竟 調整 監測 異常數 據   導致 工安 意外   至於 基泰 董事 長 陳 世銘 等 2 人 被控 殺人 未遂 部分 則 予以 簽結  ', '台北 捷運 信義線 東延段 工程   疑似 造成 松山 家商 校舍 下陷 5 公分   引發 安全 疑慮   直擊 北市 福德街   住戶 反映   下陷 情況 相當 明顯   連房價 都 跌 了   對此 台北市 捷運局 表示   已 安排 台北市 結構 技師 公會 辦理 結構 安全 鑑定   同時 已針 對 周邊 建物 鄰房 損壞 部分   進行 立即 修繕 作業   台北 捷運 信義線 東延段 工程   2016 年 開工 至今   工程 目前 還在 進行 中   不過 近期 北市 議員接 獲民眾 陳 情   說 先前 開 挖 工程   釀成 鄰近 建物 塌陷   實際到 現場 一看   發現 原本 馬 路 是 平   但 塌陷 狀況 確實 越來 越 明顯   附近 住戶 說     對   本來 都 是 平   這邊 全部 都 下陷   我 就 住 二樓   那個 球 很 明顯 從 這樣 滑下去     說 到 地層下陷   附近 住戶 超級 有感   北市 福德街 一旁 騎樓   明顯 受到 捷運開 挖 工程 影響   下陷 相當 嚴重   連住 戶 都 直呼   這裡 房價 都 跌 了     里長 更 指出   福德街 51 巷到 89 巷是 影響 最明顯 地方   附近 住戶 擔心 說     補 了 沒用   看 就 這樣   結構 已經 不行 了   除非 重建     對此 台北市 土木 技師 公會 理事 長 莊均緯 表示     通常 捷運 施工 比較 容易 下陷 部分   就 是非 結構體   像是 水溝   人行道   瓷磚 部分   要 安全 檢測   看 是否 造成 結構 上 問題     而 松山 家商 校舍 被 發現 下陷 狀況   議員 指出   經過 一年 監測   確認 已經 下陷 約 5 公分   安全 疑慮 浮上 檯 面   捷運 工程局 承包商   趕緊 進行 結構 補強   施作 地質 鑽 探作業   要 確認 校舍 承受能力   台北市 政府 捷運局 第二 工程 處 主任 陳 建仁則 表示   110 年 9 年 接到 學校 通報   監測 作業 進行 修繕   今年 暑假 陸續 修繕 完成   這個 月 安全 鑑定   兩個 月 後 就 安全 報告   而 台北 捷運局 表示   施工期 間 因為 極端 地質 水文 條件 不利   釀成 地下 土層 沉陷   目前 已經 安排 結構 安全 鑑定   並進行 立即 修繕   捷運 施工 周邊 建物   都 有安裝 建物 監測 儀器   按時 觀測 監控   研判 施工 是否 再 造成 影響  ', '台北市 中山 大直 街 94 巷 周邊 民宅 嚴重 塌陷   市長 蔣萬安強 調   會 徹底 調查 建管處 處理 過程 是否 違失     絕不寬貸   護短     同時 會 檢視 基泰 建設 台北市 建案   不合 規定 就 會 勒令停工   北市 府 成立 律師團 協助 住 戶後續 追償   蔣萬安今   8 日   接受 資深 媒體 人 黃 光芹 主持 節目 專訪   坦言 建管處 4   5 月 收到 住戶 書面 申訴 牆壁 龜裂   獲報 後 派員 了解   當時 認為 與 基泰 建設 開 挖 無 直接 相關   而 當時 仍施 作連續 壁   直至 7 月 24 日才 開 挖   至於 大直 災民 安置 問題   蔣萬安 表示   會 找 時間 了解 住戶 需求   昨   7 日   就 成立 群組   包含 民政局   社會局   衛生局 等 局處   需要 領藥 開綠色 通道 至 台北市 聯合 醫院   後 續 會 協助 住戶 追究 責任   求償   至於 市議員陳怡 君質疑   住戶僅 被 安置 1 天   蔣萬安否 認   目前 安置 到 11 日   即刻 請觀 傳局 了解   協調 旅宿業者   以 降低 大家 搬動   當然 住戶 不想 住 那麼 長   只要 確認 安全 無虞   就 會 讓 住戶 回去   蔣萬安強 調   將 重新 檢視   調查 事情 原委   包含 住戶 起初 提出 申訴   建管處 判斷 過程 是否 違失 或 違法   才 導致 今天 狀況     絕不寬貸   絕不護 短     若 發現 是 機制   SOP 出 了 問題 就 會 修正   蔣萬安 提及   台北 30 年 以上 老舊 建物 超過 7 成   危老 都 更案 經常 緊臨 老房子   現在 危老 都 更 都 會 較 過往 開 挖 來 深   基泰 大直 就 開 挖 到 地下 3 層   故會 要求 建管處 增加 查核 頻率   尤其 地下 深開 挖 部分 要 確保 施工 安全   黃 光芹 詢問   是否 可能 要求 任何 局處 首長 下台 或 撤 職來 負責   蔣萬安 回應   只要 徹底 調查 發現 任何 違法 情事   或 發現 當時 處理 不當   表態   該換 就換   這沒有 疑問     強調 重新 檢視 後   需要 撤換 就 撤換     至於 基泰 建設 台北 尚有 4 個 建案 是否 會 要求 全面 停工   蔣萬安 回應   會 全面 檢視 基泰 建設 台北市 所有 建案   包含 今日 已 派員去 基泰 建設 勞檢   會 檢視 相關 施工 是否 合乎 規定   若未 依規 就 會 依法 勒令停工   蔣萬安稱   北市 府 已 成立 跨局 處 一站式 聯合 服務 中心   成立 律師團 協助 住 戶後續 求償   他 下午 再度 前往 視察時   重申 要 重檢視 北市 建物   而 北市 府 會 向 建商 與 施工 廠商 追究 到底   蔣萬安 撂 狠話     建商 要負 全面 責任   否則 未來 台北市   很 抱歉   不 符合 相關 規定 或 標準 就 別 想 台北市 取得 任何 案子     而 下午 建管處 已經 發文稱 基泰 北市 7 個 工地 全面 停工  ']</t>
+          <t>['台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶 10 多人   並劃 設緊 戒線   並 通知 市府 相關 單位 到場 處理       天坑 位 於 新建 工地 民宅 中間 巷弄 道路   塌陷 時 發出 聲響   驚動 住戶   但 因為 坑洞 擋 在家 門前   第一 時間 無法 脫困   消防局 緊急 到場   以 爬梯 方式 救援 住戶 出來                             消防局 救出 2 名 女子   疏散 1 男 1 女   人員 已 全數 疏散 完畢   另外 1 名 85 歲 老婦   因長 期行動 不便   雖無外傷   意識 清醒   但家屬 要求 預防性 送醫   由 消防局 送北醫   由 於 天坑 危及 安全   影響 周遭 至少 五戶 民宅   部分 住戶 無法 回家   估計 10 餘人受 影響   將由 台北市 府 處理 安置 問題       台北市 信義區 出現 天坑   目前 市府 新工處   建管處   勞檢處 等 相關 單位 都 已 派 人 到場   現場 設置 指揮 所   初步 懷疑 與 民宅 對面 新建 工地 工程 有關   現以 灌漿 方式 緊急 處置   至於 天坑 出現 原因   將 交由 市府 建管   新工 等 單位 調查   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝', '〔 記者 蔡亞樺 ／ 台北 報導 〕 台北市 信義區 出現 天坑   台北市 消防局 下午 3 時 13 分接 獲通報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   長 15 公尺   寬 3 公尺   深度 2 至 3 公尺     附近 住家 門口 2 部機車 一部 腳踏車 瞬間 掉 進 天坑   幸無人 受傷     台北市 政府 表示   目前 已 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   信義區 長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置     台北市 建築 管理 處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   目前 了解 是 連續 壁 滲水   工地 正在 止水 當中   消防局 現場 協助 鄰 房民眾 疏散  ', '台北市 信義區 一處 新建 大樓 工地 旁 巷道   蹋陷   緊急 灌漿 回填   住戶 驚慌 撤離         消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷 ( 長 15 公尺   寬 3 公尺   深度 2   3 公尺 )   幸無人 受傷                             警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   目前 評估 約 10 餘位 住戶 需要 安置   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影警 消緊 急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   住戶 心有 餘悸 驚慌 撤離   到 一旁 安全 區域   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   警方 疏導 住戶 驚慌 撤離   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影']</t>
         </is>
       </c>
     </row>
@@ -511,21 +511,21 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1_地層下陷區_高鐵_道路_壅塞</t>
+          <t>1_地下水_地層下陷_面積_區域</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['地層下陷區', '高鐵', '道路', '壅塞', '路段', '捷運局', '交通', '沿線', '路面', '台灣']</t>
+          <t>['地下水', '地層下陷', '面積', '區域', '坑洞', '環境', '水', '當地', '地', '洞']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['去年 再增 5.4 公分   累計達 114.2 公分   防治 卻 遇 瓶頸   〔 記者 鄭旭凱 ／ 雲林 報導 〕 鐵道局 公布 台灣 高鐵 路段 下陷 監測 報告   去年 雲林 路段 不僅 持續 下陷 五 ． 四 公分   且 累積 下陷 量 已 達 一一 四 ． 二 公分   全國 最高   雲林縣 政府 水利 處處長 許 宏博 表示   針對 高鐵 沿線 地層下陷 問題   中央 成立 跨部會 平台 進行 監控   整治   但 沿途 現有 十二 萬 六千 口 灌溉 水井   政府 只能 管制 限制 其繼續 深挖   無權 禁止 使用   地下水 入不敷出   地層 自然 持續 下陷   地層下陷 遭遇 瓶頸 仍待 解決     12.6 萬口 灌溉 水井   無法 禁用   台灣 高鐵行經 彰化   雲林 嘉義 等 地層下陷區   高鐵 公司 從 二 三年 起委 託 學術 單位 監測   最新 監測 報告 指出   去年 高鐵 沿線 持續 下陷 路段 包 彰化 雲林 共八處   最 值得 關注 路段 包括 彰化 溪州 高鐵 與 中山 高 跨交段   高鐵 雲林 車站區   高鐵 跨雲一 五八 縣道 高鐵 跨台 七八 線 快速道路 等 四個 地點   下陷 量 從 二 ． 六 公分 到 五 ． 四 公分 不 等   且 比 前年 增加   但 嘉義 卻 未 再 下陷   甚至 已連續 兩年 地層還 上升     與 土庫 台 78 線 交界 處   下陷 最 多   監測 報告 指出   高鐵 沿線 最大 累積 下陷 量 已 達 一一 四 ． 二 公分   地點 雲林縣 土庫 鎮台 七八 線 與 高鐵 交界 處   進行 改善 工程 後   墩柱 差異 沉陷 量 逐年 降低   與 高鐵行車 安全 有關 橋墩 間 差異 沉陷 所累 積角 變量   目前 都 容許 範圍   高鐵 結構 安全 無虞     許 宏博 表示   地層下陷 防治 工作 遭遇 瓶頸   雲林 高鐵 沿線 既有 水井 擁有 合法 水權   數量 多 達 十二 萬 六千 口   政府 不能 禁止 農民 抽水   何況 這更關 係 到 大約 十二 萬 六千 戶農民 生計   農民持續 抽水   地層 自然 持續 下陷     輔導 水田 轉作 旱田   推動 不易   許 宏博 表示   一公頃 水田 轉作 旱田   一年 可望 省下 八千 噸 灌溉水   縣府 積極 輔導 高鐵 沿線 種植 水稻 農民 轉作 大豆 玉米 等   但 雲林 農村 人力 嚴重 老化   種植 水田 老 農無力 自行 耕種   多數委 託 代耕   但 旱田 卻 沒 代耕 業者   即使 水田 利潤 低   農民 無力 轉作   類 似的 瓶頸 仍 有待 中央 統籌 解決  ', '台灣 高鐵 公司 從民國 92 年 至今   委 託 學術 單位   持續 每年 定期 針對 高鐵 沿線 結構 墩 柱 下陷 進行 監測   並提報 交通部   鐵道局 日前 公布 2023 年 監測 報告   根據 最新 報告   高鐵 彰化   雲林 路段 下陷 持續   高鐵路線 最大 累積 下陷 量 已 達 到 114.2 公分   位 於 雲林縣 土庫 鎮台 78 線 與 高鐵 交界 處 墩 柱   但 自 103 年 進行 改善 工程 後   目標 範圍 墩 柱 差異 沉陷 量 呈 逐年 降低 趨勢     監測 報告 顯示   2023 年 高鐵 彰化   雲林 共 8 處 路段 下陷 量 從 2.6 公分   彰化 溪洲   到 5.4 公分   雲林縣 土庫鎮 與 元長 鄉 交界     都 比 2022 年 增加   嘉義 不但 未 再 下陷   還連續 2 年 回脹   但 2023 年 回脹量 比 2022 年少     鐵道局 說   較 值得 關注 高鐵 下陷 路段   包括   彰化 溪州 高鐵 與 中山 高 跨交   高鐵 雲林 車站區   高鐵 跨 雲 158 縣道   高鐵 跨台 78 號 快速道路   與 高鐵行車 安全 有關 橋墩 間 差異 沉陷 所累 積角 變量   目前 皆 容許 範圍   連續 梁為 1 1500   簡支梁 1 1000     高鐵 結構 安全 無虞     鐵道局 說   高鐵有 零星 數處 累積角 變量 逾容 許範圍 橋墩   結構 型式 皆 為 簡支梁     台灣 高鐵 已納入 定期 軌道 巡檢及 土建 設施 維護 計畫   持續 密切 關注   並依角 變量 變化 速率   按風險 等級 高低   採取 相應 加密 監測 頻率   並已備 妥 軌道 調整 預防性 結構 補強 方案   根據 監測 報告   目前 高鐵累 積角 變量 過標 準值 橋墩   反而 是 位 沉陷 改善 嘉義 路段   位 朴子溪 河 中   目前 簡支 梁累積 角 變量 達 1.96 1000   而 朴子溪 北岸 簡支 梁累 積角 變量 為 0.395 1000   雖 仍 許值 範圍   但 已 從 2020 年 起 逐年 增加  ', '  中央社 記者 汪淑芬 台北 29 日電   根據 鐵道 局新 公布 台灣 高鐵 路段 下陷 監測 報告   彰化   雲林 下陷 持續   累積 下陷 量 最大 是 雲林 114.2 公分   鐵道局 表示   高鐵墩 柱角 變量 都 容許 範圍   結構 安全 無虞     高鐵路線 通過 彰化   雲林 嘉義 主要 地層下陷區   台灣 高鐵 公司 從民國 92 年 至今   委 託 學術 單位   持續 每年 定期 針對 高鐵 沿線 結構 墩 柱 下陷 進行 監測   並提報 交通部   鐵道局 日前 公布 112 年 監測 報告     根據 最新 報告   高鐵路線 最大 累積 下陷 量 已 達 到 114.2 公分   其位 於 雲林縣 土庫 鎮台 78 線 與 高鐵 交界 處 墩 柱   但 自 103 年 進行 改善 工程 後   目標 範圍 墩 柱 差異 沉陷 量 呈 逐年 降低 趨勢     監測 報告 顯示   112 年 高鐵 彰化   雲林 共 8 處 路段 下陷 量 從 2.6 公分   彰化縣 溪州 鄉   到 5.4 公分   雲林縣 土庫鎮 與 元長 鄉 交界     都 比 111 年 增加   嘉義 不但 未 再 下陷   還連續 2 年 回脹   但 112 年 回脹量 比 111 年少     鐵道局 指出   較 值得 關注 高鐵 下陷 路段   包括 彰化 溪州 高鐵 與 中山 高 跨交段   高鐵 雲林 車站區   高鐵 跨 雲 158 縣道   高鐵 跨台 78 號 快速道路   與 高鐵行車 安全 有關 橋墩 間 差異 沉陷 所累 積角 變量   目前 都 仍 容許 範圍   連續 梁為 1 1500   簡支梁 1 1000     高鐵 結構 安全 無虞     鐵道局 指出   高鐵 零星 數處 累積角 變量 逾容 許範圍 橋墩   結構 型式 皆 為 簡支梁     台灣 高鐵 已納入 定期 軌道 巡檢及 土建 設施 維護 計畫   持續 密切 關注   並依角 變量 變化 速率   按風險 等級 高低   採取 相應 加密 監測 頻率   並已備 妥 軌道 調整 預防性 結構 補強 方案     根據 監測 報告   目前 高鐵累 積角 變量 超過 標準值 橋墩   反而 是 沉陷 改善 嘉義 路段   位 於 朴子溪 河 中   目前 簡支 梁累 積角 變量 達 1.96 1000   而 朴子溪 北岸 簡支 梁累 積角 變量 為 0.395 1000   雖 仍 許值 範圍   但 已 從 109 年 起 逐年 增加     編輯   張雅淨   1130429']</t>
+          <t>['桃園市 蘆竹 區南興 水岸 遊憩 公園 耗資 1 億元   2019 年 竣工 不到 4 年   近期 卻 被 發現 步道 草原 都 因 地層下陷   出現 大大小小 坑洞   遭議員 批評 宛如 成 了   地 雷公 園     市府 工務局 表示   地層下陷 原因 可能 是 水路 沖 刷 造成   後 續會 再 前往 會勘 確認       南興 水岸 遊憩 公園 2019 年 完工   當時 市府 進行 南 崁 溪 整治 建置 自行 車道 會勘 過程 中   發現 綠地 水 利用 地未 被 徵收   經與 地方 討論 後   市府 決定 徵收 開闢 為 水景 公園   引進 共融式 設計   設置 樹屋   人文 廣場   森林 小徑   遊戲 沙坑   自行 車道 等   成為 南 崁 住宅 密集 區   都 會 中 綠洲                               市議員 張桂綿 近期 發現   公園 中 步道 嚴重 下陷   凹 了 一塊   包括 法式 滾球區 兒童 奔跑 大 草原 出現 大小不一 坑洞   甚至 掏空 成 了 無底 洞   主因 就是 鄰近 河川 水流 滲透導致 地層下陷 嚴重   土壤 幾乎 全都 流失         這裡 宛如 地雷 區     張桂綿 直言   如果 民眾 或 兒童 沒 注意   一不小心 可能 會 踩 空 受傷   先前 已 向區 公所 反映   但 至今 仍無解方   呼籲 市府 公務 單位 多 幫忙   盡速 拆除   地雷     還給 鄉親 安全 遊憩 環境       工務局 長 汪在宙 表示   初步 判斷 可能 是 施工 時 夯土 不夠 扎實   附近 水流 滲透 加上 行人 重量 造成 壓力   才 導致 夯土 流失   地層下陷   市府 後 續會 協同 各 單位 前往 會勘   了解 發生 原因 並盡速 改善 施工 缺失   桃園 蘆竹 區南興 水岸 遊憩 公園 竣工 不到 4 年   步道 卻 嚴重 凹陷   恐影響 市民 安全   圖 ／ 張桂綿 提供 桃園 蘆竹 南興 水岸 遊憩 公園 耗資 1 億元   卻 出現   無底 洞     遭議員 批評 宛如 成 了   地 雷公 園     圖 ／ 張桂綿 提供', '〔 記者黃淑莉 ／ 雲林 報導 〕 為 防治 地層下陷   行政院 同意 明年 一期 作恢 復 高鐵 沿線 左右 1.5 公里 半範圍 農民種 植 低耗 水 作物 節水 獎勵   即種 植轉作 作物 每公頃 給予 3 萬元   種綠肥 4 萬 2000 元   種景觀 作物 5 萬 2000 元     有鑑 雲林 高鐵 沿線 地層下陷 嚴重   避免 影響 到 高鐵行車 安全   中央 相關 部會   雲林縣 府 近 幾年 積極 推動 地層下陷 防治 工作   其中 農業 方面 輔導 沿線 種植 水稻 農民 轉作 其他 節水 作物   減少 地下水 抽取 量     縣府 農業 處 指出   農委會 2013 年 至 2020 年 辦理 雲林 高鐵 沿線 3 公里 範圍 內節 水獎勵   給予 轉作 低耗 水 作物 或 運用 科技 節水 農業 生產者 獎勵   有效 減少 地下水 抽取   地層下陷 明顯 減緩     農業 處 表示   獎勵 措施 至 2020 年 截止   去年 今年 沒有 辦理   統計 發現   高鐵 沿線 第一期 作種 稻面積 又 恢 復   為 避免 地層下陷 再 惡化   縣府 向 中央 爭取 持續 辦理節 水獎勵   經 行政院 審查 核定 明年 2023 年 第一期 作恢 復 節水 獎勵     農業 處 說   這次 行政院 核定 是 針對 雲林 虎尾   土庫   元長 北港 等 四鄉 鎮高鐵 沿線 左右 1.5 公里 農地   獎勵 措施 比照   綠色 環境 給付 計畫   中水 資源 競用 區大區 輪作 節水 獎勵 額度   歡迎 符合 申辦 資格 農民 踴躍 配合   相關 資訊 可 洽詢 縣府 農業 處  ', '〔 記者 詹士弘 ／ 雲林 報導 〕 困擾 雲林 多年 地層下陷 有解 了   第四 河川 局在 濁 水溪林 內段 河槽 河床 設置 地下水 補注池   成效 卓越   今年 補注池 蓄水 面積 已 增加 至 20 公頃   等 於 添增 一座 隱形 湖山 水庫   源源 不斷 滲水來 補充 雲林 地下水 源   對 減緩 地層下陷 很大 助益     林內 鄉 公所 今天 林內 鄉 觸口 堤防   國道 3 號 高速公路 橋下   舉辦 河川 淨堤 活動   由 鄉長 張維崢 第四 河川 局長 李友平 帶領 公所 員 工及 環保志工   淵明國 中師 生及 地 居民 約 200 人   沿觸 口 堤防 道路 進行 清掃   清理 河堤 內外 垃圾   用行 動守護 環境     張維崢 表示   林內 鄉位 於 濁 水溪 沖 積扇 水源 頭之頂點   有得天 獨厚 天然 地理 環境 與 豐富 自然 生態   緊鄰 濁 水溪 河畔   水源 供 雲林縣 鄰近 縣 市民   農業 工業 用水   為 重要 水源地     李友平 表示   台灣 早年 因超 抽 地下水   導致 地層下陷   濁水溪長 186.7 公里   林內 河段 是 河 寬 最窄 處   造就 了 林內 好 水質   就 可以 從事 很多 水環境 水資源 保護 措施   經調查 林內 三號 水門 附近 河段   是 濁 水溪 唯一 能 從 事 地下水 補助 河段   經由 設置 蓄水池 留住 地面水   挖掘 入 滲補 注池   以 河水 補注 地下水   可補充 最深 達 地下 400 公尺 地下水 源   再 流往 海岸 地區   能 減輕 地下水 洩降   舒緩 地層下陷 問題     李友平 表示   第一座 地下水 補助池 於 2020 年 完成   效果 非常 好   今年 擴大 辦理   蓄水池 面積 已 達 20 公頃   源源 不絕 地面水 持續 往 地下 滲入   可 有效 減緩 地層下陷   挹注 地下水 資源     李友平 指出   去年 全國 百年 大旱   各地 都 沒 水 灌溉   別 縣市 就算 地下水 井   抽 不到 水   唯一 有水 就是 雲林   因為 地下水 補助   所以 農民 可以 抽 得到 地下水   他 強調   要 好好 保護林 水資源   因為 林內 水 如果 受到 污染   河川 局 不敢 讓 水 滲到 地下   因 為 髒 水下 滲就會 變成 地下水 深層 污染  ']</t>
         </is>
       </c>
     </row>
@@ -534,21 +534,21 @@
         <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2_中國_北京_城市_都市</t>
+          <t>2_道路_路段_地層下陷_路面</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['中國', '北京', '城市', '都市', '災害', '氣候變遷', '洪水', '風險', '地區', '人口']</t>
+          <t>['道路', '路段', '地層下陷', '路面', '交通', '混凝土', '施工', '水泥', '下陷', '凹陷']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['中國 過度 抽取 地下水   導致 近 40% 主要 城市 土地 下陷     路透     陳 麗珠 ／ 核稿 編輯   〔 財經 頻道 ／ 綜合 報導 〕 中國 近一半 主要 城市 正 遭受   中度 至 重度   不 等 程度 沉降   海平面 上升 情況 下   恐有 數百萬人將 面臨 洪水 風險     路透   指出   中國 都市人口 約 9 億人   當中 約 2.7 億人 生活 每年 下陷 逾 3 公 釐 地區   相當 於 都市人口 29%     中國 82 個 城市 中   約 45% 每年 下沉 超過 3 公 釐   16% 土地 平均 每年 下沉 更是 超過 10 公 釐   約 6700 萬 居民 生活 於 此   研究 小組 指出   由 於 中國 城市 人口 多   即使 是 一小部分 地層下陷   可能 造成 重大 威脅     據 了解   而 造成 中國 土地 逐年 下沉   最 主要 是 地下水位 下降 所致     路透 表示     土地 下陷   對 中國 每年 造成 超過 75 億元 人民 幣   約 新 台幣 337 億元   損失   研究 人員 預計   下個 世紀   中國將 約 近 四分之一 沿海 土地   恐低 於 海平面   數億人將 面臨 大 洪水 風險     最 嚴重 受災 城市 是 北方 天津   這 城市 約 1500 萬 人口   2023 年 一場   突發 地質 災害     導致 3000 名 居民 被 疏散   調查 人員將 這場 災害 歸咎 於   水資源 枯竭 地 熱井 建設       一手 掌握 經濟脈 動點 我 自由 財經 Youtube 頻道', '中國 有將 近一半 主要 城市 正 面臨   中度 至 重度   地層下陷 威脅   根據 最新 研究 顯示   中國 都市人口 約 9 億   其中 約 2.7 億人 生活 每年 下陷 逾 3 公分 地區   相當 於 都市人口 29%   加上 海平面 上升 情形 日漸 加劇   最終 中國會 約 四分之一 沿岸 地帶 低 於 海平面   上 億 居民 將 面臨 洪水 危機     綜合外 媒報導   這篇 有關 中國 土地 現況 報告 期刊   科學     Science   上 發表   研究 團隊 透過 衛星 雷達 觀測 中國 82 個 主要 城市 近幾年 地層下陷 情形   發現 約 45% 地區 每年 下沉 超過 3 公 釐   更 16% 土地 平均 每年 下沉 超過 10 公 釐   且 約 6700 萬 居民 生活 於 此   研究 小組 指出   由 於 中國 城市 人口 眾多   即使 地層下陷 只 占 一小部分   威脅 仍 不容 忽視     根據 了解   造成 中國 土地 逐年 下沉 主因 是 過度 抽用 地下水   另 一 因素 為 城市 土地 上 重量 不斷 增加   不斷 增加 沉重 建物 將 土壤 越壓 越 緊實   且 研究 人員 預計   由 於 地層下陷 海平面 上升   最終 中國會 約 四分之一 沿岸 地帶 低 於 海平面   包含 天津   上海   廣州 等 都市   數億人將 面臨 洪水 威脅     人口 超過 1   500 萬 天津市 被 認為 是   最 嚴重 受災 城市     2023 年 6 月間   一場   突發 地質 災害   讓 3 幢 大樓 出現 裂痕   地下室 滲水   3   000 名 居民 被 緊急 疏散   事發 後   調查 人員將 災害 肇因 歸咎 於 地下水 資源 枯竭   以及 地熱井 鑽井 施工 觸動 深層   地質 空腔   所致     不僅 是 中國 此 問題   世界各地 皆 面臨 地層下陷 危機   今年 2 月 發表 另項 研究 指出   全球 約 630 萬 平方公里 土地 下陷 風險   尤為 印尼 情況 最為 告急   首都 雅加 達 大部分 地區現 已 低 於 海平面   另據 新加坡 2022 年 一項 研究   提及 全世界 有著 嚴重 地層下陷 44 個 沿海 主要 城市 中   就 30 個位 於 亞洲  ', '最新 一份 根據 衛星 雷達 觀測 研究 顯示   中國近 40% 主要 城市 土地 正發生   中度 至 重度   地層下陷   上 億 居民 面臨 洪水 風險   加上 海平面 上升   上海   廣州   天津 都 面臨 災害 風險     綜合 路透社 與 美國 有線 電視 新聞網   CNN   報導   這篇 研究 今天   4 19   發表 期刊   科學     Science   上   由 中國華南師 範大學 教授 敖祖銳領 軍 研究 小組   透過 衛星 雷達 觀測 中國 82 個 主要 城市 2015 至 2022 年 地層下陷 情況   發現 40% 城市 土地 每年 平均 下沉 超過 3 公 釐     中國 都市人口 約 9 億   約 2.7 億 人口 生活 這些 每年 下陷 逾 3 公 釐 地區   相當 於 都市人口 29%     這 82 個 城市 中   更 16% 土地 平均 每年 下沉 超過 10 公 釐   6700 萬 居民 生活 於 此   研究 小組 指出   由 於 中國 城市 人口 多   即使 是 一小部分 地層下陷   可能 造成 重大 威脅     導致 中國 都市 地層下陷 主因 是 過度 抽用 地下水   另 一大 因素 是 城市 土地 上 重量 不斷 增加   時間 推移 下   沉積物 堆積   以及 不斷 增加 沉重 建物   將 土壤 越壓 越 緊實   導致 土地 下沉     研究 顯示   由 於 地層下陷 海平面 上升   最終 中國將 約 四分之一 沿岸 地帶 將低 於 海平面   天津   上海   廣州 周邊 都 面臨 這樣 風險     中國 一些 地區 已經 建立 保護 措施   這份 研究 並未 探討 這些 措施 效果   報告 合著 者   北京 大學 城市 與 環境 學院 教授 陶勝利 說   上海 就 建造 了數 公尺 高 堤防     即使 地層下陷 海平面 上升   這樣 龐大 沿海 堤防 能 很大 程度 上 降低 城市 被淹 沒 風險     就 他 所知   沒有 其他 國家 打造 過規模 這麼 大 堤防     陶勝利稱   中國 政府 實施 嚴格 地下水 管制法 規   減緩 了 上海 周邊 地層下陷 速度     全球 多個 城市 都 下陷   維吉尼亞 理工大 學 博士 後 研究 員 奧恩亨   Leonard   Ohenhen   最近 一份 針對 美國 地層下陷 狀況 報告 指出   大部分 城市 都 會 發生 土地 下沉   但 因為 沿海 地區 海平面 上升 問題   大家 比較 關心 沿海 城市     但 大多 數 城市 下沉 速度   沿海 城市 其實 都 差不多   甚至 還更快       地層下陷 不僅 是 中國 才 問題   CNN 指出   美國 紐約市 等 數十個 沿海 城市 正在 下沉   墨西哥 首都 墨西哥城   土地 每年 最 多 下沉 50 公分   可能 是 全球 沉 最快   荷蘭 已有 25% 土地 低 於 海平面     今年 2 月 另 一項 研究 指出   全球 約 630 萬 平方公里 土地 下陷 風險   印尼 是 最 嚴重 國家 之一   首都 雅加 達 大部分 地區現 都 已 低 於 海平面   新加坡 2022 年 一項 研究 提到   全球 面臨 嚴重 地層下陷 44 個 沿海 大城市 當中   30 個 亞洲  ']</t>
+          <t>['〔 記者 詹士弘 ／ 雲林 報導 〕 全國 最 嚴重 高鐵 地層下陷區 雲林 土庫 石廟 里   位 於 土庫 國中 附近 高鐵橋 下 道   路面 龜裂   坑坑洞洞   路況 極差   但 因 工程 涉及 鐵路 禁限 建範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   日前 終獲 高鐵局 同意   預計以 50 個 日 曆 天 完成 改善     土庫 鎮鎮長 陳 特凱 表示   石廟 里 高鐵橋 下 道路   經長 年 使用   平時車 流量 極大   加上 重車 違規 行駛   造成 路面 凹陷   破損 不堪   導致 居民 行車 時 容易 引發 交通事故   嚴 重影 響行車 安全   所以 向 縣府 反映   希望 能 儘 速 改善     高鐵土庫 段 是 高鐵 沿線 地層下陷 最 嚴重 地方   每年 平均 下陷 6.5 公分   工務 處長 汪令堯 表示   道 位 高鐵 正下方   涉及 鐵路 禁限建   範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   故 改為 專案 發包 方式 辦理   由 於 該 路段 交通量 極大   雖然限 10 噸 以下 車輛 行駛   但 還是 很多 重車 違規   加上 道路 路基 鬆 軟   所以 路況 極差     汪令堯 指出   由 於 道路 位 地層下陷區   加上 原先 就是 農地   土 質 鬆 軟   光重 鋪 路面   一下 大雨   重車 再 輾壓   道路 很快 就 會 再度 損壞   所以 需地質 改良   但 高鐵局 不 同意 用 給配 改善 路基   所以 工務處 改用 低 強度 水泥 替代   終獲 同意     汪令堯 表示   道路 改善 工程 總 預算 390 萬元   預期 改善 道路 長 度 兩側 約 630 公尺   寬 4.7 公尺   預計 9 月 中旬 發包   工期 為 50 日 曆 天   改善 後 可 提 昇 居民 生活 品質   維護用 路 人行 車安   另 他 會 建議 警察局   多派 員取 締重車 違規 行駛   才能 確保 道路 改善 後   以維持 好 行車 品質  ', '雲林縣 土庫 鎮高鐵 沿線 列屬 地層下陷區   軌道 下方 雲 158 甲線 通往 雲 97 線 道   雖 只 短短 約 500 公尺   但車 流大 路面 受損 累累   縣府 以 專案 向 高鐵局 申請 修繕 獲准   將以 不 影響 高鐵 地基 安全 低 強度   高流動 建材 施工   縣長 張麗善 昨天 會勘 後 表示   近期 封路 動工   10 月 完工       土庫 鎮長 陳 特凱 說   高鐵 道 開通 多年   車流 大 卻 未曾 修繕   路面 凹陷 破損 累累   影響 行車 安全   居民 陳 情 希望 改善   縣府 表示   路口 設 有限 重 10 噸 以下 車輛 通行   但 地方 反映 長 期來 仍 不少 大型 車為求 方便 直接 通行   才 使 路面 受損   將請 警方 加強 取締                             昨縣 府 會 同議員現 勘   工務 處長 汪令堯 說   高鐵軌 道 下 寬度 4.7 公尺 兩側 道   將修繕 共約 630 公尺   採低 強度   高流動 混凝土 施工 法   打造 路基 更加 穩固   預算約 390 萬元       張麗善 指出   高鐵下 道路 屬鐵路 禁限 建範圍   道 不能 任意 挖掘 施工   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   因此 工務處 以 專案 計畫 向 高鐵局 申請 修繕   預定 今年 9 月 動工   屆 時將 封路 約 50 天   請 車輛 繞 道       高鐵土庫 段過 去 以 每年 約 6.5 公分 沉陷 量 下陷   後 來 沿線禁 抽 地下水   推廣 旱作   廣闢 黃 金 廊道   才 較 為 減緩  ', '雲林縣 土庫 鎮高鐵 沿線 列屬 地層下陷 管制 區   高鐵 下方 雲 158 甲 通往 雲 97 線 道   雖 只 短短 約 500 公尺   但車 流大 路面 受損 累累   雲林縣 府 以 專案 經向 高鐵局 申請 修繕 獲准   將以 不 影響 高鐵 地基 安全 低 強度   高流動 建材 施工   預定 近期 封路 動工   10 月 完工       高鐵 雲林縣 土庫 段 受 地層下陷 影響   過去 以 每年 約 6.5 公分 沈陷 量 下陷   為維護 高鐵 安全   多年 前 曾 下陷區 動工將 橫跨 高鐵 台 78 線 快速道路   原為 土方 高架 改以 輕質 建材   重新 施工 進行   減重     此外   高鐵 沿線禁 抽 地下水   推廣 旱作 廣闢 黃 金 廊道   才 使 高鐵 雲林 段 沈陷 獲得 紓 緩                             位 於 土庫 高鐵 下方   連接 雲 158 甲及 雲 97 線 公路 高鐵 道   雖僅 短短 約 500 公尺   卻 是 管制 區內 唯一 高鐵 通道   土庫 鎮長 陳 特凱 說   高鐵 道 開通 多年   車流 大 卻 未曾 修繕   路面 凹陷 破損 累累   影響 行車 安全   居民 陳 情 希望 改善       雲林縣 長 張麗善 今天 會 同工 務處 縣 議員 王鈺齊   張維心 等 人現 勘   張麗善 說   道 位 於 高鐵 管制 區   不能 任意 挖掘 施工   因此 工務處 以 專案 計畫 向 高鐵局 申請 修繕   預定 今年 9 月 動工   10 月 完工   提供 平整 安全 道路   屆 時將 封路 約 50 天   請 車輛 繞 道       工務 處長 汪令堯 指出   高鐵下 道路 屬鐵路 禁限 建範圍   須依   鐵路 兩側 禁建限建 辦法   規定 辦理   未來 將以 390 萬元   對 高鐵下 寬 4.7 公尺 兩側 道 共 修繕 約 630 公尺   採   低 強度   高流動   混凝土 施工 法   打造 路基 更加 穩固       縣府 表示   為維護 高鐵 道 承載 安全   路口 設 有限 重 10 噸 以下 車輛 通行   但 地方 反映   長 期來 仍 不少 大型 車為求 方便 直接 通行   才 使 道路 面受損   將會 請 警方 加強 取締       隨後縣 長 張麗善 一行 人 再 轉往 土庫崙 雲 101   雲 98 道路 西螺 鎮九隆里 農路 等 會勘 改善 工程   雲林縣 長 張麗善 一行 人 再 轉往 土庫崙 等 地   會勘 多條 道路 工程   記者 蔡維斌 ／ 攝影 高鐵 雲林 土庫 段位 於 地層下陷 管制 區   高鐵下 唯一 道破 損 累累   經縣 府 向 高鐵局 專案 申請 後   近期 內將 封路 動工 修路   記者 蔡維斌 ／ 攝影']</t>
         </is>
       </c>
     </row>
@@ -557,21 +557,21 @@
         <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3_台北市_慶城街_興安街_基隆市</t>
+          <t>3_台北市_王玉芬_四川_北市</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['台北市', '慶城街', '興安街', '基隆市', '松山區', '新竹', '市府', '路旁', '台北', '交叉路口']</t>
+          <t>['台北市', '王玉芬', '四川', '北市', '建設', '施工', '住戶', '下陷', '陳', '建案']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['台北市 松山區 慶城街 一處 新建 工地 昨   23   天晚間 發生 地基 塌陷 意外   停 路旁 4 台車 受到 波及   人行道 路面 凹陷   北市 府 緊急 成立 指揮 中心 處理   台北 市長 蔣萬安今 早 二度 到 現場 視察 現況   被 問及 北市 議員 許淑華 爆出 年前 就 接獲 異常 通報   市府 無 因應   對此 他 表示 會 請 建管處 全面 清查   台北 慶城街 塌陷 案   截至 上午 11 點   已 回填 360 立方公尺   回填 高度 已近 安全 目標值 3 公尺   約 12 點 左右 就 會 完成 作業   而 比 對 相關 數據 檢測   目前 僅有 塌陷 處東側 超過 15 公分 裂痕   西 南北 側比 對 監測 數值 正常   都 沒 地面 塌陷   鄰房 傾斜 狀況   管線   路樹 等 一 併 檢查 處理   此次 台北市 政府 昨晚 慶城街 工地 塌陷 事發 後   緊急 成立 指揮 中心   開罰 18 萬並 勒令 停業   要求 工作 灌漿 回填   確保 安全   這也 是 蔣萬安任 二度 建案 塌陷 發生   此次 處理 速度 較 上次 更 快   蔣萬安強 調   每 一次 事件 發生 都 會 一次 檢視   只要 機制 完善   每個 人員落 實運作   其實 反應 就 會 快速 確實   確保 各項 安全   讓 一切 恢 復 正常   不過 外界 質疑   相比 日前 雙北惡 臭案   市府 被質 疑動作 慢半拍   蔣萬安 回應   往後相關 機制 調整 完善   確 保人 員透過 機制 系統 運作   其實 各項 反應 就 能 即刻 因應   後 續 處理 就 會 到位   至於 許淑華 透露 年前 就 接獲 異常 通報   且 未來 可以 跟 外審 單位   大地   工程   結構 技師 等 一起 監工   對此 蔣萬安 表示   異常 通報   會 請 建管處 全面 清查     另外 此次 第一 時間 邀 請 四大 工會   技師   結構   大地   建築師 工會 參 與   謝 謝里長 到 現場 協助 各項 監測   這 部份 第一 時間 都 溝通 聯 繫  ', '〔 記者 陳 奕 劭 ／ 台北 報導 〕 台北市 松山區 慶城街 興安街 交叉路口 一處 工地   昨晚   23 日   發生 地基 塌陷   工地 旁有 4 輛停 路邊 停車格 轎車   車身 隨著 地基 塌陷 呈 70 度 傾斜   幸好 無人 傷亡   對此   台北市 前 市長 柯文 哲今 早   24 日   受訪 表示   台北市 是 地層下陷 警示 區   這是 本來 就 問題     台北市 松山區 慶城街 興安街 交叉路口 一處 工地 昨晚 發生 地基 塌陷   而 柯文 哲 卸任 後 發生 好 幾起 地層下陷 事件   柯文 哲今 早 關渡 宮前 受訪 表示   台北市 本來 就是 地層下陷 警示 區   其實 去 工務局 網站 看 就 知道   地層下陷 警示 區有 好 幾個   台北 是 盆地   這是 本來 就 問題     媒體 詢問   地層下陷 是 建商 問題 或是 地質 需進 一步 檢查   柯文 哲回 應   他們 地圖 已經 相當 完整   高 危險區 要 能夠 事先 知道  ', '台北市 松山區 慶城街 一處 工地 附近   今   23   晚傳出 地層下陷 狀況   停 路邊 停車格 車輛   車身 甚至 已經 傾斜   影響 4 台車輛 傾斜   現場 為 新建 工地 地基 下陷   下陷 範圍 評估 中   無人 受傷   已劃 設 警戒 線   台北 市長 蔣萬安 副 市長 李 四川 正 趕往 現場   台北 市長 蔣萬安 發文 表示     稍早 慶城街 興安街 交叉口 發生 工地 地基 下陷   我正 趕往 現場   請 周遭 居民 經過 民眾 注意安全   最新 資訊   市府 會 即刻 通知    ']</t>
+          <t>['台北市 中山 區 大直 民宅 塌陷 案   基泰 建設 總經理 馮先勉 委屈 地稱   事發 當晚 就 現場 且 站 台北市 副 市長 李 四川 旁邊   對此   李 四川 今 受訪 還原 真相   馮當晚 確在 現場   但 當晚 後 就 沒見 到 馮到 現場 關心   還 一度 失聯 找 不到 人談 相關後續 事宜   李 四川 今   11 日   接受 媒體 人王 淺秋廣播 專訪   千秋 萬事     談及 基泰 建設 董事 長 陳 世銘 昨   10 日   快 閃離 開記者 會 一事   直言 碰到 問題 只能 面對   不能逃避   至於 基泰 總經理 馮先 勉聲 稱 一直 現場   李 四川 則還原   事發 當天   7 日 晚間 抵達 現場 後   一直 處理 救災 灌水 任務   最後因 灌水 速度 不及 搶救   他 現場 超過 約 30 分鐘 後 房子 才 全部 沉陷 下去   李 四川 當時 就 疑惑 詢問 工地 主任   這麼 大 事情   你們 負責人 沒 現場   只有 一個 主任 這     而 工地 主任 才 回應   我們 總經理 站 旁邊 那邊     李聲 稱 當下 自己 不 認識 馮   且 之 後 沒見 到 馮   直至 9 日救災 告一段落   需談 安置 時   尋找 基泰 建設 祕 書要 馮來 談 一談   結果 馮 卻 沒接 電話   連 祕 書 找 不到 馮   他 才 會 媒體 前 嚴厲 譴責 基泰   李 四川 回憶 說 道   直至 10 日 上午 才 聯 繫 到 馮 勉   雙方約 好 9 時 30 分到 台北市 政府 開會   會 同 法制局 後 達 成後續 3 點承諾   王淺秋 詢問   發生 事故 當晚   工地 主任 介紹 馮先勉 後   馮有 無過 來 稍微 討論 一下 發生 什麼 事   還是 馮 就 旁邊 像 個 路 人 一樣 圍觀   李 四川 回應   馮先 勉有 過來 打招呼 說 自己 是 總經理   但 沒談 任何 相關 事宜   李 四川 提及 當天 搶 救 緊急 過程   當時 第一 時間 緊急 疏散 住戶且 擴大 預防性 疏散   聽 到 消防局 回報 工地 一直 傳出   啪啪 啪   聲音   察覺 不妥 後 就 要求 立即 消防局 疏散 住民   同時 詢問 單號 住戶 對面 無 房子 間 隔   獲得 對面 還有 一排 雙號 住戶   因此 當下 就 下令 對面 要 依法 全部 撤離   並請區 公所 找到 實踐 大學 先行 安置   李 四川 當天 到 現場 約 22 時   當時 單號棟 已有 稍微 傾斜   但 未 沉下去   立即 要求 消防局   衛工處   水處 全部 灌水   看能 不能 讓 基地 平衡   不過 隨   啪啪 啪   間 隔 時間 越來 越短   他 就 要求 全部 站 旁邊 人 全部 快 疏散   李 表示   他 現場 約 40 分鐘 後   因 灌水 無法 讓 基地 平衡   眼睜睜 看著 房子 沉陷   垮掉 就 等同 連續 壁 全部 斷掉   緊急 改為 灌漿 處理   李 四川 提及 退休 後 又 重新 回到 北市 府 工作   很多 市政 幾乎 都 不 陌生   不過 比較 麻煩 是 極端 氣候 影響   市區 很多 側溝 設計 是 無法 承受 近來 豪 大雨   若   用 工程 技術 去 追   不斷 投入 資源 改善   怎樣 都 無法 追上 老天 給的 挑戰   舉例 豪 大雨 對 一些 老舊   低窪 社區   市府 要 想 辦法 減災   這也 是 他 回到 北市 府 任職 最大 考驗  ', '基泰 建設 新建 案   基泰 大直   因 施工 不慎 釀嚴重 公安 意外   台北市 都 發局 長 王玉芬 今日 受訪   說明 提供 3 方案 供 受損 嚴峻 25 戶長 期 安置 計畫   公開 基泰 大直 連續 壁廠 商為   齊崴 營造     至於 本刊 揭監測 報告 早就 顯示   已 超出 警戒 值     王則 稱 沒 看過 這份 監測 報告   後 續會 要求 建商 提供   本刊 今   11 日   獨家 揭露   基泰 建設委 託 儀大 工程 顧問 公司   提供 北市 都 發局 7 月 26 日 監測 報告 顯示   坍塌 前 44 天 監測 報告 結論 說 明一欄 中 已 明確 指出     部分 監測 儀器 已 超出 警戒 值     然而 基泰 建設 卻 未 積極 處理   9 月 照常 大規 模開 挖   最終 釀成 這起 嚴峻 公安 事故   對此   王玉芬 回應   昨   10 日   才 收到 建商 提供 8   9 月 監測 報告   7 月 尚未 收到   已 要求 建商 提供 完整 監測 資料   並請 專業 技師 公會 判讀   如有 發現 任何 違失   會將 技師   建築師 等 相關 人員 移送 懲戒   媒體 追問   判讀 需要 多少 時間   王玉芬 回應   由 於 資料 應該 很多   但會用 最快 時間 得出 結論   除 25 戶重 災戶 外   其他 居民 可 返家 住   但 居民 因 安全 疑慮僅 38 戶 返回   王玉芬 稱   近期 會 召開 說 明會   由技師 公會 對 所有 疑慮 住 戶 說 明檢測 結果   以 解除 住戶 疑慮   而 這次 共 撤離 236 戶民眾   除 25 戶 以外 撤離戶   每戶 家中 是否 有裂 縫 需要 補強   會 由 技師 逐步 去 勘檢   逐戶 記錄 去 修繕     我們 沒 有所 謂 強迫 住戶 入住 南港 社宅   這都 是 讓 住戶 可以 自己 選擇     王玉芬 指出   北市 府將 於 週三   13 日   召說 明會   說 明長 期 安置 3 個 方案   包含 南港 國宅備 妥 25 戶   內有 家具   冷氣   冰箱 等   若想 住 附近   會持續 提供 安置 旅館   最後民眾 可 自由 選擇 居住地   1 坪 補貼 1   600 元 租金   此外   王玉芬 指出   今日 已 啟動 4 大技師 公會 對 184 處開 挖 工地 進行 嚴格 檢查   第二 波是 針對 地下室 有開 挖導溝   連續 壁 工程 檢查   另 對 所有 工地 加強 加強 頻率 檢查   預計 每月 1 次   地下室 開挖 會 增加 檢查 頻率   而 鄰損 規則   SOP 結構 外審 規定 會 一個 整體 檢視   即刻 啟動 修法   王玉芬 強調   未來 只要 建設 公司   營造 廠 或 分包 廠商   相關 技師   工地 涉及 公安 跟 鄰損   嚴重 時 就 會 全部 公開 資訊   包括 下 包廠 商   而 今日 公布   基泰 大直   下 包連續 壁廠 商為   齊崴 營造       一個 都 不要 跑掉   讓 大家 可以 避開 雷區    ', '台北市 中山 大直 街 94 巷 周邊 民宅 嚴重 塌陷   市長 蔣萬安強 調   會 徹底 調查 建管處 處理 過程 是否 違失     絕不寬貸   護短     同時 會 檢視 基泰 建設 台北市 建案   不合 規定 就 會 勒令停工   北市 府 成立 律師團 協助 住 戶後續 追償   蔣萬安今   8 日   接受 資深 媒體 人 黃 光芹 主持 節目 專訪   坦言 建管處 4   5 月 收到 住戶 書面 申訴 牆壁 龜裂   獲報 後 派員 了解   當時 認為 與 基泰 建設 開 挖 無 直接 相關   而 當時 仍施 作連續 壁   直至 7 月 24 日才 開 挖   至於 大直 災民 安置 問題   蔣萬安 表示   會 找 時間 了解 住戶 需求   昨   7 日   就 成立 群組   包含 民政局   社會局   衛生局 等 局處   需要 領藥 開綠色 通道 至 台北市 聯合 醫院   後 續 會 協助 住戶 追究 責任   求償   至於 市議員陳怡 君質疑   住戶僅 被 安置 1 天   蔣萬安否 認   目前 安置 到 11 日   即刻 請觀 傳局 了解   協調 旅宿業者   以 降低 大家 搬動   當然 住戶 不想 住 那麼 長   只要 確認 安全 無虞   就 會 讓 住戶 回去   蔣萬安強 調   將 重新 檢視   調查 事情 原委   包含 住戶 起初 提出 申訴   建管處 判斷 過程 是否 違失 或 違法   才 導致 今天 狀況     絕不寬貸   絕不護 短     若 發現 是 機制   SOP 出 了 問題 就 會 修正   蔣萬安 提及   台北 30 年 以上 老舊 建物 超過 7 成   危老 都 更案 經常 緊臨 老房子   現在 危老 都 更 都 會 較 過往 開 挖 來 深   基泰 大直 就 開 挖 到 地下 3 層   故會 要求 建管處 增加 查核 頻率   尤其 地下 深開 挖 部分 要 確保 施工 安全   黃 光芹 詢問   是否 可能 要求 任何 局處 首長 下台 或 撤 職來 負責   蔣萬安 回應   只要 徹底 調查 發現 任何 違法 情事   或 發現 當時 處理 不當   表態   該換 就換   這沒有 疑問     強調 重新 檢視 後   需要 撤換 就 撤換     至於 基泰 建設 台北 尚有 4 個 建案 是否 會 要求 全面 停工   蔣萬安 回應   會 全面 檢視 基泰 建設 台北市 所有 建案   包含 今日 已 派員去 基泰 建設 勞檢   會 檢視 相關 施工 是否 合乎 規定   若未 依規 就 會 依法 勒令停工   蔣萬安稱   北市 府 已 成立 跨局 處 一站式 聯合 服務 中心   成立 律師團 協助 住 戶後續 求償   他 下午 再度 前往 視察時   重申 要 重檢視 北市 建物   而 北市 府 會 向 建商 與 施工 廠商 追究 到底   蔣萬安 撂 狠話     建商 要負 全面 責任   否則 未來 台北市   很 抱歉   不 符合 相關 規定 或 標準 就 別 想 台北市 取得 任何 案子     而 下午 建管處 已經 發文稱 基泰 北市 7 個 工地 全面 停工  ']</t>
         </is>
       </c>
     </row>
@@ -580,21 +580,21 @@
         <v>4</v>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4_道路_萬華區_路面_坑洞</t>
+          <t>4_地層下陷_大樓_地下水_地層</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['道路', '萬華區', '路面', '坑洞', '塌陷', '南京', '水溝', '北市', '巷', '南港路']</t>
+          <t>['地層下陷', '大樓', '地下水', '地層', '建築', '地區', '下陷', '未來', '多', '地面']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['北市   天坑   事件 接連 3 天發生   今 傍晚 萬華區 昆明街 320 巷 出現 路面 坑洞   民進 黨 北市 議員 洪婉臻 晚間 表示   短短 時間 發生 多起 塌陷 意外   道路 品質 堪憂   根本 不堪 大雨 考驗   每下 一次 大雨 前進 指揮 所 就 出動   然 後 各局 處分別 擔責任   批 市府 便宜行事   罔顧 公共安全       洪婉臻 說   昆明街 320 巷 9   2 號 今天下午 4 點 42 分出 現 天坑 事件   該 事件 是 因建案 開 挖   造成 長 3 公尺   寬 2 公尺   深度 1.5 公尺 地層下陷   約 一輛 汽車 車身   所幸 塌陷 部分 位 工地 範圍   未影響 到民眾 安全 與 通車                             表示   據 建管處 施工 科回報   查明 連續 壁 並無滲 水破損 情形   與 之前 南京 西路 發生 塌陷 原因 不同   比較 可能 是 因為 連日豪 大雨 造成 土 質 鬆 動   才 發生 整體 事件   因 基地 退縮 建築線 3.64 米開 挖   故 坍陷 處裡開 挖面 仍 2 至 3 米 距離   坍陷 原因 還在 查明       洪婉臻 指出   繼 之前 大同 區 南京 西路 後   今天 已 是 北市 第 3 次 發生 路面 塌陷 事件   短短 時間 發生 多起 塌陷 意外   北市 道路 品質 堪憂   根本 不堪 大雨 考驗   直言 北市 府 真應 該 好好 檢討 路面 品質       呼籲 市府   對 於 道路 品質 不要 便宜行事   屢次 臨時 抱 佛腳   每下 一次 大雨 前進 指揮 所 就 出動   然 後 各局 處分別 擔責任   上次 是 衛工處   這次 是 建管處   簡直罔顧 公共安全     一次 又 一次   只會 讓 人民 對 政府 失去 信心           北市   天坑   事件 接連 3 天發生   今 傍晚 萬華區 昆明街 320 巷 出現 路面 坑洞   圖 ／ 洪婉臻 辦 公室 提供   北市 短短 3 個 月 出現 第 5 個   天坑     此為 今日 萬華區 某處 工地   圖 ／ 居民 提供', '繼 前天 南港區   昨日 中山 區   北市 今 傍晚 萬華區 某處 工地 再現 路面 坑洞   這也 是 北市 短短 3 個 月 出現 第 5 個   天坑     台北市 工務局 表示   該處 為 新建 工地   疑 基地 外舊 水溝 加上 地基 較 鬆 軟   遇上 大雨 沖 刷   導致 土石 流失 下陷   這處 天坑 約長 3 公尺   寬 2 公尺   深度 1.5 公尺   無人 受傷   已畫 設 警戒 線   淘空 點位 在建 築 基地   建商 已 接手 灌漿 處 理完 畢       萬華區 天坑 位 於 昆明街 320 巷 9   2 號 新建 工地 旁   今天下午 16 時 42 分 左右   疑似 因 基地 外舊 水溝 加上 地基 鬆 軟   遇 大雨 沖 刷   導致 土石 流失 下陷                             北市 府 表示   這起 萬華 地層下陷   長 寬 約 一輛 汽車 車身   還好 塌陷 時   無 造成 人員 受傷   目前 北市 府 已 畫設 警戒 線   消防局 已 現場 成立 前進 指揮 所 警戒 守視       新工處 表示   本案 經 工地 主任 說明   是 因 基地 外舊 水溝 加上 地基 較 鬆 軟   遇上 大雨 沖 刷   疑似 導致 土石 流失 下陷   建商 已 緊急 調用 水泥 車搶修   晚間 19 時 完成 灌漿 回填 作業   目前 初步 評估 並無 擴大 危害 之虞       北市 近期 五度 出現 路面 坑道   分別 為 5 月 13 日 信義區 崇德 街   7 月 10 日 大同 區 南京 西路   8 月 18 日 南港區 南港路   8 月 19 日 中山 區 民生 東路   以及 今天 萬華區 昆明街   北市 萬華 某處 工地 今天 出現 路面 坑洞   圖 ／ 居民 提供 工務局 表示   掏空 點位 在建 築 基地   建商 已 接手 灌漿 處 理完 畢   圖 ／ 居民 提供 北市 短短 3 個 月 出現 第 5 個   天坑     此為 今日 萬華區 某處 工地   圖 ／ 居民 提供 北市 萬華 某處 工地 今天 出現 路面 坑洞   圖 ／ 居民 提供', '台北市 短短 3 個 月 出現 4 個 天坑   遭批 天龍國 變成 了   天坑 國     對此   工務局 今   20   日強 調   今年 發生 四案 道路 坑洞 情形   均 非 道路 受 輾壓 破 損導致   工務局 已針 對 四案 成因 擬定 預防 道路 塌陷 方案   以 避免 類似 情形 發生   北市 民生 東路 二段 159 巷口 19 日 晚間 出現 道路 坑洞   新工處 接獲 通報 立即 調派 開 挖機 進場   確認 為 路旁 側溝 破損 造成 道路 掏空   新工處 進行 路面 回填   後 續 由 水利 處修 復 溝體   水利 處下 工科 科長 邱佑銘 表示   經現場 勘查 破損 側溝位 排水 下游 處   可能 因 水流 長 期 沖 刷 或 施作 年代 久遠   溝底 出現 局部 破損 情形   水利 處並 已督商 今日 進場 辦理 搶 修作業   因案址 位處 8 公尺 以下 單行 道   因此 施工期 間會 派義交 於 路口 指揮 暫時 禁止通行   當日 傍晚 收工 後則 於 側溝 開 挖邊 以槽 鋼護欄 圍設   並可回 復 道路 通行   為確 保側 溝結構 強度 混凝土 澆置 後 需養護 時間   溝底 牆 身及 頂版會 分次 施工   預計 2 天可將 側溝 搶修 完成   工務局 說明   北市 近期 出現 4 個 道路 坑洞 事件   歸納為 3 種 原因 造成   5 月 19 日 信義區 崇德 街因 建案 工地 開挖 地下 基礎   連續 壁 滲水 造成 地下水 湧入 基地   周邊 道路 沙土 被 帶 走 而 出現 坑洞   7 月 10 日 大同 區 南京 西路 坑洞 是 因該 處 地層 軟弱   長 期受 潮汐 影響 地下水位 升降   使 污水 管線 下方 土壤 承載力 不佳   導致 污水 管接 頭 鬆 脫 錯 位   土砂 沿管線 破 損處 流失 所致   後 衛工處 以 內視鏡 巡檢車 檢視 淡水河 沿岸 11 條 汙水 管均 正常   近 兩日 發生 兩 案件 均 與 水利 管渠 破損 有關   南港區 南港路 出現 坑洞   市府 初判 因事 發地 點位 於 南港 東區 門戶 計畫 範圍   許多 建案 均 施工 中   南港路 47 巷 道路 狹小   因此 水利 處無法 深埋 排水 箱涵 接側 溝的連 接管   研判 與 重車 來 往頻 繁有間 接關 係   使得 連 接管 間 出現 縫隙   地下水 帶 走 土沙 而 發生 地層下陷   至於 昨夜 民生 東路 二段 159 巷口 坑洞   則因 道路 側溝 溝體 老舊 破損   而 造成 近期 下雨 排水 淘涮   因應 幾次 道路 塌陷 坑洞 問題 事件   北市 府 已 擬定 防範 措施   新工處 將加強 定期 道路 巡查   如發現 路面 曾 出現 塌陷 修補 狀況   會 再 使用 透地雷達 確認 道路 無 孔洞   若有 土壤 流失   透過 預判 可 先行 強化 道路   衛工 處則 啟動 攝影機 巡視 各個 大型 管道   水利 處 將針 對 管路   箱涵 等 進行 巡視 機制   多管 齊下 避免 類似 坑洞 情形 再 發生  ']</t>
+          <t>['一項 最新 研究 發現   美國 紐約市 長 期 承受 大量 建築物 重量 之下   地層 正在 下陷   加上 紐約市 海平面 上升 速度 高居 全球 2 倍 以上   恐為 紐約市 招致 洪災 等 危機     美國 有線 電視 新聞網   CNN   報導   據 推估   紐約市 2050 年 海平面 將 上升 8 至 30 英寸   20.32 至 76.2 公分     更 重要 是   科學家 預期 由 於 人 為 引發 氣候 危機   類似 東北 風暴   nor   easter     颶風 這類 極端 降雨 事件 將更頻 繁地 出現                           美國 地質 調查 所   US   Geological   Survey   專家 帕森斯   Tom   Parsons   說     我們 離 海水倒灌 還有 一段 很長 路 … 但 我們 紐約 市經 歷過 數次 嚴重 颶風 事件   像 颶風珊迪   Sandy   艾達   Ida   帶來 暴雨 使得 城市 淹水 成災   都市化 帶來 部分 影響 使得 水災 發生       這篇論 文發表 期刊   地球 未來     Earth   sFuture   上   旨在 展示 沿海   河濱 或 湖濱 地區 高樓 大廈 何以 增加 未來 洪災 風險   以及 應 採取 相關 措施 來 降低 潛在 危險 衝擊     研究 人員藉 當時 紐約市 5 個 行政 區約 108 萬座 建築物 質量   計算出 這些 建築物 重量 約 為 7620 億 公斤   相當 於 約 190 萬架 滿載 波音 747   400 客機     研究 團隊 接著 利用 模擬 方式   計算出 這些 重量 對 地面 影響   並和 顯示 實際 地表 地質 情況 衛星 數據 進行 比 較   帕森斯 說   這項 分析 揭露 紐約市   平均 每年 下陷 約 1 至 2 毫米   部分 下陷 較 嚴重 地區 每年 下陷 約 4.5 毫米       然而   並非 所有 地層下陷 都 是 建築物 造成   帕森斯 說     我們 可想 見 非常 鬆 軟 土壤 人工 填土 地面 上 建造 建築 地層下陷 關聯 … 其他 地方   我們則 看到 難以 解釋 地層下陷   它 很多 不同 成因   例如 上個 冰河 時期 後 發生 後 冰期 回落   或是 抽取 地下水       研究 表明   地層下陷 可能 比 海平面 上升 更 早構 成洪災 威脅   而且 這種 情況 不 只 發生 紐約市     帕森斯 說     這是 一個 全球性 問題   我來 自羅德島 大學   University   of   Rhode   Island   合著 者 研究 了 世界各地 共 99 座 城市   不 只有 沿海 城市 內陸 城市   其中 絕 大多 數都 存在 地層下陷 問題    ', '美國 紐約 是 東部 最熱鬧 城市 之一   是 美國 人口 最多 城市   但 研究 顯示   這座 重要 城市 卻 每年 都 下沉 中   部分 地區 最 後 可能 還會 被淹 沒   電影   明天 過後   海水倒灌 場景   未來 恐怕 真的 會 發生   美國 紐約 摩天 大樓 林立   但 多 達 百萬棟 建築物實 太重 了   讓 整座 城市 地層 正在 下陷   再 加上 紐約市 海平面 上升 速度 高居 全球 2 倍 以上   長 久 下來 恐發生 海水倒灌 等 洪水 災害   美國 地質 調查 所 專家 帕森斯 表示     無可 避免   地面 下降   水面 上升   某些 時候   這兩層 面會 同時 發生   但 我 沒辦 法給 確切 時間點     帕森斯 說   超過 百萬座 建築物 分布 五個 行政 區上   加起 來 約 1.7 兆 磅 混凝土   金屬 玻璃 等 建材   相當 於 4700 座帝 國大廈 重量 壓在 地球 上   其中   部分 大樓 建築 布魯克林   皇后 區和曼 哈頓 市中心 土 質 鬆 散 地 區 上   下沉 速度 更 快   美國 地質 調查 所 專家 帕森斯 表示     中部 大陸 上升   東 海岸 每年 下沉 約 1 至 2 公 釐   這是 我們 看到 主要 警訊   再 加上 紐約市 不同 土壤 質地   還有 人工 填土 來 增加 土地 面積   但 它們 土壤 固結度 很 差   還是 可以 讓 地層下陷     帕森斯 還說   雖然 下沉 速度 很 緩慢   但 紐約 部分 地區 最 終將 被淹 沒   猶如 電影   明天 過後   海水倒灌 場景   未來 恐怕 真的 會 發生   至於 紐約 是否 會 變成 美國版 威尼斯   帕森斯 表示   確切 時間點 目前 尚 不 清楚   可能 還 需要 數 百年 時間   但 他 研究 不是 危言 聳 聽   只是 希望 透過 科學 數據   問題 擴大前   採取 行動  ', '紐約市 正在 下陷   美國 地質 專家 研究 發現   由 於 紐約市 摩天 大樓 眾多 加上 地質 變動   部分 紐約市 地層 已 下陷 至少 2 公分   未來 若 再 加上 海平面 上升   恐讓 沿海 地區 居民 生存 備受 威脅     紐約 每年 均 下沉   據   獨立報   報導   紐約市 人口 約 800 萬   美國 地質 調查局 研究 人員 指出   包括 布魯克林   皇后 區與 下曼哈頓 部分 紐約市 因為 地層下陷   每年 下沉 1 到 2 公分                           該 研究 更納入 土壤 條件 與 100 萬棟 大樓 7620 億 公斤 重量 等 因素   除此之外   研究 更 指出   紐約 市還 面臨 洪水 危害 風險     海平面 上升 亦 是 威脅   稍早 研究 曾 指出   全球 暖化 帶來 海平面 快速 上升   2050 年前 全球 海平面 將 上升 200 到 600 公分     研究 人員還 指出   紐約市 每年 下陷 約 1 到 2 公分   部分 地區 下沉 速度 更 快   原因 除了 近期 不斷 興建 摩天 大樓 外   還 包括 抽取 地下水   土壤 壓實 與 地震 等 因素   都市 建築物 面臨 其他 風險   例如 地層 暴露 鹽水 後   可能 導致 鋼筋 混凝土 受到 侵蝕   因此 減少壽命     下 沈是 自然 造成   據   Live   Science   報導   研究 指出   紐約市 下 沈 部分 原因 可能 是 自然 形成   因為 上 一次 冰河 時期 最 寒冷 時候   巨大 冰層 曾 覆蓋 大部分 地球   造成 冰層 下方 地面 下陷   進而 讓 陸地 邊緣 升起   等到 冰層 融化 後   被 抬升 地區則 開始 下陷     之前 研究 就 指出   到 2100 年   美國 東岸 可能 會 下陷 48 至 150 公分   除了 大自然 力量 之外   研究 人員 認為還 可能 包括 其他人 為 因素   且 科學家 發現 當地 某些 地區 下沉 速度 更 快   原因 可能 是 建築物 重量 造成     本次 研究 結果 刊登 Earth   s   Future 期刊   【 更 多 精采   詳見 】']</t>
         </is>
       </c>
     </row>
@@ -603,21 +603,21 @@
         <v>5</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5_碼頭_漁港_沿海_嘉義</t>
+          <t>5_巷道_地層下陷_市府_道路</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['碼頭', '漁港', '沿海', '嘉義', '漁業', '屏東縣', '海水', '海', '海水倒灌', '縣府']</t>
+          <t>['巷道', '地層下陷', '市府', '道路', '塌陷', '巷', '路', '下陷', '地下', '下']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['屏東縣 沿海 佳冬 鄉 塭 豐養殖 漁業 生產區   養殖 面積 漁產量 居 全縣 之冠   當地 漁民 卻 一直 飽受 地層下陷 帶來 溢 淹 問題 道路 顛簸 路況 所苦   縣府 向 中央 爭取 8861 萬元 經費 投入 治水 道路 改善 工程   縣長 周春米 今天 主持 動工 儀式   將 改善 排水 護岸 總長 854.8 公尺   道路 面 平均 抬升 1.3 公尺   定 明年 10 月 完工       周春米 說   佳冬 鄉 塭 豐養殖 漁業 生產區 擁有 全台 首座 大型 海水 供水 設施   供 地養 殖區 穩定 水質 足夠 水量   以達 養殖 環境 永續 經營 目的   成為 全台 指標性 建設   吸引 各地 機構 團體 來   取經     居民 卻長 期苦 於 地層下陷 帶來 排水 問題 既有 路況 顛簸 起伏   縣府 向 中央 爭取 經費 改善   可 降低 區域 淹水 風險   提升 當地 生產 生活 環境 品質                             說   佳冬 鄉 塭 豐養殖 漁業 生產區 面積 470 公頃   是 屏東縣 最大 養殖 漁業 生產區   塭 豐 二中 排旁 豐 海路 是 塭 豐生 產區 東西 向 重要 主要 聯絡 道路   改善 工程 不僅針 對 塭 豐 二中 排進行 改善   對豐 海路 路面 裂化   高程 不足 等 問題 一 併 改善   完工 後 可 改善 路面 破損   道路 淹水 等 問題   讓 風災來 臨時 漁民有 安全 通行 道路 進出 養殖區   強化 養殖 漁業 生產 環境 安全       縣府 海洋 漁業 事務 管理所 表示   工程 護岸 採用 預力 混凝土 板樁   具有 施工 快速   振動 噪音 低及 材料 品質 穩定 等 優點   減少 施工 時 對 養殖 魚塭 影響   防汛 道路 高度 平均 抬升 1.3 公尺   路面 鋪設 厚度 為 10 公分   讓 道路 平順銜 接   防止 溢淹 情形   營造 優質 自然 安全 水環境       屏東縣 沿海 佳冬 鄉 塭 豐養殖 漁業 生產區   養殖 面積 漁產量 居 全縣 之冠   居民 卻 一直 為 地層下陷 帶來 溢 淹 問題 顛簸 起伏 路況 所苦   圖 ／ 屏東縣 政府 提供 屏東縣 沿海 佳冬 鄉 塭 豐養殖 漁業 生產區   縣府 爭取 8861 萬元 經費 治水   縣長 周春米 今天 主持 動工 儀式   定 明年 10 月 完工   圖 ／ 屏東縣 政府 提供 屏東縣 沿海 佳冬 鄉 塭 豐養殖 漁業 生產區   縣府 爭取 8861 萬元 經費 治水   縣長 周春米 今天 主持 動工 儀式   定 明年 10 月 完工   圖 ／ 屏東縣 政府 提供', '嘉義 縣東 石鄉 鰲 鼓   副瀨及網 寮 等 3 漁港 碼頭 作業 平台   因 地層下陷 問題   逢農 曆 大潮 時   就會 發生 海水 溢漫 淹過 碼頭 平台   長 期 危及 漁民作業 安全   為解 決此 問題   今天 縣長 翁章 梁 抵副瀨漁港 現勘 聽 簡報   將採取 由 縣府 自掏腰包 以稅 收超 徵數 支應 1510 萬元   來 改善 漁港 環境   預計 今年 6 月 動工 10 月 完工       縣長 翁章 梁 表示   鰲 鼓及 副瀨等 二個 漁港   是 中央 列冊 低 利用 度漁港   另網 寮 漁港 南側 作業 平台 則是 位 漁港 範圍 外   因此 無法 爭取 中央 經費 挹注 改善   他 深知 這 3 個 漁港 碼頭 作業 平台 高度 不足   危及 漁民作業 安全   即 指示 農業 處 規畫 改善                               大潮 來   沒 看到 路 怎麼 走     鰲 鼓 蚵 農何 金聰 說   大潮 時   整個 平台 都 淹滿水   碼頭 完全 消失   漁民 不得已 都 要 冒險 拿 著長 竹竿   撐 著 地面 去 探路   走下 碼頭 上船 隻   長 期 都 很 危險       漁業 科長 張 建成 表示   3 處 增高 碼頭 平台 改善 工程   目前 已 辦理 設計 工作   預計 今年 6 月 完成 發包動工   10 月底 前 完工   讓 各 碼頭 高度 可 提升 到暴 潮位 以上   讓 漁民有 安全 作業 環境       縣議員 黃 嫈 珺 在場 指出   漁民向 反應 鰲 鼓   副 瀨   網寮 白水 湖導 航燈 壞 掉   導致 漁民 都 是 摸黑 出海   靠 得 全是 經驗值   相當 危險   盼 增經費 盡快 設置 完成       對此 科長 張 建成 回應   前年 導航燈 已 爭取 到 中央 經費 完成 第一期 改善   議員 反應 4 處漁港   他 已 跟 東石 漁會 總幹事 討論   並進行 其他 漁港 是否 需求 盤點   將一 併 向 中央 爭取 第二期 改善 經費   嘉縣 議員 黃 嫈 珺 今天 現勘 反應 鰲 鼓   副 瀨   網寮 白水 湖導 航燈 壞 掉   導致 漁民 摸黑 出海   靠 得 全是 經驗值   相當 危險   盼 增經費 盡快 改善   記者 呂慧瑜 ／ 攝影嘉縣 長 翁 章梁 今現 勘東 石鄉 副 瀨漁港   包括 鰲 鼓 及網 寮 等 3 漁港 碼頭 作業 平台   縣府 自掏腰包 1510 萬元   增高 改善 漁港 環境   預計 今年 6 月 動工 10 月 完工   記者 呂慧瑜 ／ 攝影嘉縣 東石鄉 鰲 鼓   副瀨及網 寮 等 3 漁港 碼頭 作業 平台   逢農 曆 大潮 時   就會 發生 海水 溢漫 淹過 碼頭 平台   長 期 危及 漁民作業 安全 問題   記者 呂慧瑜 ／ 攝影嘉縣 東石鄉 鰲 鼓   副瀨及網 寮 等 3 漁港 碼頭 作業 平台   縣府 自掏腰包 1510 萬元   增高 改善 漁港 環境   預計 今年 6 月 動工 10 月 完工   記者 呂慧瑜 ／ 攝影', '〔 記者 林宜 樟 ／ 嘉義 報導 〕 嘉義 縣東 石鄉 鰲 鼓   副瀨和網 寮 等 3 座 漁港 碼頭 作業 平台 因 高度 不足   每逢 大潮 海水 經常 漫溢 危及 船 隻 漁民作業 安全   嘉義 縣 政府 斥資 1510 萬元 規劃 改善   今天 縣長 翁章 梁 前往 副瀨漁港現 勘時 表示   3 座 漁港 加高 工程 預計 今年 6 月 發包動工   10 月底 完工   讓 碼頭 高度 可 提升 至暴 潮位 以上   解決 漁民 多年 來 面臨 作業 困難 困境     翁章 梁   立委 蔡易餘   東石 鄉長 林俊雄   嘉義 區漁會 總幹事 林佳瑩   縣議員 姜梅紅   李國勝   黃 嫈 珺 等 今天 到 副 瀨漁港 現勘   翁章 梁說   為 保障 漁民 需求   因此 以 縣府 經費 1510 萬元 進行 加高 工程   規劃 完善 基礎 建設     農業 處漁業 科長 張 建成 說   鰲 鼓   副瀨漁港 碼頭 及網 寮 漁港 南側 作業 平台 因 地層下陷   高度 明顯 不足   每逢 大潮   海水 漫溢 到 碼頭 影響 安危   由 於 鰲 鼓及 副 瀨漁港 為 中央 列冊 低 利用 度漁港   網寮 漁港 南側 作業 平台 則是 位 漁港 範圍 外   無法 爭取 中央 經費     翁章 梁說   漁港 是 出海 養殖 牡蠣 捕魚 重要 基地   更是 漁民 生命 財產 保障   是 海洋 漁業 發展 最 基本 建設   但 小漁港 年久失修   加上 地層下陷   漁民作業 困難   漲潮 時海 水淹 沒 港口   中央 無法 補助   縣府 就 必須 出手   架 高作業 平台   解決 高漲 潮水   既 保障 漁民 日常 工作 需求   能 化解 安全 問題     副瀨村長 林泰平 說   因副瀨漁港 很 淺   數 十年 來 出入 困難   感謝 翁 縣長 關心 漁港 基礎 建設   除 加高 平台 協助 清淤   讓 漁民有 更好 作業 環境   黃 嫈 珺 說   東石 沿海 導航燈 多處 損壞   漁民 只能 摸黑 出海   靠 經驗 航行   建議 縣府 要 修繕 導航燈   張 建成 回應   將再 請 嘉義 區漁會 盤點 損壞 導航燈   再 向 中央 爭取 經費 改善     農業 處 表示   鰲 鼓   副瀨及網 寮 漁港 加高 工程 改善 包括 碼頭面   作業區 加高   以及 其他 附屬 設施 銜接   鰲 鼓 工程 預算 經費 288 萬元   副 瀨 工程 經費 912 萬元   網寮 工程 預算 經費 310 萬元  ']</t>
+          <t>['新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     凹陷 面積 約 1 公尺 見方   雖然 緊急 灌漿 回填   但 今天 又 發現 巷 另 處 凹陷 下沉   由 於 一旁 不到 3 公尺 緊鄰 20 多戶 住戶   引發 住戶 擔憂   整夜 睡不著     民代質疑 工法 問題   未來 恐繼續 塌陷       市府 都 發處 指出   昨天 已 勒令 建案 停工   裁罰   並 要求 廠商 進行 加固 支撐 灌漿 作業   自來 水 公司 今天 派員現 勘 要汰換 道路 下方 自來 水管 線   之後將 觀察 管線 狀況 再 重鋪 路面   現場 將加裝 傾斜儀 24 小時 檢測   預警   以確 保住 戶 安全 為 最大 前提                             據 了解   該 建案 基地 正下 挖 到 地下 3 層   頻繁 重車 進出   先前 就 有人 發現 建案 基地 旁 道路 與 民宅 出現 裂縫   昨天 則開始 出現 道路 地層下陷   還伴 隨 瓦斯 異味   讓 周邊 住戶 相當 害怕   就 怕 上演 基泰 大直 工地 事件       竹 市府 指出   地層下陷 疑似 為 建案 基地 內側 開 挖 後   造成 基地 外側 道路 內部 土壤 位移   連帶 造成 自來 水管 線 破裂   沖 刷 土壤 泥沙 後 再 造成 地層下陷   瓦斯 管線 破裂       市議員陳慶齡 熟悉 建築 營造 工程   他 說 該 建案工 地位 於 沙地   正在 下 挖 地下室   懷疑 打 基樁 過程 不夠 密實   導致 基地 旁 道路 沙土 不斷 流失 流進 地下室   才 會 造成 道路 沈陷   如果 沒有 妥善 處理   未來 還是 會 發生 道路 沈陷 可能       和平路 20 巷 住 戶 約 20 多戶   居民 無奈   不敢 休息     擔心 瓦斯 味 很重   萬一 爆炸 怎麼 辦   平常 只有 兩老住 這 而已   半夜 已經 沒法 入睡   眼看 住家 旁建案 工地 才 剛蓋   未來 至少 還要 辛苦 兩   三年   希望 做好 偵測   事先 預防   否則 出事 就 麻煩 了   新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     今天 還有 另處 塌陷   記者 張裕珍 ／ 攝影 新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     雖然 已經 回填   但 仍 可見 到 住家 前方 有裂 縫   記者 張裕珍 ／ 攝影 新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     雖然 已經 回填   但 仍 可見 到 住家 前方 有裂 縫   記者 張裕珍 ／ 攝影 新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     今天 還有 另處 塌陷   記者 張裕珍 ／ 攝影', '新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   還有 自來 水洩漏   瓦斯 異味 飄散 情形   引起 住戶 疑慮   雖然 天坑 處緊 急 回填   但 仍 持續 他 處 下陷   建物 傾斜計 監測 數值 逼近 警戒 值   自來 水 公司 將於 明天 起汰換 上百 公尺 老舊 自來 水塑膠 管線   市長 高虹安 下午 赴 前進 指揮 所 了解 應變 情形       新竹市 和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   未料 前天 竟釀 緊鄰 巷弄 道路 下陷   由 於 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 相當 擔憂   市府 今天下午 請 來 4 大技師 公會 到場 了解   確認 工地 與 道路 下陷 情形                             據 了解   前天 發生 和平路 20 巷   天坑   事件 後   建商 取得 住戶 同意 20 巷前   中   後 段 設置 建物 傾斜計 監測 傾斜 情形   今天 最新 測得 最大值 每秒 387   已經 接近 每秒 413 警戒 值   由 於 和平路 20 巷 仍 道路 下陷   漏水 情形   今天 緊急 加裝 關水閥 處理       建案 營造 商工 務經理 黃 姓 經理 說   建案 地質 為 砂質 帶土   下 挖 施工 採鑽掘 方式 進行   強度 類似 連續 壁 工法   但蔽 體開 挖 壓力 造成 基地 外側 道路 內部 土壤 位移   加上 巷內 老舊 自來 水管 線 破裂   漏水 導致 土壤 泥沙 流失   進而 造成 地層下陷   水 流入 基地       由 於 和平路 20 巷內 約 3   40 戶 民宅   民富 里里長 沈朝旺 說   住戶 都 擔心 房子 會 塌陷   不要 等到 真正 傾斜 就 來 不及 了   希望 相關 單位 公告 監測 數據   並 加快 自來 水 與 瓦斯 管線汰換   自來 水 公司 明天 將進場 開 挖   汰換 鑄鐵管   盼 建商 同步 處理 好 地基         各項 資訊要 更 透明   讓 住 戶們 安心     楊姓 住戶 說   他 巷 住 了 20 年   其他 老住 戶 更 住 了 40 多年   大家 都 擔心 道路 下陷 擴大   希望 檢測 資訊 更加 透明   因為 他們 肉眼 看不到 傾斜 程度   很 需要 科技 儀器 來 幫忙 監測   數據 要 公開 讓 住 戶 都 了解       由 於 建案 工地 旁不斷 道路 下陷   建案 自行 組成 應變 中心   應變 中心 代表 允諾   已經 協調 明天 自來 水 公司 進場 換管   加派 人力 前   後 分頭 施工 情形 下   能 7 天汰管 完成   預計 10 月初 再換 瓦斯 管線   若 傾斜計 監測 到 了 警戒 值   將 安置 住戶 入住 旅館       新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   造成 緊鄰 和平路 20 巷道 路 下陷   明天 將進 場汰換 老舊 自來 水管 線   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影', '新竹市 和平 路竹 慶建設   筑光   建案 工地 下 挖 地下室   未料 前天 發生 基地 旁 道路 下方 自來 水管 線   瓦斯 管線 洩漏   連帶 造成 和平路 20 巷 地層下陷   由 於   天坑   填平 後   今天 又 他 處 塌陷   竹 市府 下午 成立 前進 指揮 所   市長 高虹安 提出 8 點 指示   包括 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置 並即 時 回報   確保當 地 安全       和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   前天 竟釀 緊鄰 巷弄 道路 下陷 後   被 市府 勒令停工   不過   因為 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 對 道路 持續 下沉 塌陷 狀況 相當 擔憂   市府 今天下午 請來 4 大技師 公會 到場 會勘                             高虹安 今天 中午 下令 於 竹光國 中旁 成立 災害 應變 前進 指揮 所   並 要求 廠商 與 消防局   警察局   都 發處   民政 處   產發處   區 公所 立即 派員進 駐   下午 4 點半   高虹安 會 同 土木 技師 等 四大 專業 技師 公會 民富 里 沈朝 旺里長 聽取 簡報   並 了解 居民 訴求       高虹安 今晚 臉書 發文 說明   針對 此案 已下 達 8 項 指示   包含 責成 消防局   工務處 與 產發處 聯 繫 自 來 水 與 瓦斯 公司 明天 立即 進場 全面 開 挖汰 換成 最新 管線   因無法 同 時汰換 兩種 管線   將 依序 先後汰換 自來 水 與 瓦斯 管線       由 於 傾斜計 監測 數值 逼近 警戒 值   高虹安 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置   並即 時 回報   要求 消防局 會同 民政 處   社會處 研擬 若事態 進 一步 擴大時   緊急 撤離 與 安置 措施   並預 準備       明天 開始 於 管線汰換 與 相關 改善 工程 期間   要求 廠商 每日 提供 足量 飲 用水 與 水車 供 停水 住戶 使用   要求 交通 處開放 周邊 停車場 供 居民 暫時 停放 車輛   竹光 國民運動 中心 免費 開放 居民 盥洗 使用       高虹安 說   確認 改善 完成 前   要求 災害 應變 前進 指揮 所 全天候 開設   隨時 提供 居民 諮 詢 與 處理 居民 回報 相關 問題   於 管線汰換 與 相關 改善 工程 期間   要求 警察局 做好 周邊 交通管制   確保 對 當地 交通 衝擊 降到 最低       高虹安說   今天 現場 與 當地 居民 溝通 與 聆 聽 心聲   並 一一 記錄   要求 廠商 與 局處 盡 全力 處理   強調 市府 團隊 一定 是 各位 最大 靠山   不僅會 要求 廠商 負起 責任   完成 改善 並經 確認 安全 無虞 之前   不得 進行 除了 安全工程 以外 其他 工程   新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影 新竹 市長 高虹安 今天下午 到 和平路 20 巷 了解 居民 心聲   圖 ／ 竹 市府 提供 新竹 市長 高虹安 今天下午 進入 建案 基地 勘查 狀況   圖 ／ 竹 市府 提供 新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影']</t>
         </is>
       </c>
     </row>
@@ -626,16 +626,16 @@
         <v>6</v>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6_台北市_台北_市府_信義區</t>
+          <t>6_台北市_台北_市府_地層下陷</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['台北市', '台北', '市府', '信義區', '街', '危險區', '地面', '北市', '道路', '塌陷']</t>
+          <t>['台北市', '台北', '市府', '地層下陷', '信義區', '街', '面積', '地面', '塌陷', '坍塌']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -649,21 +649,21 @@
         <v>7</v>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7_浴室_地底_溫泉_新北市</t>
+          <t>7_坑洞_破洞_區域_地下</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['浴室', '地底', '溫泉', '新北市', '投溫泉', '地面', '公共', '地上', '新北', '萬里區']</t>
+          <t>['坑洞', '破洞', '區域', '地下', '建管處', '坍陷', '塌陷', '土', '當地', '現場']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['新北市 萬里   加投 溫泉   公共 浴室   算是 古 蹟 了   它 是 日據 時期 就 蓋 好   而且 到現 很多 人   喜歡 來 這裡 泡湯   不過 上個 月 開始   這裡 出現 大大小小 問題   浴池 磁磚 掉落   水泥柱 裂痕   地面 嚴重 傾斜   因此 現在 浴池 已經 暫時 封閉 了   等到 廠 商都 修繕 完畢   確認 安全 都 沒 問題   才 會 再度 開放       鏡新聞 已 上架 86 台   若無法 收看   請 洽詢 當地系 統台     鏡新聞 APP   iOS 👉 https   reurl . cc kqyqML   鏡新聞 APP   Android 👉 https   reurl . cc Ay2y63   有話 鏡來講 YT 👉 https   reurl . cc A4DjQj   少年 新聞 週記 YT 👉 https   reurl . cc K4DeN9', '新北 萬里 加頭 溫泉 2 月份 被 遊客 發現   不僅 燈管   溫度 顯示氣 等等 設備 問題   更 地層下陷   因此 趕緊 請 公所 找人 檢修   目前 已經 緊急 封閉   確認 沒有 安全 疑慮   才 會 再度 開放     浴池 整塊 磁磚 脫落   地磚 不平   甚至 還 有些 地層下陷   看起 來 相當 老舊   這裡 是 新北 萬里 加頭 溫泉   從 日據 時代起   就 受到 不少 民眾 喜愛   許多人 泡 完湯   都 覺得 放 鬆 筋骨     不過 2 月份 卻 被 發現   不僅 燈管   溫度 顯示器   一些 溫泉 管線 設備 問題 外   還有 地層下陷 跡象   鐵鋁罐 放在 地上   都 會 不 自主   滾向 一邊   加上 後 方 就是 溫泉 露頭   要是 坍方 相當 危險   萬里區 長 黃 雱 勉     技師 建議 我們   要 專業 技師 公會 去   針對 結構物 下陷 狀況   去 監測   評估後續 是不是 可以 用   液壓 灌漿 部分 改善       地質 人員 透過 地雷 達 偵測 結果 發現   確實 男女 湯內 地底   大量 孔隙   造成 土壤 流失   目前 公所 已經   緊急 封閉 浴室   以民眾 安全 為 第一 考量   盡快 修建       封面 圖 ／ 東森新聞  ', '新北市 萬 里加 投溫泉 公共 浴室 歷史 悠久   吸引 許多人 前來 泡湯   不過   今年 2 月   有民眾 反應 溫泉 設備 出 問題   沒 想到 廠商 進場 維修 後   發現 浴池 磁磚 掉落   水泥柱 充滿 裂痕   地面 嚴重 傾斜 等 狀況   更 仔細 勘查 下   竟然 地層下陷 現象   地質 檢測 人員 檢查   原來 湯室 地底 大量 孔隙   造成 土壤 流失   目前 封閉 整修     鋁罐 放在 地上 一路 滾 不停   不 只 地面 嚴重 傾斜   浴池 還有 一 大片 磁磚 脫落   水泥柱 充滿 裂痕   原來 這處 溫泉 發生 地層下陷     新北市 萬 里加 投溫泉 公共 浴室 日治時 代興建   歷史 相當 悠久   水質 相當 不錯   吸引 許多人 前來 泡湯     不過 今年 2 月 開始   就 泡 湯遊客 反應   燈管   溫度 顯示器 溫泉 管線 設備 問題   區 公所 派 人 前往 了解 狀況   由廠 商進場 維修   發現 不 只是 設備 故障   還有 磁磚 脫落   地磚 不 平等 狀況   仔細 勘查 下 發現 地層下陷 現象   公所 從 4 號開始 封閉 浴室   趕緊 找 專業 技師 到場 檢查   男女 湯室 地底 大量 孔隙   造成 土壤 流失   懷疑 可能 跟 一旁 溫泉 露頭 有關 係     大鵬里長 李建才     露頭 我 不敢 說絕 對 沒 有關 係   因為 這個 是 相通 東西   地底下 看不到   以 目前 整個 狀況 來講 話   下陷 狀況 速度 應該 不是 很 急速   這是 很多年 類似 有點 掏空 感覺       溫泉 從 溫泉 露頭 自然 湧出   抽到 蓄水池 後   流入 浴池   可能 連帶 影響 地基 被 掏空     萬里區 長 黃 雱 勉     技師 建議 我們 要 專業 技師 公會   針對 結構物 下陷 狀況 去 監測   再 去 評 估後續 是不是 可以 用液 壓 灌漿 部分 改善   還是 可能 要大動 作去 做後續 改建   這個 部分 後 續 可能 會 需要 比較 多 費用       公所 強 調 儘 快 修建 完成   提供 民眾 安全 舒適 泡 湯空間  ']</t>
+          <t>['路透 報導   一段 無人機 影片 揭露 巴塔 蓋卡 坑洞   Batagaika   crater   近況   這道 長 1 公里 塌陷 區域 位 於 俄羅斯遠 東地區   是 世上 最大 永凍土 巨坑   俄羅斯薩哈 共和 國的 當地 人稱 之 為   地獄 之門         影片 中   兩名 探險者 爬過 巨坑 底部 凹凸不平 地形   這種 高低 起伏 地表 1960 年代 周圍 森林 整地 後 開始 形成   因 地下 永凍土 融化 導致 地層下陷                             當地 居民 兼 探險 家史 特魯奇 科夫   Erel   Struchkov   表示     當地 人稱 之 為 塌陷   1970 年代 形成   最初 是 條溝 壑   然後在 晴天 高溫 下 解凍   開始 擴大         科學家 說   俄國暖化 速度 比 世界 其他 地區 至少 快 2.5 倍   占 俄國國 土面 積達 65% 苔原 因此 融化   釋出 溫室 氣體       位 於 亞庫 次克 梅爾 尼科夫 永凍土 研究所 首席 研究 員尼塔納 納耶夫   Nikita   Tananayev   表示   雖然 這 可能 吸引 遊客   但 坑洞 擴大是   危險訊號       今 後   隨著 氣溫 升高 人 為 壓力 增加   我們將 看到 越來 越 多 這種 巨型 塌陷 形成   直到 所有 永凍土 都 消失 為止         永凍土 融化 已威脅 到 俄國 北部 與 東 北部 城鎮   導致 道路 坍塌   房屋 崩裂   管線 中斷   最近 幾季 愈演愈烈 大規模 野火 使 問題 更加 嚴重       薩哈 共和 國當 地人 注意 到 巨坑 迅速 擴大   史特魯奇 科夫 說       兩 年前   巨坑 邊緣   距離 這條 小路 大約 20 到 30 公尺   現在 它 顯然 離 我們 更 近 了         科學家 不 確定 巴塔 蓋卡 坑洞 擴大 確切 速度   但是 塔納納 耶夫 說   巨坑 下面 土地   有些 地方 深約 100 公尺   含有   大量   有機 碳   隨著永凍 土 融化   這些 機碳 將釋 放到 大氣 中   加劇 全球 暖化     隨著 氣溫 升高   我們 可以 預計   巨坑   將以 更 快 速度 擴大   這將 導致 未來 幾年 氣候 更加 暖化             路透 報導   一段 無人機 影片 揭露 巴塔 蓋卡 坑洞 近況   這道 長 1 公里 塌陷 區域 位 於 俄羅斯遠 東地區   是 世上 最大 永凍土 巨坑   俄羅斯薩哈 共和 國的 當地 人稱 之 為   地獄 之門     路透', '首次 上稿   00   04 更新 時間   06   09   〔 記者 蔡亞樺 ／ 台北 報導 〕 台北市 信義區 崇德 街 60 巷一處 華熊 營造 建案 工地 旁 巷道   13 日 下午 3 點多 發生 地層下陷   出現 長 15 公尺   寬 3 公尺   深 3 公尺 巨大 坑洞   台北市 政府 與 建 商展 開搶 救   灌漿 填補 坑洞 與 建案 基地   晚間 11 點 坑洞 初步 填平 完成   北市 府 啟動 預防性 疏散   疏散 安置 11 名住 戶到 旅館 住宿     台北市 建管處 指出   崇德 街 60 巷華熊 營造 建築 工地 旁發生 道路 坍陷   建管處 收到 訊息 立刻 派員 現場 了解   工地 正 進行 地下室 開挖   因連續 壁體 滲水 造成 地下水 湧入 引發 道路 坍陷   立即 指揮 承造 人 進行 緊急 處置   要求 基地 外 道路 下陷 處 進行 灌漿 回填   基地 內採 填砂 灌水 以 平衡 水壓   至 13 日 晚間 11 點 道路 下陷 處 已 初步 填補 完成   趨 於 穩定   基地 仍 監督持續 進行 填砂 灌漿     台北市 建管處 長 虞 積學 表示   經 建管處 緊急 聯 繫   台北市 土木 技師 公會莊 理事 長 結構 技師 公會 徐 理事 長   均 第一 時間 趕 現場 協助 緊急 處置 事宜 確認 疏散 範圍   目前 採預 防性 疏散 措施   疏散 12   24 號計 5 戶 需 安置 11 名住 戶   均 已 安排 至 旅館 住宿     虞積學 強調   該 建案 違反   建築法   部分 現場 已 立即 勒令停工   並處 以 18 萬元罰 鍰   建管處 將持續 現場 指揮 搶 救   現場 並已 要求 承商 加強 設置 周遭 鄰房 安全 觀測   提高 觀測 頻率   直到 確認 安全 無虞   該 工地 目前 已 勒令停工   後 續須 確認 週邊 地質 鄰房 安全 無虞   並檢具 改善 計畫 經相關 公會 審 查核 可 後   始得 復工  ', '〔 記者 楊 心慧 ／ 台北 報導 〕 台北市 信義區 崇德 街 60 巷華熊 營造 建案 工地 旁 巷道   昨   13   日 下午 發生 地層下陷   出現 長 15 公尺   寬 3 公尺   深 3 公尺 巨大 坑洞   昨晚 灌漿 填補 坑洞 與 建案 基地   坑洞 初步 填平 完成   但 目前 為將 土水壓 平衡   仍 基地 內持續 灌水   台北市 都 發局 長 王玉芬 今   14   日 上午 說明   灌水 作業 預計 今 下午 完成   至於 住戶 回家 需達 3 條件   估計 作業 需 1 至 2 週     王玉芬 今 上午 抵達 現場 說明 進度   並 表示 造成 道路 塌陷 初步 判斷 是 工地 地下 連續 壁 約 11   12 公尺 處有 破洞   造成 水 與 砂往 工地 內流   產生 破洞 原因   疑似 為 連續 壁 施工 時有 包土 狀況   目前 已 坑洞 進行 灌漿 回填   基地 內則 採填砂 灌水 以 平衡 水壓     至於 安置 在外 住戶   王玉芬 指出   住戶 回到 家 需有 3 個 條件   包含 透過 雷達 探測 檢查 無 孔洞 或 軟弱 土層   監測 建築物 無 傾斜   由 專業 技術 人員 進入 屋內 檢查 無 毀損 或 裂縫   預計 時間 需 1 至 2 週   希望 可盡 早 完成   讓 住戶 回到 家園   安置 費用則 由 廠商 全部 負擔     針對 現場 作業 進度   王玉芬 說   目前 基地 水位 地下 5.5 公尺   大約 下午 會 灌到 地下 3 公尺   雖然 昨晚 已 初步 判斷   狀況 趨 於 穩定   但 北市 府 要求 持續 灌水 至 地下 3 公尺 處   預計 灌水 作業 今 下午 可 完成     台北市 信義區 長 陳 冠伶今 受訪 表示   調查 結果 撤出 有七戶   需要 安置 住戶 一共 5 戶 10 人   目前 都 安置 信義區 旅館   按照 規定 發生 緊急 災害 補助 可 申請 安置 補助   每人 一天 1600 元   最多 可 申請 七天   超過 部分   廠 商承諾 超出 部分 可 負擔  ']</t>
         </is>
       </c>
     </row>
@@ -672,21 +672,21 @@
         <v>8</v>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8_紐約市_紐約_城市_市區</t>
+          <t>8_台北市_區域_當地_〔</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['紐約市', '紐約', '城市', '市區', '高樓', '洪災', '海水倒灌', '大樓', '防洪', '建築物']</t>
+          <t>['台北市', '區域', '當地', '〔', '〕', '地層下陷', '地下水', '路段', '地方', '地基']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['紐約市 正在 下陷   美國 地質 專家 研究 發現   由 於 紐約市 摩天 大樓 眾多 加上 地質 變動   部分 紐約市 地層 已 下陷 至少 2 公分   未來 若 再 加上 海平面 上升   恐讓 沿海 地區 居民 生存 備受 威脅     紐約 每年 均 下沉   據   獨立報   報導   紐約市 人口 約 800 萬   美國 地質 調查局 研究 人員 指出   包括 布魯克林   皇后 區與 下曼哈頓 部分 紐約市 因為 地層下陷   每年 下沉 1 到 2 公分                           該 研究 更納入 土壤 條件 與 100 萬棟 大樓 7620 億 公斤 重量 等 因素   除此之外   研究 更 指出   紐約 市還 面臨 洪水 危害 風險     海平面 上升 亦 是 威脅   稍早 研究 曾 指出   全球 暖化 帶來 海平面 快速 上升   2050 年前 全球 海平面 將 上升 200 到 600 公分     研究 人員還 指出   紐約市 每年 下陷 約 1 到 2 公分   部分 地區 下沉 速度 更 快   原因 除了 近期 不斷 興建 摩天 大樓 外   還 包括 抽取 地下水   土壤 壓實 與 地震 等 因素   都市 建築物 面臨 其他 風險   例如 地層 暴露 鹽水 後   可能 導致 鋼筋 混凝土 受到 侵蝕   因此 減少壽命     下 沈是 自然 造成   據   Live   Science   報導   研究 指出   紐約市 下 沈 部分 原因 可能 是 自然 形成   因為 上 一次 冰河 時期 最 寒冷 時候   巨大 冰層 曾 覆蓋 大部分 地球   造成 冰層 下方 地面 下陷   進而 讓 陸地 邊緣 升起   等到 冰層 融化 後   被 抬升 地區則 開始 下陷     之前 研究 就 指出   到 2100 年   美國 東岸 可能 會 下陷 48 至 150 公分   除了 大自然 力量 之外   研究 人員 認為還 可能 包括 其他人 為 因素   且 科學家 發現 當地 某些 地區 下沉 速度 更 快   原因 可能 是 建築物 重量 造成     本次 研究 結果 刊登 Earth   s   Future 期刊   【 更 多 精采   詳見 】', '一項 最新 研究 發現   美國 紐約市 長 期 承受 大量 建築物 重量 之下   地層 正在 下陷   加上 紐約市 海平面 上升 速度 高居 全球 2 倍 以上   恐為 紐約市 招致 洪災 等 危機     圖 ／ Unsplash   一項 最新 研究 發現   美國 紐約市 長 期 承受 大量 建築物 重量 之下   地層 正在 下陷   加上 紐約市 海平面 上升 速度 高居 全球 2 倍 以上   恐為 紐約市 招致 洪災 等 危機       美國 有線 電視 新聞網   CNN   報導   據 推估   紐約市 2050 年 海平面 將 上升 8 至 30 英寸   20.32 至 76.2 公分     更 重要 是   科學家 預期 由 於 人 為 引發 氣候 危機   類似 東北 風暴   nor   easter     颶風 這類 極端 降雨 事件 將更頻 繁地 出現       美國 地質 調查 所   US   Geological   Survey   專家 帕森斯   Tom   Parsons   說     我們 離 海水倒灌 還有 一段 很長 路 … 但 我們 紐約 市經 歷過 數次 嚴重 颶風 事件   像 颶風珊迪   Sandy   艾達   Ida   帶來 暴雨 使得 城市 淹水 成災   都市化 帶來 部分 影響 使得 水災 發生         這篇論 文發表 期刊   地球 未來     Earth   sFuture   上   旨在 展示 沿海   河濱 或 湖濱 地區 高樓 大廈 何以 增加 未來 洪災 風險   以及 應 採取 相關 措施 來 降低 潛在 危險 衝擊       研究 人員藉 當時 紐約市 5 個 行政 區約 108 萬座 建築物 質量   計算出 這些 建築物 重量 約 為 7620 億 公斤   相當 於 約 190 萬架 滿載 波音 747   400 客機       研究 團隊 接著 利用 模擬 方式   計算出 這些 重量 對 地面 影響   並和 顯示 實際 地表 地質 情況 衛星 數據 進行 比 較   帕森斯 說   這項 分析 揭露 紐約市   平均 每年 下陷 約 1 至 2 毫米   部分 下陷 較 嚴重 地區 每年 下陷 約 4.5 毫米         然而   並非 所有 地層下陷 都 是 建築物 造成   帕森斯 說     我們 可想 見 非常 鬆 軟 土壤 人工 填土 地面 上 建造 建築 地層下陷 關聯 … 其他 地方   我們則 看到 難以 解釋 地層下陷   它 很多 不同 成因   例如 上個 冰河 時期 後 發生 後 冰期 回落   或是 抽取 地下水         研究 表明   地層下陷 可能 比 海平面 上升 更 早構 成洪災 威脅   而且 這種 情況 不 只 發生 紐約市       帕森斯 說     這是 一個 全球性 問題   我來 自羅德島 大學   University   of   Rhode   Island   合著 者 研究 了 世界各地 共 99 座 城市   不 只有 沿海 城市 內陸 城市   其中 絕 大多 數都 存在 地層下陷 問題           Take   action   加入   倡議 +    ', '一項 最新 研究 發現   美國 紐約市 長 期 承受 大量 建築物 重量 之下   地層 正在 下陷   加上 紐約市 海平面 上升 速度 高居 全球 2 倍 以上   恐為 紐約市 招致 洪災 等 危機     美國 有線 電視 新聞網   CNN   報導   據 推估   紐約市 2050 年 海平面 將 上升 8 至 30 英寸   20.32 至 76.2 公分     更 重要 是   科學家 預期 由 於 人 為 引發 氣候 危機   類似 東北 風暴   nor   easter     颶風 這類 極端 降雨 事件 將更頻 繁地 出現                           美國 地質 調查 所   US   Geological   Survey   專家 帕森斯   Tom   Parsons   說     我們 離 海水倒灌 還有 一段 很長 路 … 但 我們 紐約 市經 歷過 數次 嚴重 颶風 事件   像 颶風珊迪   Sandy   艾達   Ida   帶來 暴雨 使得 城市 淹水 成災   都市化 帶來 部分 影響 使得 水災 發生       這篇論 文發表 期刊   地球 未來     Earth   sFuture   上   旨在 展示 沿海   河濱 或 湖濱 地區 高樓 大廈 何以 增加 未來 洪災 風險   以及 應 採取 相關 措施 來 降低 潛在 危險 衝擊     研究 人員藉 當時 紐約市 5 個 行政 區約 108 萬座 建築物 質量   計算出 這些 建築物 重量 約 為 7620 億 公斤   相當 於 約 190 萬架 滿載 波音 747   400 客機     研究 團隊 接著 利用 模擬 方式   計算出 這些 重量 對 地面 影響   並和 顯示 實際 地表 地質 情況 衛星 數據 進行 比 較   帕森斯 說   這項 分析 揭露 紐約市   平均 每年 下陷 約 1 至 2 毫米   部分 下陷 較 嚴重 地區 每年 下陷 約 4.5 毫米       然而   並非 所有 地層下陷 都 是 建築物 造成   帕森斯 說     我們 可想 見 非常 鬆 軟 土壤 人工 填土 地面 上 建造 建築 地層下陷 關聯 … 其他 地方   我們則 看到 難以 解釋 地層下陷   它 很多 不同 成因   例如 上個 冰河 時期 後 發生 後 冰期 回落   或是 抽取 地下水       研究 表明   地層下陷 可能 比 海平面 上升 更 早構 成洪災 威脅   而且 這種 情況 不 只 發生 紐約市     帕森斯 說     這是 一個 全球性 問題   我來 自羅德島 大學   University   of   Rhode   Island   合著 者 研究 了 世界各地 共 99 座 城市   不 只有 沿海 城市 內陸 城市   其中 絕 大多 數都 存在 地層下陷 問題    ']</t>
+          <t>['〔 記者 吳昇儒 ／ 新北 報導 〕 受   尼莎   颱 風共伴 效應 影響   新北市 汐止 地區 降下 豪 大雨   不 只 發生 土石 流   就 連工 建路 出現 地層下陷 情形   工務人員 初步 搶 修後工 建路 一度 恢 復 通行   但 昨日 夜間 卻 發現 地基 仍須 補強   必須 再次 施工   警方 獲報 後   立刻 派員 前往 進行 交通管制   全線 封閉 該 路段   為 加快 搶救 速度   警方 還 徒手 協助 搬運 30 多輛 機車   讓 工程 能 順利 進行     汐止 區工 建路 地層下陷 後   經工務 人員 搶 救   暫時將 凹陷 地基 填補 起來   未料 這兩天 又 因受 豪雨 影響   再此 下陷   汐止 警 分局 接獲 通報 後   即刻 拉起 封鎖線   並連夜 將規劃 好 改 道路 線 公告 各 臉書 地方 集團 供民眾 參考     深夜 中   員警手 拿 指揮棒   持續 管制 車流   柏油路 面上 出現 許多道 裂痕   除了 用 交通 錐 警示 阻擋   立起 告示牌   請行經 車輛 改道 行駛   經過 徹夜 管制 後   施工 單位 評估 現場 完畢 於 今早 6 點準備 開工   卻 發現 許多 機車 車主未 依 通知 移置 車輛   造成 施工 路段 周圍 停滿 機車   負責 交通管制 社后 派出所 2 名員警   見狀 趕緊 上前 幫忙   短短 10 幾分鐘 就 徒手 移 了 3   40 台機車   讓 搶 救 工程 得以 順利 進行     新北 市長 侯友宜 上午 特別 到工 建路 了解 現場 狀況   並感謝 汐止 警 分局   區 公所 施工 單位   連夜 辛苦 進行 管制 勘查   並 指示 相關 單位務 必 儘 速 完成 搶修 並維持 交通 順暢   全力 協助民眾 解決 問題     民進 黨籍 市議員 張錦豪 請 助理 前往 工 建路 現場   向 周邊 住戶 詢問 是否 需要 協助 之處   並與 施工 單位 保持 聯 繫   希望 能 早日 恢 復 正常 通行  ', '〔 記者 蔡思培 ／ 台北 報導 〕 台北市 近來 天坑 事件 頻傳   萬華區 一處 建案 工地 旁 道路 日前 發生 地層下陷   坑洞 面積 約 一輛 汽車 車身   所幸 無人 受傷   不過當 地里 長 蔡岳樺 表示   工地 已 二度 出包   天坑 修補 後 又 出現 積水   北市 議員 應曉薇 質疑   建案 若 未 側溝   未來 仍 可能 天坑 事件   台北市 建管處 表示   會 要求 將 排水 系統 完   已將個 案列 為 重點 稽查 個案     應曉薇 今天 與 多位 萬華里 長 前往 萬華 工地 會勘   應曉薇 質疑 建案 是否 側溝   若側 溝都 沒有   未來 仍 可能 天坑   若 再有 大雨   台北市 衛工處 又 要 幫忙 清砂   發現   坑洞 日前 雖已 填補   但現 又 出現 積水   對 於 台北市 副 市長 李 四川 認為 路 塌 與 極端 氣候 溫室 效應 有關   她則 稱 這 就是 沒有 側溝 造成 人 為 疏失     蔡岳樺 說   福音 里 3 個 工程   每次 都 是 這個 建案 出事   他 對 於 都市 更新 樂觀 其成   但 不 希望 影響民眾 安全   他 呼籲 建商 出事 要 負責   不要 什麼 就 推給 別人   蔡 表示   天坑 意外 當天 建案 負責人 推 託 說 下雨   地基 掏空   又 說 沒 危險 沒什麼   讓 他 相當 憤怒   難道 要 出事 才 算 問題   呼籲 建商要 把 事情 做好     萬華區 全 德里 里長 趙 素美 認為   這個 問題 應該 可以 提前 處理   不能 發生 事情 才 處理   里長 都 為 里 民保護 身家 財產   建商 與 里 長 應該 互相 尊重     建管處 表示   此 都 更案 採用 是 舊 法令   本案 涉有 公有   私有土地   法令 上不會 要求 現在 就 按照 使用 執照 竣工 時 排水 系統 完   但 目前 排水 系統 不 完整 才 導致 大雨 後 排水 不順 地基 下陷   現行 法令 對 於 打通 道路   區域 排水 沒 規範   但 建管處 會 要求 將 排水 系統 完   改善 區域 排水     建管處 說   已將 此案 列為 重點 稽查 個案   未來會 加強 稽查   目前 坑洞 已 填好   初步 安全 無虞   並將 安全 疑慮 地方 阻隔  ', '宜蘭縣 蘇澳鎮 民富 街   部分 路段 緊臨 蘇澳 海事 游泳池   居民 質疑   疑似 校方 長 期為 泳池 抽 地下水   導致當 地底 層 下陷   連 住家 地基 都 被 掏空   嚴 重影 響 居住 安全   校方 否認 超 抽 地下水   立委 陳 琬惠會 同 教育部   水利 署 官員   到 當地 與 居民 研商 解決 辦法   宜蘭 蘇澳鎮 民富 街 部分 與 蘇澳 海事 緊鄰 路段   長 年 發生 地層下陷 問題   住戶 房子 地基 被 掏空   地面   牆面 出現 裂縫   從 住家 滾一個 鐵罐 到 道路 對面   相當 順暢   可以 見 到 坡度 相當大   且 道路 表面 比旁邊 側溝 還要 矮   根本 沒有 排水 功能   居民 指出     游泳池 建好 以 後   大概 有用 了 4 年 多 就 塌 掉 了   影響 到 我們     當地 地層下陷 情況   從 2017 年 蘇澳 海事 游泳池 塌陷 後   就 開始 發生   多年 來無法 完全 改善   即使 2021 年 蘇澳 海事 當地 進行 壓力 灌漿   道路 仍持續 塌陷   居民 質疑   當年 是 蘇澳 海事 為 了 游泳池 超 抽 地下水   才 導致 地層下陷 情形   教育部 高級 中等教育 組 行政 資源 科長 黃 懷瑩 表示     我覺 得 地質 監測 這一塊   我們 可以 持續   讓 大家 安心 說   我們 是不是 持續 劇烈 沉降 或 傾斜 狀況   會 定期 跟 大家 報告 我們 監測 結果     校方 否認 超 抽 地下水   表示 當年 泳池 塌陷 後 就 沒 抽水   過去 抽 是 溢流 出 地面 水源   教育部 則說   過去 壓力 灌漿 是 延緩 地質 沉降 效果   立法 委員陳琬惠 表示     房子 跟 道路 就是 脫離 當中   所以 我 希望 我們 今天 要 找到 一個 方法   不是 只有 檢測 而已     水利 署 組長 簡昭群 說     技師 公會 去 依據 他 測量 結果   找出 造成 沉陷 具體 原因     陳 琬惠 近期 邀集 中央 單位 與 地方 居民 開會   研商 解決 辦法   水利 署 說   要 確定 當地 地層下陷 真正 原因   是 抽水 行為 還是 土質 問題   才能 根治 問題  ']</t>
         </is>
       </c>
     </row>
@@ -695,21 +695,21 @@
         <v>9</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9_農地_耕作_公頃_農業</t>
+          <t>9_坑洞_市府_坍陷_路面</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['農地', '耕作', '公頃', '農業', '農會', '作物', '環保局', '土地', '國產', '農民']</t>
+          <t>['坑洞', '市府', '坍陷', '路面', '塌陷', '道路', '北市', '巷', '地基', '天坑']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['〔 記者 陳 彥廷 ／ 屏東 報導 〕 屏東縣 政府 於 東港   林邊   佳冬 枋寮 4 個 沿海 鄉鎮   劃定   嚴重 地層下陷區 光電計畫   專區   為確 保農民 耕作 權   不過   近來坊 間質 疑聲 浪漸 漲   環保局 強調   該區 計畫 發電量 為 800MW   百萬瓦     不會 無 限制 擴張   因此 至少 會 仍 3000 公頃 以上 農地 可供 農作     地面 型 光電場 成為 選戰 攻防 議題   屏東 因 沿海 嚴重 地層下陷區 為 全國 首個 縣府 核淮得 設光 電案場 專案   成 在野 黨攻 詰 對象   近期 坊 間 又 再 傳出 農民因 種電 失去 農保   老農 退場 又 留不住 青農及 蛇 鼠 窩 藏 副作用 等 爭議     屏縣 府 環保局 指出   這 4 鄉鎮過 去 因超 抽 地下水   曾列 為 嚴重 地層下陷區   現 仍屬 第 1   2 級 地下水 管制 區   且 海水 上溯 下   許多 土地 都 已 出現 鹽化   不少 已 是 不利 耕地 多年   因此 縣府 尊重 地主 利用 土地 意願 權益 前提 既有 電力 設施 併 網 上限 條件 下   限度 推動 光電 專區   預計 發電量 為 800MW     環保局 指出   部分 農地 轉作 太陽 光電 後   減少 農民 抽取 林邊 溪 下游 地下水 需求   並 搭配 上游 設置 大 潮州 人工湖 補注 地下水   減緩 地層下陷   達到 國土 復 育及 產業 永續 發展 目的   而 近年 同樣 大小 光電板 發電 效率 已較 八八 風災 後   養水 種電   到 近 2 倍   單 一片 就 可 發電達 400w   以 目前 併 網約 300MW 太陽光 電裝置 容量   使用 農地 比例 約 250 公頃 左右   未來 達 到 目標 單位 發電量 更大下   所 需面積 比例 一定 更 小   至少 會 3000 公頃 以上 農地 可供 農作 使用   另外   對 於 無力 管理 田間 工作   又 土地 鹽化 等 不利因素 無法 耕作 年 邁老農   則 可以 穩定 收入 過 退休 生活     至於 農保 問題   環保局 重申   農地 若 有意 願 出租 供 人 種電   一定 要 進行 變更 地目   但 這是 完全 基 於 地主 利用 土地 意願 權益   縣府 環保局 從 未 要求 廠商 提供 所謂   不利 耕作 同意 書   或 其他 網路 媒體 謠傳 不 平等 條約 相關 文件   先前 更 製 作 地主 注意 事項 手冊 Q &amp; A 圖卡   公告 於 縣府 綠辦 官網   讓 地主 了解 相關 權利 與 義務   只要 民眾 對 合約 疑問   均 可 撥 打 專線 電話詢 問綠能 專案 推動辦 公室   針對 部分 地區 爭議 案件   未 取得 居民 同意 之前   縣府 已 要求 業者 停止 施工     蛇鼠 患 問題   縣府 環保局 長 顏幸 苑則 認為   作物 收成 期間 食物 充沛 易 引鼠   鳥禽 覓 食   但 太陽能 案場 並無食源   應非屬 引鼠 主因   縣府 要求 專案 輔導業者 維護 周遭 環境 整潔   至於 選址 不當   縣府 重申   屏東縣 綠能 推動 政策 以   專案 專區 計畫       土地 複 合式 利用   兩大 策略 為主   專案 為 限度 使用 相對 不 適合 耕種 土地 發展 綠能   專案 專區 外 鄉鎮 優先 鼓勵 結合 既有 設施 與 光電   複 合 利用   方式     屏東縣 環保局 表示   民眾 對 於 光電 發展 與 環境 保護 議題 逐漸 重視   縣府 尊重 私有 地主 處置 自家 土地 財產   以及 業者 依法 申請 案件 權利   惟審查 過程將 審慎 關注 山坡地   耕作 農地   歷史 遺跡   生態 保育 或 重要 觀 光景 點聯絡 道路 沿線 等 議題   並 要求 廠商 提出 因應 作為   以 避免 衍生 爭議性 問題   兼顧 開發 合理性 及維護 本縣 農民 耕作 權益  ', '〔 記者黃淑莉 ／ 雲林 報導 〕 防治 高鐵 沿線 地層下陷   行政院 同意 明年 一期 作恢 復 雲林 高鐵 沿線 左右 一 公里 半範圍 農民種 植 低耗 水 作物 節水 獎勵   即種 植轉作 作物 每公頃 給予 三萬元   種綠肥 四萬 二千元   種景觀 作物 五萬 二千元     雲林 高鐵 沿線 地層下陷 嚴重   避免 影響 到 高鐵行車 安全   中央 相關 部會   雲林縣 府 近 幾年 積極 推動 地層下陷 防治 工作   農業 方面 輔導 沿線 種植 水稻 農民 轉作 高粱   大豆 等 低耗 水 作物   減少 地下水 抽取 量     縣府 農業 處 表示   為 鼓勵 農民 農委會 二 一 三年 推出 節水 獎勵   針對 雲林 高鐵 沿線 三 公里 範圍 轉作 低耗 水 作物 或 運用 科技 節水 農業 生產者 獎勵     農業 處 指出   獎勵 計畫 二 一 三年 至 二 二 年期 間   地下水 抽取 減少   地層下陷 明顯 減緩   獎勵 計畫 截止 後   統計 發現   高鐵 沿線 第一期 作種 稻面積 又 恢 復   為 避免 地層下陷 再 惡化   縣府 向 中央 爭取 持續 辦理節 水獎勵   經 行政院 審查 核定 明年 第一期 作恢 復 節水 獎勵     農業 處 說   這次 行政院 核定 是 針對 雲林 虎尾   土庫   元長 北港 等 四鄉 鎮高鐵 沿線 左右 一 公里 半內 農地   獎勵 措施 比照   綠色 環境 給付 計畫   中水 資源 競用 區大區 輪作 節水 獎勵 額度   歡迎 符合 申辦 資格 農民 踴躍 配合  ', '〔 記者黃淑莉 ／ 雲林 報導 〕 為 防治 地層下陷   行政院 同意 明年 一期 作恢 復 高鐵 沿線 左右 1.5 公里 半範圍 農民種 植 低耗 水 作物 節水 獎勵   即種 植轉作 作物 每公頃 給予 3 萬元   種綠肥 4 萬 2000 元   種景觀 作物 5 萬 2000 元     有鑑 雲林 高鐵 沿線 地層下陷 嚴重   避免 影響 到 高鐵行車 安全   中央 相關 部會   雲林縣 府 近 幾年 積極 推動 地層下陷 防治 工作   其中 農業 方面 輔導 沿線 種植 水稻 農民 轉作 其他 節水 作物   減少 地下水 抽取 量     縣府 農業 處 指出   農委會 2013 年 至 2020 年 辦理 雲林 高鐵 沿線 3 公里 範圍 內節 水獎勵   給予 轉作 低耗 水 作物 或 運用 科技 節水 農業 生產者 獎勵   有效 減少 地下水 抽取   地層下陷 明顯 減緩     農業 處 表示   獎勵 措施 至 2020 年 截止   去年 今年 沒有 辦理   統計 發現   高鐵 沿線 第一期 作種 稻面積 又 恢 復   為 避免 地層下陷 再 惡化   縣府 向 中央 爭取 持續 辦理節 水獎勵   經 行政院 審查 核定 明年 2023 年 第一期 作恢 復 節水 獎勵     農業 處 說   這次 行政院 核定 是 針對 雲林 虎尾   土庫   元長 北港 等 四鄉 鎮高鐵 沿線 左右 1.5 公里 農地   獎勵 措施 比照   綠色 環境 給付 計畫   中水 資源 競用 區大區 輪作 節水 獎勵 額度   歡迎 符合 申辦 資格 農民 踴躍 配合   相關 資訊 可 洽詢 縣府 農業 處  ']</t>
+          <t>['北市   天坑   事件 接連 3 天發生   今 傍晚 萬華區 昆明街 320 巷 出現 路面 坑洞   民進 黨 北市 議員 洪婉臻 晚間 表示   短短 時間 發生 多起 塌陷 意外   道路 品質 堪憂   根本 不堪 大雨 考驗   每下 一次 大雨 前進 指揮 所 就 出動   然 後 各局 處分別 擔責任   批 市府 便宜行事   罔顧 公共安全       洪婉臻 說   昆明街 320 巷 9   2 號 今天下午 4 點 42 分出 現 天坑 事件   該 事件 是 因建案 開 挖   造成 長 3 公尺   寬 2 公尺   深度 1.5 公尺 地層下陷   約 一輛 汽車 車身   所幸 塌陷 部分 位 工地 範圍   未影響 到民眾 安全 與 通車                             表示   據 建管處 施工 科回報   查明 連續 壁 並無滲 水破損 情形   與 之前 南京 西路 發生 塌陷 原因 不同   比較 可能 是 因為 連日豪 大雨 造成 土 質 鬆 動   才 發生 整體 事件   因 基地 退縮 建築線 3.64 米開 挖   故 坍陷 處裡開 挖面 仍 2 至 3 米 距離   坍陷 原因 還在 查明       洪婉臻 指出   繼 之前 大同 區 南京 西路 後   今天 已 是 北市 第 3 次 發生 路面 塌陷 事件   短短 時間 發生 多起 塌陷 意外   北市 道路 品質 堪憂   根本 不堪 大雨 考驗   直言 北市 府 真應 該 好好 檢討 路面 品質       呼籲 市府   對 於 道路 品質 不要 便宜行事   屢次 臨時 抱 佛腳   每下 一次 大雨 前進 指揮 所 就 出動   然 後 各局 處分別 擔責任   上次 是 衛工處   這次 是 建管處   簡直罔顧 公共安全     一次 又 一次   只會 讓 人民 對 政府 失去 信心           北市   天坑   事件 接連 3 天發生   今 傍晚 萬華區 昆明街 320 巷 出現 路面 坑洞   圖 ／ 洪婉臻 辦 公室 提供   北市 短短 3 個 月 出現 第 5 個   天坑     此為 今日 萬華區 某處 工地   圖 ／ 居民 提供', '繼 前天 南港區   昨日 中山 區   北市 今 傍晚 萬華區 某處 工地 再現 路面 坑洞   這也 是 北市 短短 3 個 月 出現 第 5 個   天坑     台北市 工務局 表示   該處 為 新建 工地   疑 基地 外舊 水溝 加上 地基 較 鬆 軟   遇上 大雨 沖 刷   導致 土石 流失 下陷   這處 天坑 約長 3 公尺   寬 2 公尺   深度 1.5 公尺   無人 受傷   已畫 設 警戒 線   淘空 點位 在建 築 基地   建商 已 接手 灌漿 處 理完 畢       萬華區 天坑 位 於 昆明街 320 巷 9   2 號 新建 工地 旁   今天下午 16 時 42 分 左右   疑似 因 基地 外舊 水溝 加上 地基 鬆 軟   遇 大雨 沖 刷   導致 土石 流失 下陷                             北市 府 表示   這起 萬華 地層下陷   長 寬 約 一輛 汽車 車身   還好 塌陷 時   無 造成 人員 受傷   目前 北市 府 已 畫設 警戒 線   消防局 已 現場 成立 前進 指揮 所 警戒 守視       新工處 表示   本案 經 工地 主任 說明   是 因 基地 外舊 水溝 加上 地基 較 鬆 軟   遇上 大雨 沖 刷   疑似 導致 土石 流失 下陷   建商 已 緊急 調用 水泥 車搶修   晚間 19 時 完成 灌漿 回填 作業   目前 初步 評估 並無 擴大 危害 之虞       北市 近期 五度 出現 路面 坑道   分別 為 5 月 13 日 信義區 崇德 街   7 月 10 日 大同 區 南京 西路   8 月 18 日 南港區 南港路   8 月 19 日 中山 區 民生 東路   以及 今天 萬華區 昆明街   北市 萬華 某處 工地 今天 出現 路面 坑洞   圖 ／ 居民 提供 工務局 表示   掏空 點位 在建 築 基地   建商 已 接手 灌漿 處 理完 畢   圖 ／ 居民 提供 北市 短短 3 個 月 出現 第 5 個   天坑     此為 今日 萬華區 某處 工地   圖 ／ 居民 提供 北市 萬華 某處 工地 今天 出現 路面 坑洞   圖 ／ 居民 提供', '台北市 短短 3 個 月 出現 4 個 天坑   遭批 天龍國 變成 了   天坑 國     對此   工務局 今   20   日強 調   今年 發生 四案 道路 坑洞 情形   均 非 道路 受 輾壓 破 損導致   工務局 已針 對 四案 成因 擬定 預防 道路 塌陷 方案   以 避免 類似 情形 發生   北市 民生 東路 二段 159 巷口 19 日 晚間 出現 道路 坑洞   新工處 接獲 通報 立即 調派 開 挖機 進場   確認 為 路旁 側溝 破損 造成 道路 掏空   新工處 進行 路面 回填   後 續 由 水利 處修 復 溝體   水利 處下 工科 科長 邱佑銘 表示   經現場 勘查 破損 側溝位 排水 下游 處   可能 因 水流 長 期 沖 刷 或 施作 年代 久遠   溝底 出現 局部 破損 情形   水利 處並 已督商 今日 進場 辦理 搶 修作業   因案址 位處 8 公尺 以下 單行 道   因此 施工期 間會 派義交 於 路口 指揮 暫時 禁止通行   當日 傍晚 收工 後則 於 側溝 開 挖邊 以槽 鋼護欄 圍設   並可回 復 道路 通行   為確 保側 溝結構 強度 混凝土 澆置 後 需養護 時間   溝底 牆 身及 頂版會 分次 施工   預計 2 天可將 側溝 搶修 完成   工務局 說明   北市 近期 出現 4 個 道路 坑洞 事件   歸納為 3 種 原因 造成   5 月 19 日 信義區 崇德 街因 建案 工地 開挖 地下 基礎   連續 壁 滲水 造成 地下水 湧入 基地   周邊 道路 沙土 被 帶 走 而 出現 坑洞   7 月 10 日 大同 區 南京 西路 坑洞 是 因該 處 地層 軟弱   長 期受 潮汐 影響 地下水位 升降   使 污水 管線 下方 土壤 承載力 不佳   導致 污水 管接 頭 鬆 脫 錯 位   土砂 沿管線 破 損處 流失 所致   後 衛工處 以 內視鏡 巡檢車 檢視 淡水河 沿岸 11 條 汙水 管均 正常   近 兩日 發生 兩 案件 均 與 水利 管渠 破損 有關   南港區 南港路 出現 坑洞   市府 初判 因事 發地 點位 於 南港 東區 門戶 計畫 範圍   許多 建案 均 施工 中   南港路 47 巷 道路 狹小   因此 水利 處無法 深埋 排水 箱涵 接側 溝的連 接管   研判 與 重車 來 往頻 繁有間 接關 係   使得 連 接管 間 出現 縫隙   地下水 帶 走 土沙 而 發生 地層下陷   至於 昨夜 民生 東路 二段 159 巷口 坑洞   則因 道路 側溝 溝體 老舊 破損   而 造成 近期 下雨 排水 淘涮   因應 幾次 道路 塌陷 坑洞 問題 事件   北市 府 已 擬定 防範 措施   新工處 將加強 定期 道路 巡查   如發現 路面 曾 出現 塌陷 修補 狀況   會 再 使用 透地雷達 確認 道路 無 孔洞   若有 土壤 流失   透過 預判 可 先行 強化 道路   衛工 處則 啟動 攝影機 巡視 各個 大型 管道   水利 處 將針 對 管路   箱涵 等 進行 巡視 機制   多管 齊下 避免 類似 坑洞 情形 再 發生  ']</t>
         </is>
       </c>
     </row>
@@ -718,21 +718,21 @@
         <v>10</v>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10_印尼_曼谷_東南亞_全球</t>
+          <t>10_大樓_巷弄_信義區_破洞</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['印尼', '曼谷', '東南亞', '全球', '海平面', '海域', '遊客', '海岸', '地區', '世界']</t>
+          <t>['大樓', '巷弄', '信義區', '破洞', '市府', '倒塌', '地下', '台北市', '牆壁', '壁']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['[ 周刊 王 CTWANT ]   泰國以 觀光業 聞名   不少 觀光客 都 會 造訪 首都 曼谷   Bangkok     然而 全球 暖化 問題 加劇   導致 海平面 不斷 上升   泰國 氣候變遷 辦 公室 評估   曼谷 本世紀 末 恐 被 海 水淹 沒   為 了 避免 曼谷 成為   海底 之 城     泰國 官方 為此 考慮 遷都   不過 目前 仍處 於 假 設階段     根據 新加坡   亞洲 新聞台   等 外媒 報導   泰國 首都 曼谷 過往 雨季 時   經常 飽受 洪水 問題 困擾   天災 一直 是 政府 頭痛 議題   隨著 曼谷 人口 已破千萬   加上 全球 暖化 趨勢   專家 示警   因為 海平面 不斷 上升   曼谷 恐在 21 世紀 結束 前 遭海 水淹 沒     根據 泰國 氣候 變化 與 環境局 副 局長 帕維奇   Pavich   Kesavawong   警告   曼谷 可能 無法 適應 當前 全球 暖化 趨勢     全球 暖化 已經 超過 攝氏 1.5 度   如果 我們 繼續 保持 當前 趨勢   曼谷 大概 會 被淹 沒     他 透露   關於 首都 曼谷 面臨 氣候 危機   政府 正在 研究 因應 措施   像是 參考 歐洲 著名 低 地國 荷蘭   藉由 興建 堤防 方式 來 防堵 海水倒灌   同時 當局 有將   遷都   納入 計畫 之中     這並 非泰國 首次 提出 遷都   前首相 帕拉 育 在位 時   曾 提出 同樣 建議   2019 年時   這位 前 總理   泰國 與 世界 相連大會     Connecting   Thailand   with   the   World   Conference   拋出 遷都 議題   藉此 因應 曼谷 海平面 上升 以及 交通 壅塞   環境 汙染 人口 過度 稠密 問題     針對 遷都 議題   帕維奇 提到   這 部分 牽涉 問題 太過 複 雜   因此 仍 初期   假設 階段   除了 泰國 打算 遷都   目前 東南亞 計劃 遷都 國家 就 緬甸   當地 軍 政府 於 2005 年 11 月 6 日將 首都 從 仰光 遷到 北方 320 公里 奈 比 多   Naypyidaw     此外   印尼 首都 雅加 達   Jakarta   因為 面臨 人口 過剩   環境 污染   於 交通 壅塞 地層下陷 等 危機   預計 今年 正式   遷都   至婆羅洲島 東 加里曼丹 省   East   Kalimantan     新 首都 名為   努山 塔拉     Nusantara     印尼 語中   群島   之意   不過 高達 350 億 美元 遷都 計畫 備受 爭議  ', '科技 大亨 馬 斯克   Elon   Musk   今天   5 19   抵達 印尼 峇里島   將與 印尼 總統 佐科威   Joko   Widodo   一起 參加 星鏈   Starlink   網路 服務 啟用   印尼 將是 東南亞 第三 個 使用 星鏈 服務 國家   政府 希望 星鏈 能夠 提高 各島嶼 網路 普及 度   這是 印尼 一個 月 迎接 第 3 名 科技 企業 執行長   此前 蘋果   微軟 執行長 都 已來訪     綜合 路透社 與 美聯社 報導   太空 科技 公司 SpaceX 執行長 馬 斯克 今天 搭乘 私人 飛機 抵達 印尼 峇里島 機場   印尼 首席 投資部長 盧胡特   Luhut   Binsar   Pandjaitan   機場 迎接   預計 兩人 將會 討論 一些 重要 合作   包含 星鏈 服務 啟動   馬 斯克 還會 簽署 一項 協助 印尼 加強 衛生 與 教育 單位 聯絡 互通 合約     盧胡特 表示   馬 斯克 今天 稍晚 將和 印尼 總統 佐科威 一起 峇里島 首府 登巴薩   Denpasar   社區 衛生 中心 一起 啟動 星鏈   盧胡特 說   衛生 機構 啟動 這項 服務   呼應 星鏈   提供 平價 高速 網路   宗旨   尤其 是 網路 收訊 不佳 或過 於 偏遠 地區     印尼 是 個 群島 國家   約 1.7 萬座 島嶼   橫跨 3 個 時區   人口 超過 2.7 億   盧胡特 說   印尼 偏鄉 需要 星鏈 來 拓展 高速 網路   尤其 是 要 用 來 解決 衛生   教育 海事 單位 問題     印尼 通訊 部長 布迪   Budi   Arie   Setiadi   上週 表示   星鏈 已經 獲得 印尼 營運許 可   布迪 強調   星鏈 低 軌衛星 可以 讓 網路 擴及 目前 印尼 通訊 商無法 到 達 地區     據報   位 於 印尼 婆羅洲   Borneo   新 首都 努山 塔拉   Nusantara   本月 將先 試用 星鏈   8 月 正式 上線   印尼 正準備 遷都 努山 塔拉   因為 受 海平面 上升 與 地層下陷 影響   預計 目前 首都 雅加 達 大部分 地區將 2050 年 被淹 沒     印尼 將是 東南亞 第三 個 使用 星鏈 服務 國家   馬 來 西亞 去年 已核 發許 可證 給營 運星鏈 SpaceX 公司   菲律賓 一家 公司 則是 2022 年 與 SpaceX 簽約 合作     馬 斯克訪 印尼 前   蘋果 公司 執行長 庫克   Tim   Cook   4 月 17 與 印尼 總統佐科 威會面   並 表示 會將 印尼 產能 納入 考慮   兩周 後   微軟 執行長 納 德拉   Satya   Nadella   同月 30 日訪 印尼   承諾 未來 4 年 印尼 投資 17 億 美元   強化 印尼 新雲端 運算 與 人工智慧 基礎 設施     馬 斯克 此次 訪 峇里島   將參加 第十 屆 世界 水論壇   World   Water   Forum     研討 全球 水資源 衛生 挑戰  ', '印尼 海域 珊瑚礁 面積 超過 5 萬 平方公里   占 全世界 18%   但過 去 飽 受 非法 炸魚 破壞   一項 復 育計畫 讓 非法 捕撈 漁民搖身 一變   成 了 保護 珊瑚礁 尖兵   另外 印尼 首都 雅加 達 地層下陷 嚴重   當局 開發 紅樹林 生態 觀光   讓 遊客 種樹救 環境   寓教 於 樂   印尼 首都 雅加 達 北部 海岸 一片 紅樹林 自然 保護區   遊客 划著 小艇 來 這裡 享受 遠離 塵囂 寧靜 自然   還能 環保 人士 引導 下親 手種 植紅樹 林樹苗   為 保護 首都 環境 盡 一份 心力   保護區 遊客 娜塔莉 亞 指出     紅樹林 是 很 獨特 生態 系統   一種 植物   有趣 是 紅樹林 可 吸收 危險 金屬   還 可以 改善 空氣 品質   這不 正是 我們 人類 所 需要     印尼 首都 雅加 達長 期受 極端 氣候 引發 洪水 暴風雨 衝擊   加上 超 抽 地下水   地層下陷 快速   平均 一年 15 公分   已經 面臨 遷都 危機   紅樹林 是 能夠 抵擋 潮汐 上升   保護 土地 天然屏障   印尼 當局 去   2022   年 啟動 了 一項 恢 復 60 萬公頃 紅樹林 計畫   但 紅樹林 必須 成長 5 到 10 年   才夠 強壯能 抵禦 海浪 潮汐   而 周邊 還有 很多 建商虎視 眈眈   想 把 紅樹林 開發 成沙 灘遊樂區   保育 計畫 困難 重重 卻 是 必須 堅持 到底   而 這片 98 公頃 保護區   只是 印尼 全國 沿岸 410 萬公頃 紅樹林 一小部分   過去 一年 就 70 萬公頃 被 砍伐   另外 印尼 望 加錫海峽 120 個 珊瑚礁 島組成 斯珀 蒙德 群島 海域   20 年前 因為 非法 捕魚 猖獗   海底 珊瑚礁 被 炸魚 毒魚 破壞 成 了 廢墟 般的 碎片   只 剩 2% 倖存   前偷 獵者 達林 表示     我們 需要 生存 下去   但 很 難 找到 像樣 工作   當時 唯一 知道 工作 是 盜獵   所以 我們 開始 炸 珊瑚礁     這片 海域 位 東南亞 從菲律 賓到 印尼   澳洲 之間 珊瑚 大 三角 區域   物種 豐富 多樣   是 海底 生態 搖籃   破壞 至此 非常 可惜   科學家 尤素夫 教授 過去 20 年 來 當地 巴迪島   努力 復 育 周邊 3 公頃 珊瑚礁   耐心 說 服漁民 保育   從 珊瑚 產卵 受精 繁殖 開始 做起   把 蜘蛛 型 框架 結構 放入 海底   上面 綁 著 珊瑚 碎片 讓 它們 生長   過去 炸魚 毒魚 盜 獵者   變成 生態 守護者   長 期紀錄 並且 細 心照 顧   已經 慢慢 看到 荒蕪 海底 回春   熱帶 魚群 穿梭 新生 珊瑚礁 之間   環境 科學家 尤素夫 提及     印尼   菲律賓 與 印度 太平洋   這片 珊瑚 大 三角 必須 得到 保護   才能 為 後 代子 孫 保留 這片 海中 世界 遺產   一個 小小的 努力 都 可能 影響 世界     印尼 海域 珊瑚礁 面積 5 萬 875 平方公里   占 世界 珊瑚礁 總面積 18%   珊瑚 大 三角 區域 佔 比 更 高達 65%   尤素夫 教授 了 成功 經驗   現在 把 保育 觸角 擴展 到 鄰近 兩個 島嶼   將近 5 公頃 海域   一步 一步 把 失去 珊瑚礁 補 救回 來   但 這還 是 一條 漫漫 長 路  ']</t>
+          <t>['台北市 中山 區 大直 街巷 弄 今晚 多棟 大樓 傾斜   警方 初步 了解   大樓 附近 建案 施工 開挖 地下 連續 壁 最後一層 工程 時   疑因 土質 問題 導致 地基 不穩   造成 民宅 傾斜     台北市 警消 晚間 8 時 34 分獲報   大直 街巷 弄 民宅 傾斜   出現 磁磚   牆壁 龜裂   警消 派員 到場   發現 建案 工地 旁 5 至 6 棟大樓 受 影響   立即 拉 警戒 線   並 疏散 25 戶   無人 受傷   目前 住戶 疏散 到 實踐 大學                           警方 初步 了解   新建 工地 工程 人員開 挖 地下 連續 壁 最後一層 時   疑因 土質 問題 導致 地基 不 穩定   造成 旁邊 民宅 傾斜且 地基 變形   出現 可能 倒塌 狀況   消防 車已 持續 針對 建案 基地 灌水   協助 穩定 地質     民進 黨 台北市 議員陳怡君 第一 時間 赴 事故 現場   勘災後發布 新聞 資料 表示   附近 民眾 提及 晚間 曾 聽 見   蹦   聲響   工地 先緊 急 疏散 工人   才 通知 住戶     說   附近 民眾 提到 此建案 動工 後   住家 就 龜裂 狀況   已 多次 向 建商 反映   但 都 無 處理   市府 主管 機關 無作 為   才 釀成 此 狀況   要求 市府 清查 受災戶 狀況   並 立刻 協助 安置     台北市 信義區 崇德 街 60 巷 5 月份 才 因建案 工地 連續 壁 滲水   導致 道路 地層下陷   危及 旁邊 民宅  ', '北市 信義區 驚見 天坑   市政府 表示   坍塌 原因 指向 旁邊 大樓 建案   因為 地下 連續 壁 破洞   都 發局 初步 調查 後   對 承造 人 監造 人 各 開出 9 萬元罰 單   等 釐 清責任 歸屬   再進 一步 開罰   至於 附近 住戶   目前 共 10 人 接受 安置   暫住 信義區 旅館   相關 費用 將由建 商來 負責   巷弄 路面 塌陷 好大 一塊   深度 達到 3 公尺   一旁 民宅 門口 遭殃   鐵門 幾乎 懸空   這樣 情況 就 發生 台北市 信義區   短時間   房子 是 不能 住 了   住戶們 該何 去 何 從   台北市 信義區 長 陳 冠伶 指出     昨天 疏散 撤離   範圍 是 從 12 號到 24 號   調查 結果 發現 需要 安置 住戶 一共 5 戶     市府 緊急 介入 安置   一共 撤離 7 戶   需要 安置 5 戶   一共 10 人   暫時 住 信義區 旅館   依照 規定   每人每天 可以 請領 補助 金 1600 元   可以 請領 7 天   但 看 這情況   住戶們 一週 是 回 不了 家 了   超出 費用 將由建商 全額 買單   另外   台北市 都 發局 局長 王玉芬 表示   第一 時間 已經 勒令停工   現在 進行 是 搶災 部分   同時會 對 承造 人 跟 監造 人   處 各 9 萬元罰 鍰   根據 初判 是 建商要 負責   因為 是 一旁 建案 施工   地下 連續 壁 破洞 釀災   原本 要 蓋 大樓   地下 4 層   地上 17 層   負責 營造 華熊 營造 公司   興建過 包括 台北 101   世貿 中心 陶朱 隱園   都 是 赫赫有名 建築   如今 卻 發生 工安 意外   讓 工程 暫時 喊 卡   首要 之務得 設法 解決 安全 問題   還給 當地 居民 一個 安全 家  ']</t>
         </is>
       </c>
     </row>
@@ -741,458 +741,21 @@
         <v>11</v>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>11_坍塌_坍方_崩塌_塌陷</t>
+          <t>11_台北市_道路_塌陷_地層下陷</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['坍塌', '坍方', '崩塌', '塌陷', '路旁', '意外', '慶城街', '路邊', '災情', '路面']</t>
+          <t>['台北市', '道路', '塌陷', '地層下陷', '路面', '市府', '台北', '巷', '下', '地下水位']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['台北市 松山區 慶城街   興安街 一處 新建 工地   昨   23   天晚間 發生 地基 塌陷 意外   造成 停 路旁 四台 車 受到 波及   人行道 路面 呈現 V 字型 凹陷   面積 約 4 公尺 長   30 公尺 寬   深度 約 1.5 公尺   所幸 週邊 建築物 沒有 危險   相關 單位 連夜 現場 進行 回填 作業   不過 工地 遭罰 18 萬 勒令停工   事發 原因 尚待 調查   慶城街 新建 工地 地基 下陷   路面 坍塌   人行道   工程 圍籬 都 明顯 下陷   路旁 停車格 消失 一大半   當時 路邊 4 輛汽車 遭殃 歪斜   建商 連夜 回填 灌漿   避免 塌陷 擴大   據 了解   該 處興 建工 地原 是 要 蓋 豪宅 大樓   原先 工地 上 地下 三層 地下室 建物   疑似 拆除 建物 後   地下室 進行 導溝 作業 時候   內部導 溝支 撐力 不足 才 發生 坍塌 意外   所幸 工地 尚未 進行 大規模 開 挖   沒 再 釀 更 大 事故   此次 路面 坍塌 面積長 約 4 公尺   寬約 30 公尺   深度 1.5 公尺   目前 週邊 建築物 沒有 相關 安危   而 北市 建管處 勘查 後   昨天 深夜 確定 裁罰 18 萬   並 勒令 回填 穩定 後 停工   待 確保 工地 安全   業者   建商 提出 復工 審查   才 會 進行後續 作業   至於 事發 原因 仍待 調查  ', '台中市 沙鹿 區一處 工地 旁 路面 坍方   今天 造成 一輛 預拌 混凝土車 側翻   壓傷 一名 工人   圖 ／ 台中市 消防局 提供 台中市 沙鹿 區一處 工地 旁 路面 今天 塌陷   一輛 預拌 混凝土車 側翻   壓傷 一名 工人   被 送醫 急救   台中市 勞檢處 已 派 人 到場 調查   並 勒令停工   因 工地 沒 擋 土   地面 承載力 不足 等 缺失       台中市 消防局 今天 早上 9 點接 獲 報案   沙鹿 區錦華街 一處 工地 旁發生 緊急 創傷 救護   出動 沙鹿   龍井   梧棲   西屯 分隊 第四 大隊   各式 消防 車輛 10 輛   消防人 員 25 名   由大隊 長 蔡孟栩帶 隊 指揮 搶 救                             現場 是 路面 坍方   造成 一輛 預拌 混凝土車 側翻 壓傷 一名 工人   工地 營建廠 商已 協助 聯 繫 吊 車 到 場   地層下陷 造成 預拌 混 泥土 車車輛 翻覆   沙鹿 消防 分隊 到 場後先 以 消防 車絞盤   梧棲分隊 使用 車 吊臂 共同 固定 預拌 混 泥土 車   確保 傷者 安全 無虞   因 該車 重量 達 35 噸 以上   需 等待 業者 配合 大型 吊車 到 場方能 吊掛   先由救護 人員 接觸 患者 進行 緊 急救 護處 置       早上 9 點 34 分   業者 調派 吊車 至 現場 進行 車輛 吊掛   消防局 搶 救人 員協助 以油 壓破壞 器材   協助 傷者 脫困   10 點 4 分傷者 順利 脫困   送 梧棲童 綜合 醫院       傷者 到 醫院 時 意識 清楚   雙 下肢 背部 擦 挫傷   右 大腿 燙傷   應是 鋼版 高溫 造成   目前 仍 醫院 檢查 中   台中市 勞檢處 表示   工地 地面 承載力 不足   造成 地面 塌陷   車翻 傷心 意外   已 要求 停工   將開罰 3 到 30 萬元 不 等 罰 鍰   台中市 沙鹿 區一處 工地 旁 路面 坍方   今天 造成 一輛 預拌 混凝土車 側翻   壓傷 一名 工人   圖 ／ 台中市 消防局 提供 台中市 沙鹿 區一處 工地 旁 路面 坍方   今天 造成 一輛 預拌 混凝土車 側翻   壓傷 一名 工人   圖 ／ 台中市 消防局 提供 台中市 沙鹿 區一處 工地 旁 路面 坍方   今天 造成 一輛 預拌 混凝土車 側翻   壓傷 一名 工人   圖 ／ 台中市 消防局 提供 台中市 沙鹿 區一處 工地 旁 路面 坍方   今天 造成 一輛 預拌 混凝土車 側翻   壓傷 一名 工人   圖 ／ 台中市 消防局 提供 台中市 沙鹿 區一處 工地 旁 路面 坍方   今天 造成 一輛 預拌 混凝土車 側翻   壓傷 一名 工人   圖 ／ 台中市 消防局 提供', '台北市 松山區 慶城街 一處 新建 工地 旁   昨天 晚間 發生 路面 塌陷 意外   經過 將近 20 小時 搶 救   工地 崩塌 範圍 已 完成 回填   今天下午 開始 灌漿 工地 外圍 塌陷 路面   初步 研判   疑似 是 新建 工程 拆除 建 地 既有 地下 建築 結構 時   挖到 不連續 弱面   才 導致 導溝 崩塌   台北市 松山區 慶城街 新建 工地 23 日 晚間 發 生地 層 坍陷 意外   經過 約 18 小時 緊急 搶 救   工地 外圍 崩塌 範圍終 於 展開 回填 作業   從制 高點 俯瞰 更 清楚   混 泥土 車來 回 進出 灌漿 沒 停過   因為 這一崩   不僅 人行道 嚴重 下陷   路邊 車格 消失 一大半   當時 還有 4 輛汽車 差點 被 吞噬   附近 住戶 直言     好 意外   真的 很 意外   文華飯 店 當初 蓋 時候 這麼 近   沒 發生過 問題     精華 地段 豪宅 新建 案出 現大 坍塌   讓 附近 居民 全都 嚇壞   畢竟 這長 約 4 公尺   寬約 30 公尺   深度 達到 1.5 公尺 坍陷 範圍 實在 不小   而且 建案 甚至 才 正 準備 施作 連續 壁   基礎 地基 都 還沒大規 模開 挖   竟然 就 前置 導溝 作業發 生意 外   初步 研判   坍塌 原因 跟 建地 原先 存在 地下室 結構 脫 不了 關 係   原來 這回 要 建立 深導溝   越過 既有 結構 時   卻 不慎 碰到 既存 不 連續面   才 會 釀禍   台北市 土木 技師 公會 理事 長 莊均緯 指出     破除 既有 連續 壁 跟 外牆   那個 地方 有個 不 連續面   原有 地下室 這個 部分   外牆 它 推擠 進來 變位   就 把 原來 深導溝 側壁壓 變形 之 後   就 產生 這樣 崩塌 現象     台北 市長 蔣萬安週 六 上午 二度 到 現場 勘查   向 居民 保證   周邊 住宅 暫無 安全 疑慮     西側   南側   北側 目前 比 對 監測 數值 是 正常   而且 都 沒 地面 塌陷 以及 鄰房 傾斜 狀況     建管處 則緊 急 開罰 18 萬   並 勒令停工   後 續 就 待 道路 回填   並由 透地雷達 確認 周邊 無 安全 疑慮   就 可 恢 復 通車   還給 居民 安全 環境  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>12</v>
-      </c>
-      <c r="B15" t="n">
-        <v>5</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>12_水利局_水權_水利_淨水場</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>['水利局', '水權', '水利', '淨水場', '水資源', '地下水', '供水', '水電比', '用水', '水量']</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>['▲ 南市 水井 納管 申報 複 查作業 同時 啟動   針對 轄 內納管 水井 辦理 複 查 暨 貼標 籤 作業   合理 使用 水資源 防治 地層下陷     記者 李 嘉祥 攝     為 保育 地下水 資源 加強 地下水 管理   避免 地下水 過度 使用 造成 地層下陷   影響 市民 人身 財產 安全   臺 南 市政府 水利局 積極 推動 水井 管理 政策   自 112 年 起 辦理 水井 納管 作業   受理 申報 於 99 年 8 月 4 日前 鑿 設且 未 辦理 水權 登記 既有 水井   納管 後 可 避免 遭檢舉 而 封井   且 取得 合法 水權 機會   並自 今年 4 月 起將 辦理 地下水 一級 管制 區 水井 申報 納管 複 查作業   針對 轄 內納管 水井 辦理 複 查 暨 貼標 籤 作業   透過 現場 訪談   測量 等 方式   建立 水井 基本 資料   以利 後 續 地下水 管理     市長 黃 偉哲 表示   水井 納管 除 可 保育 地下水 資源   對 於 使用 水井 民眾 而言   接受 輔導 合法 取得 水權 後 可 獲得 合法 用水 保障   另為 減輕 農民 負擔   經 水井 納管 農業 用 水井 免收 各項 水權 登記 規費   倘未 登記 水井 逾期 未申 報且 經查 獲者   將 要求 限期 自行 封填 水井 並 可能 面臨 罰 鍰 處分   籲請 鄉親 踴躍申報   讓 珍貴 地下水 資源 合理 使用   並同 時維護 自身 用水 權益     水利局 長 邱忠川 說   根據 水利局 統計   截至 去年 12 月底 已 受理 超過 2 萬 5000 件 既有 未登記 水井 納管 申報 案件   但 仍 部分 民眾 未及 申報   為 保障 水井 用戶 權益 落實 地下水 保育   市府 特別 再 開放 受理 申報 納管   申報 時間 於 4 月 1 日起 至 8 月 2 日 截止   時間 有限   籲請 尚未 申請 地下水 井納管 鄉 親 儘 速 於 申 報 截止 日前 申請   以維護 自身 權益     邱忠川 指出   4 月 起 將展 開 地下水 井現 地 複 查   將 以北 門區   學甲區   鹽水區   安定 區 地下水 一級 管制 區分區 方式 依序 進行   並由 專人 電話 通知 約定 複 查時間   若 申請 人無法 到場   請備 妥申 請 人 代理人 身分 證明 文件 並至 現場 填 妥委 託 書   現場 除 確認 基本 資 料及 調查 水井 狀況   坐標   地段 號   井深   井徑   出水管 徑   抽水機 位置   型式 及馬力   電表電號 用水 標 與 範圍     農用 水井 另 進行 水電比 檢測   透過 用 電量 測定 抽 水量   為節 省民眾 時間   與 請 所有人 於 預定 複 查 日期 前先 清除 水井 周圍 草叢   以 加速 複 查作業 進行     邱忠川 呼籲 水井 所有人 可 就近 至 各區 公所 或 至 臺 南 市政府 民治 行政 中心 服務台   永華 行政 中心 服務台 或 安平 水資源 回收 中心 收件 窗口 填寫 申報 書 後 投至 專用 信箱   或 透過   臺 南 市政府 水利局   網站   水井 納管 申報   Web 平台 申報   可手 機下載   水井 納管 申報 查詢   APP 申報   市府 設置 水井 納管 專線 06   6321212   主動 輔導解 決民眾 申報 問題  ', '水利 署 南投 草屯 打造 鳥 嘴潭 人工湖   環團 質疑 傾倒 工程 廢土 至 烏溪 河床   破壞 環境 生態   向 環境部 提起 行政 訴訟   5 月 1 日將 開庭   要求 移除 違法 土石   水利 署中 水分 署 表示   依環評 規定 辦理   並持續 追 蹤 態 環 境   土方 培厚 為 河道 治理   經監測 保護堤 腳   可 提升 河防 安全       水利 署 打造 鳥 嘴潭 人工湖   供水 給彰 投   改善 沿海 地下水 超 抽   地層下陷 問題   引取 烏 溪水 源蓄 存在 6 座 湖區   總 蓄水量 1450 萬噸   每日 可 供水 25 萬噸   約 百萬人 用水   目前 已近 完工   已日供 草屯 1 萬噸   彰化 6 萬噸 民生 用水                             鳥 嘴潭 人工湖 工程 啟動 後   多次遭 台灣 石虎 保育 協會   台灣 生態 學會   台灣 淺山學社   台灣 水資源 保育 聯盟 等 環團 指控   破壞 生態 環境   造成 保育 類 石虎   巴氏 銀 鮈 棲地 消失   質疑 違反 環評 程序   將廢土 傾倒 於 烏溪 河床       台灣 石虎 協會 發文   與 其他 環團 從 2022 年 7 月 起   多次 舉辦 現勘   記者 會   行文 等   反映 該 工程 破壞 生態   至今 爭議 未解   去年 7 月 已委 託 律師   向 環境部 提起 行政 訴訟   5 月 1 日 首度 開庭       協會 強調   環境 部應 開罰 中 水分 署   移除 違法 堆置 烏溪 土石方   若 未 限期 移除   應 要求 停止 鳥 嘴潭 工程       水利 署中 水分 署 表示   施工 前 生態   環境 調查   施工期 間 生態 監測   檢核 機制   保育 措施 或 土石 處理   都 依環評 規定 辦理  ', '水利 署 南投 草屯 打造 鳥 嘴潭 人工湖   遭環團 質疑 傾倒 工程 廢土 至 烏溪 河床   破壞 環境 生態   向 環境部 提起 行政 訴訟   5 月 1 日將 開庭   近期 重申 要求 移除 違法 土石   水利 署中 水分 署 表示   均依 環境 評估 相關 規定 辦理   並持續 追 蹤 態 環 境   土方 培厚則 為 河道 治理   經監 測確 保護堤 腳及 提升 河防 安全 功效       為 改善 沿海 地區 地下水 超 抽 造成 地層下陷   水利 署 打造 草屯 鳥 嘴潭 人工湖   引取 烏 溪水 源蓄存 於 6 座 湖區   總 蓄水量 約 1450 萬噸   可供 應 每日 25 萬噸   約 百萬人 用水   目前 已近 完工   並 先行 供水 草屯 每日 1 萬噸   彰化 6 萬噸 民生 用水                               但 鳥 嘴潭 人工湖 工程 啟動 後   多次遭 台灣 石虎 保育 協會   台灣 生態 學會   台灣 淺山學社   台灣 水資源 保育 聯盟 等 環團 指控   開發 破壞 生態 環境   造成 保育 類動物 石虎   巴氏 銀 鮈 棲地 消失   更質疑 施工 單位 違反 環評 程序 將廢土 傾倒 於 烏溪 河床       台灣 石虎 保育 協會 近期 發文 表示   該會 與 其他 環團 自 2022 年 7 月 起   透過 現勘   開記者 會   公開會議   行文 等 持續 向 公部門 反應 鳥 嘴潭 工程 破壞 生態   但 至今 爭議 未解   去年 7 月委 託 律師 向 環境部 提起 行政 訴訟   並將 於 5 月 1   日 首度 開庭       台灣 石虎 保育 協會 強調   環境部 應善 盡到 監督 環評 之責   對 開發 單位 水利 署 中區 水資源 分署 開罰   並命 該 分署 移除 違法 堆置 於 烏溪 土石方   若 未 依 限期 移除   環境 部應 轉請 經濟 部命 停止 鳥 嘴潭 人工湖 工程   或 由 環境 部 逕 命 其 停止 開發行 為       對此   水利 署中 水分 署 表示   鳥 嘴潭 工程 不論 施工 前 生態   環境 調查   施工期 間 生態 監測   檢核 機制   強化 保育 措施 或 土石 處理   依環評 規定 辦理   後 續 監測 發現 仍 石虎 出 沒 活動   甚至 定居 個體   巴氏 銀 鮈 棲地 沒 明顯 影響       鳥 嘴潭 土方 則是 協助 第三 河川 分署 以培厚 工法 取代 傳統 使用 混凝土 塊 進行 河道 治理   與 既有 混凝土 坡 面上 覆土 生態 工法 理念 相近   專業 技師 分析   經比 對 去年 培厚前   後 颱 洪空 拍 地形 變化   顯示 確有 保護堤 腳及 提升 河防 安全 功效   環團 指控 鳥 嘴潭 人工湖 工程 違反 環評 程序 將廢土 傾倒 烏溪 河床   為 此 提 行政 訴訟   5 月 1 日將 開庭   圖 ／ 聯合 報系 資料 照片 環團 多次 指控 鳥 嘴潭 人工湖 開發 破壞 生態 環境   並質疑 違反環 評將 廢土 傾倒 於 烏溪   為 此 提 行政 訴訟   5 月 1 日將 開庭   圖 ／ 聯合 報系 資料 照片']</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>13</v>
-      </c>
-      <c r="B16" t="n">
-        <v>5</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>13_消防局_台北市_信義區_街</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>['消防局', '台北市', '信義區', '街', '巷道', '疏散', '坐鎮', '鄰近', '大樓', '巷']</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>['【 17   27 ｜ 更新 天坑 初步 原因 】 信義區 崇德 街今   13   天 下午 3 點 13 分   傳出 一處 新建 案 工地 旁 道路   地層下陷     消防局 獲報 緊急 疏散 鄰近 住戶   無人 受傷   根據 消防局 獲報 消息   信義區 崇德 街 60 巷 22 號前 新建 工地 旁   出現 道路 地層下陷   馬 路上 出現 一個 長 15 公尺   寬 3 公尺   深度 約 4 公尺 天坑   摩托 車   腳踏車 都 掉入 坑洞   一旁 住戶 家門口 更是 危險   懸空     警消 人員 疏散 鄰近 住戶   所幸 無人 受傷   目前 劃設 警戒 線   建管處   新工處   道管 中心   瓦斯 公司   北水處 派員 趕 赴 現場 處理   信義區 區長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置   這個 天坑 幾乎 占據 整條 巷弄   北市 建管處 初步 了解   由 於 住 戶 旁 就是 工地 施工   疑似 因為 工地 連續 壁施作   且 出現 滲水 狀況   才 釀成 天坑 出現   稍早 水泥 車緊 急先 進行 灌漿 作業   主要 基本 填補 坑洞   受影響 住戶 透露   剛剛 一度 5 名住 戶 受困 屋子 裡   所幸 消防 員協助 救援   而 三戶 門口 前端 地基 被 掏空   住戶 非常 擔心 房屋 可能 會 倒塌   地基 到底 穩不穩固   住 裡面 到底 安 不 安全   今天 晚上 到底 要 住 哪裡 等 問題   不過 關於後續 賠償 等 都 還要 進 一步 釐 清  ', '台北市 信義區 一處 新建 大樓 工地 旁 巷道   蹋陷   緊急 灌漿 回填   住戶 驚慌 撤離         消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷 ( 長 15 公尺   寬 3 公尺   深度 2   3 公尺 )   幸無人 受傷                             警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   目前 評估 約 10 餘位 住戶 需要 安置   台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影警 消緊 急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 消防局 於 15 時 13 分獲報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   警消 緊急 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   住戶 心有 餘悸 驚慌 撤離   到 一旁 安全 區域   記者 林俊良 ／ 攝影 今天下午 台北市 信義區 一處 新建 大樓 工地 旁 巷道   突然 塌陷   警方 疏導 住戶 驚慌 撤離   目前 評估 約 10 餘位 住戶 需要 安置   記者 林俊良 ／ 攝影 台北市 信義區 一處 新建 大樓 工地 旁 巷道 突然 塌陷   施工 單位 緊急 灌漿 回填   防止 塌陷 區域 擴大     記者 林俊良 ／ 攝影', '台北市 信義區 崇德 街 下午 出現 地層下陷   北市 府 表示   消防局 於 15 時 13 分通報   信義區 崇德 街 60 巷 22 號前 新建 工地 旁 道路 地層下陷   長 15 公尺   寬 3 公尺   深度 2 至 3 公尺   無人 受傷       市府 表示   目前 處置 作為 已 疏散 鄰近 住戶   並劃 設 警戒 線   消防局 已先 成立 現場 指揮 站   建管處   新工處   道管 中心   瓦斯 公司   北水處 已 派員 趕 赴 現場 處理   信義區 區長 已 趕 抵 現場 坐鎮 指揮   目前 評估 約 10 餘位 住戶 需要 安置                             北市 信義區 出 現長 15 公尺   深 3 公尺   天坑     圖 ／ 北市 府 提供 北市 信義區 出 現長 15 公尺   深 3 公尺   天坑     圖 ／ 北市 府 提供']</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>14</v>
-      </c>
-      <c r="B17" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>14_村落_村民_縣府_公所</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>['村落', '村民', '縣府', '公所', '鄉', '城鎮', '鄉長', '縣', '建築', '倒塌']</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>['插 稻田 裡的 廟宇   嘉義 縣六腳 鄉 出現 了 只 露出 屋簷   底下 全 被淹 沒 田中 宮廟   事實 上 這座 宮廟 興建 清道光 年間   已有 將近 兩 百年 歷史   由 於 民國 48 年 一場 水患   廟方將 神像 遷 走 後   舊廟 就此 荒廢 下沉   如今 才 會 變成 隱身 稻田 裡的 獨特 打卡 景點   這間   插 稻田 中 廟宇   出現 嘉義 縣六腳 鄉   一片 綠 油油的 稻田 放眼望去   田中 間 竟 出現 只 剩下 屋簷 露出 廟   仔細 一看   屋頂 上 雕刻 嚴重 斑駁   奇特 景象 吸引 民眾 朝 聖 搶 拍   大批 網友 直呼     真是 神跡       從田裡 冒 出廟 頂   是 獨特 裝置 藝術     更 有人 笑稱     這是 真正 土地公 廟     而前 來 朝 聖 遊客 蕭 說     很 奇特   田中 廟     其實   這間 廟 已有 將近 兩 百年 歷史   它 先前 是 大庄 五福 宮舊 廟   興建 於 清代 道光 年間   不過 民國 48 年 碰上 水災 受損   村民 另 建新 廟   而 這間 舊廟 隨著 地層下陷 漸漸 下沉   五福 宮前 總幹事 姚水順 說     大家 都 會 好奇   裡面 東西有 沒有 搬出 來   神明 沒 沉下去   都 會問 這些 問題   其實 神明 都 請 出來       百年 舊廟 搬 遷 未 拆   隱身 稻田 裡 意外 成為 當地 打卡 熱點  ', '印度 北部 喜馬 拉雅山 區   一個 經常 有朝 聖者 觀光 客造訪 城鎮   這兩天 突然 發生 地層下陷   超過 600 棟 房屋 出現 裂縫   寺廟 紛紛 倒塌   當地 政府 緊急 撤離 將近 200 位民眾   安置 安全 避難 地點   印度 北部 山城 地層下陷   房屋   樓梯 道路 都 嚴重 龜裂   建築物 牆壁 還不斷 滲出 泥水   隨時 可能 發生 崩塌   景象 怵 目驚心   當地 居民 表示     5 戶 人家 已經 搬走   其他 好 幾戶 計劃 遷移   另 打算     官員 表示   最近 幾個 星期 當地 通報 超過 600 棟 房屋 出現 裂縫   因此 已經將 至少 193 名 居民 安置 到 安全 地點     找到 解決 方法 之前   我們 把 居民 安置 安全 無虞 飯店 賓館 跟 民宿     喬西馬斯   Joshimath   海拔 將近 2000 公尺   人口 約 2 萬 5000 人   是 朝 聖客 前往 山上 印度教 跟錫克 教寺 廟 門戶   常有 想要 征服 喜馬 拉雅山 登山 客造訪   喬西馬斯 所在 的傑 莫利 縣   Chamoli     2021 年 2 月 曾經 爆發 洪水   造成 200 多人 喪生   還 沖 走 兩座 水力 發電站   災情 相當 慘重   科學家 目前 還在 研究 氣候變遷 對 喜馬 拉雅山 影響   但 如果 不 做好 水土保持   這座   沉 沒 城鎮   可能 很快 就 會 走向 毀滅  ', '彰化縣 大城 鄉現 有納 骨塔 接近 飽   鄉 公所 規畫 第六 公墓 新建 第二 納 骨塔   頂庄 村民 群起 反對   已有 140 人連署 陳 情   村民 抱怨 縣府 裁撤 頂庄國 小   鄉 公所 村 內蓋 第二座 納 骨塔     吃 虧 都 是 我們     讓 頂 庄村 發展 雪上加霜   要求 重新 研議 興建 地點   鄉長 陳 玉照 說   納 骨塔 近 飽   將持續 溝通       大城 鄉有 8 座 公墓   頂庄村 山腳 村設 有納 骨塔   山腳村 已 飽   頂庄村 只 剩 不到 700 個 空位   鄉 公所 認為   興 建新 塔有 迫切性   日前 向 頂庄 村民 說明 新建 計畫   村民 痛批   一村 二塔   違反公 平原 則   當場 反對                             許姓 村民 表示   縣府 認為 頂 庄村 出生率 低   已 是 大城 鄉 人口 倒數 第 2   前年 裁撤 頂庄國 小   可見 頂 庄村 沒 新建 納 骨塔 需求   周邊 地層下陷 易 淹水   無論 地理 風水   都 不 適合 安放 往生 親人   新建 第二 納 骨塔 離 村落 僅 200 公尺   違反 縣府 規定 500 公尺 審查 原則   嚴 重影 響 村民 身心健康       鄉長 陳 玉照 指出   頂庄 第一 納 骨塔 建在 高灘 地   第二 納 骨塔 一樣   不開 挖 地下室   還 建造 7 層台 階 升高 塔座   沒 淹水 疑慮   第二 納 骨塔 距離 村落 人口稠密 區約 500 公尺   像 他家 距離 墓地 很近   不會 問題       頂庄 村長 許仁寶說   如非建 不可   應 提出 有力 說明   並訂定 回饋 辦法  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>15</v>
-      </c>
-      <c r="B18" t="n">
-        <v>5</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>15_地震_花蓮縣_花蓮市_地基</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>['地震', '花蓮縣', '花蓮市', '地基', '地表', '大樓', '大地', '花蓮', '建築', '地球']</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>['台灣 位處 菲律 賓海板 塊 歐亞板 塊 交界 處   因此 時常 因為 板塊 運動 而 引發 地震   台東 昨   31   日 下午 四點 多 就 發生 規模 5.0 地震   中央 氣象 局長 鄭明典 指出   台灣 真的 動     氣象局 全台 建置 超過 160 個   全球 導航衛 星系 統   測站   藉由 監測 大地 變形   地球 科學家 可以 監視 斷層   火山 活動   以及 地層下陷 或 滑動 一舉 一動   而 從 地表 來 看   除了 地震 期間   地震 前 後 台灣 斷層 都   偷偷   地亂動   氣象局 表示     既然 手機 上 GPS 可以 監測 我們 每日 移動 路線 距離   那麼   同樣 概念 技術   是不是 能 監測 台灣 地表   看看 它 每天 移動 了 多少   當然 可以     氣象局 已 全 台灣 建置 超過 160 個   全球 導航衛 星系 統   測站   結合 各 單位 建置 成果   台灣 已有 超過 450 個 連續 觀測 站   進行 大地 測量   建立 台灣 大地 變形 資料 庫   氣象局 指出   從 地表 來 看   大型 地震 會 造成 明顯 地表 位移   像是 車籠埔斷 層 錯動   為 台灣 地表 帶來 一道 劇烈   長 達 105 公里 傷痕   斷層 上盤 水平 位移 為 1 至 9 公尺 不 等   而 大甲溪 更 出現 地殼 抬高   落差 5 公尺 瀑布 景觀   氣象局 表示   除了 地震 期間   短短 數 十秒 出現   同震 滑移   之外   地震 前   間震期     地震 後   震後期     斷層 都   偷偷   地亂動   氣象局 說明   地殼 不 只 地震 時會動   平時 地殼   累積 能量   過程 中   就 會 地表 出現 非常 微量 變形   或者 是 小小的   不起眼 地震   地球 科學家 就是 透過 這個 原理   長 期連續 監測 台灣 地表 一舉 一動   希望 可以 找出 大 地震 發 生前 徵兆   氣象局 表示   雖然 目前 尚未 發 展出 成熟 地震 預測 技術   藉由 地震 前   中   後 所 蒐集 地表 微小 變形 資料   可以 讓 地球 科學家 更 了解 地殼 運動 樣態   或是 分析 出 地震 發生 週期   計算 地震 災害 潛勢   評估 台灣 各地 斷層 活動 地震 機制  ', '花蓮 近海 今天上午 發生 規模 7.2 強震   花蓮市 區有 大樓 嚴重 傾斜   學者 解釋   地震 造成 房屋 傾斜 原因   包含 地震 本身 震動 方向   建築物 結構 是否 與 土壤 液化 有關       根據 中央 氣象署 資訊   今天上午 7 時 58 分發生 芮氏 規模 7.2 地震   地震 深度 15.5 公里   震央 位 於 花蓮縣 政府 南南 東方 25.0 公里   位 於 台灣 東部 海域     最大 震度 花蓮縣 6 強   各地 陸續 傳出 災情   如 花蓮市 區 2 大樓 嚴重 傾斜 等                             中央研究院 地球 科學 研究所 副 研究 員黃信 樺 告訴 中央社 記者   地震 發生 當下   可能 有些 民眾會 發現 某些 牆面 東西 容易 倒   某些 不會   就 代表 該起 地震 震動 方向   然而 這 部分 與 地震 震源   斷層 位置   傳遞 能量 大小 等 相關   並 不好 預測       另外   黃 信樺 指出   建築 結構 工程 問題   比方 許多大樓 1 樓 可能 規畫 為 騎樓   甚至 有些 做成 挑 高大 廳   結構 上僅 靠 少數 樑 柱 支撐   因此 可能 會 大 地震 發生 時 造成 不 穩的況       黃 信樺 說   第 3 點 就是 可能 土壤 液化 問題   有些 建築物 若 座落在 比 較 鬆 軟 沉 積 層 上   如河邊 長 久 沖 積下   部分 地底 縫隙 會 被 沙石 填滿   但 地震 後 卻 又 鬆 動   或是 局部 液化 情況   造成 地層下陷       黃 信樺 提到   雖然 台北市 可能 很多 老式 騎樓   但 一來 是 震央 位置 離 台北 較遠   二來 是 老式 騎樓 通常 較 矮   不 容易 與 地震 發生 共振   反之   若 是 高樓 層   又 騎 樓式 設計 房屋   大 地震 來 臨時 就 會 相 對 危險       黃 信樺 表示   其實現 已 經有 許多 耐震 建築 技術   或許 政府 部門 未來 考量 建築 補強 上 可以 採用   增加 老建築 安全性       ▶ ▶ ▶ 花蓮 大 地震 延伸 閱讀     ▪ 一夜 83 震   氣象署 曝餘震 暴增 原因     只是 剛開始     ▪ 花蓮 強震 整理 包 ／ 釀 18 死   重大 災情   災後理 賠   專家 示警 一次 看   ▪ 花蓮 餘震 突變 多 又 變大   專家 坦言   有點 不 尋常   ▪ 大 地震 要來 了   地科 教授 分析 餘震 分布   花蓮 特性', '嘉義 縣 新港 鄉 5 日 下午 5 時 30 分發生 芮氏 規模 5.5 極淺層 地震   深度 8.5 公里   今   6   日 下午 高雄 又 發生 芮氏 規模 4.3 地震   地震 頻傳 讓 民眾 人心惶惶   而據 統計   我國 住宅 地震 基本 保險 截至 7 月底 止   投保 率約 37.53%   相當 於 約 580 萬住 戶 沒 地震 保險   住宅 地震 保險 基金 呼籲民眾 可 投保 住宅 地震 基本 保險   以 減輕 地震 災情 造成 之 財物 損失       台灣 位處環 太平洋 地震 帶   地震 發生 頻繁   為 使民眾 迅速 獲得 基本 地震 險 保障   住宅 地震 保險 基金 呼籲民眾 可 投保 住宅 地震 基本 保險   以 減輕 地震 災情 造成 之 財物 損失                             住宅 地震 保險 基金 表示   我國 住宅 地震 基本 保險 截至 2023 年 7 月底 止   以 全國戶數 922 萬戶計   投保 率約 37.53%   顯示 民眾 對 於 自身 住宅 財產 已 頗 具風險 意識   惟 仍 許多 屋主 尚未 投保   建議 應 即 早 投保   以 獲得 基本保障       住宅 地震 保險 基金 提醒   住宅 地震 基本 保險 保障 範圍 主要 包括 因 地震 震動   地震 引起 之火災   爆炸   山崩   地層下陷   滑動   開裂   決口   海嘯   海潮 高漲   洪水 等 危險 事故   造成 已 投保 住宅 地震 基本 保險 房屋 倒塌 或 不堪 居住 之   全損   損失 時   即可 取得 保險 金額理 賠及 臨時 住宿 費用       目前 保險 金額 最高 為 150 萬元   臨時 住宿 費用 為 20 萬元   保險 期間 為 一年期   每年 保費 1   350 元   相當 於 每日 只 需 3.7 元   即可 獲得 基本 地震 險 保障   🏠 udn 房地產   推薦 新聞     ▪   台南 1 預售 建案 疑營造 熱銷 假象 炒作   遭消 保官 嚴查     ▪   老 又 臭 沒人要   他 目睹 台北 老 公寓   看房 要 排隊     一堆 人 搶     ▪   天氣熱 但 電費 上 漲   高雄 人 推薦 1 降溫 神物   不用 開冷氣     ▪   換同坪數 新房   房屋 稅 3 千變 3 萬 4     他 哀號   貴到 快 哭 出來     ▪   借錢 買房   台積 輪班 工程 師   繳不出 頭期   全場 曝下場   穩死']</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>16</v>
-      </c>
-      <c r="B19" t="n">
-        <v>4</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>16_地下水_台中_溫水_水面</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>['地下水', '台中', '溫水', '水面', '台中市', '水', '池', '水壓', '抽水', '蘇澳']</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>['宜蘭縣 蘇澳鎮 民富 街   部分 路段 緊臨 蘇澳 海事 游泳池   居民 質疑   疑似 校方 長 期為 泳池 抽 地下水   導致當 地底 層 下陷   連 住家 地基 都 被 掏空   嚴 重影 響 居住 安全   校方 否認 超 抽 地下水   立委 陳 琬惠會 同 教育部   水利 署 官員   到 當地 與 居民 研商 解決 辦法   宜蘭 蘇澳鎮 民富 街 部分 與 蘇澳 海事 緊鄰 路段   長 年 發生 地層下陷 問題   住戶 房子 地基 被 掏空   地面   牆面 出現 裂縫   從 住家 滾一個 鐵罐 到 道路 對面   相當 順暢   可以 見 到 坡度 相當大   且 道路 表面 比旁邊 側溝 還要 矮   根本 沒有 排水 功能   居民 指出     游泳池 建好 以 後   大概 有用 了 4 年 多 就 塌 掉 了   影響 到 我們     當地 地層下陷 情況   從 2017 年 蘇澳 海事 游泳池 塌陷 後   就 開始 發生   多年 來無法 完全 改善   即使 2021 年 蘇澳 海事 當地 進行 壓力 灌漿   道路 仍持續 塌陷   居民 質疑   當年 是 蘇澳 海事 為 了 游泳池 超 抽 地下水   才 導致 地層下陷 情形   教育部 高級 中等教育 組 行政 資源 科長 黃 懷瑩 表示     我覺 得 地質 監測 這一塊   我們 可以 持續   讓 大家 安心 說   我們 是不是 持續 劇烈 沉降 或 傾斜 狀況   會 定期 跟 大家 報告 我們 監測 結果     校方 否認 超 抽 地下水   表示 當年 泳池 塌陷 後 就 沒 抽水   過去 抽 是 溢流 出 地面 水源   教育部 則說   過去 壓力 灌漿 是 延緩 地質 沉降 效果   立法 委員陳琬惠 表示     房子 跟 道路 就是 脫離 當中   所以 我 希望 我們 今天 要 找到 一個 方法   不是 只有 檢測 而已     水利 署 組長 簡昭群 說     技師 公會 去 依據 他 測量 結果   找出 造成 沉陷 具體 原因     陳 琬惠 近期 邀集 中央 單位 與 地方 居民 開會   研商 解決 辦法   水利 署 說   要 確定 當地 地層下陷 真正 原因   是 抽水 行為 還是 土質 問題   才能 根治 問題  ', '〔 記者 黃 旭磊 ／ 台中 報導 〕 台中市 烏日 溫水 游泳池 蓋 烏日 焚化廠 旁   由 於 地下水 井積沙 淤泥 嚴重   去年 起 停止 對外 開放   地方 民眾 認為 未 於 本月 如期 開館 營運   通報 台中市 議員 曾威   查出 泳池 前後地層 落差 約 14 公分   疑有 地層下陷 疑慮   環保局 強調   立即 通報 土木 技師 會勘 釐 清 下陷 疑慮       泳道 南側 比北側 低 了 約 14 公分     台中市 環保局 技士 本週 前往 烏日 溫水 游泳池 測量   查出 50 公尺 泳道 平面 傾斜 約 14 公分   南側 地勢 明顯 較 低   疑似 地層下陷 緊急 通報 台中市 土木 技師 公會 複 驗     曾威 說   泳池 蓋 慶 光路 焚化 爐旁   運用 焚化 爐 回饋 金設 置   當初 建造 是 因空 污影響 社區 回饋 鄉親   營運 十年 來 陸續 發生 池底 積沙   頂棚 消防 設備 被 消防局 要求 改善 等 問題   且 沒水 狀況 下   泳池 兩端 落差 14 公分   疑似 後 方有 地層下陷 相當 危險     烏日 溫水 游泳池 於 2016 年 起 營運   設有 10 道 50 公尺 泳道   兒童池   spa 池   烤箱 蒸氣室   今年 起 由 台中市 體育局 移交 給環 保局 列管     會勘 團隊 查出   泳池 北側 地勢 最高 處   水面 距 泳池 頂約 20 公分   南側 地勢 最低 處僅 約 6 公分   結構 明顯 出 問題   土木 技師 初 勘 認定 複 雜 程度 估價   再 進行後續 評估 結構 補強 作業     環保局 副 局長 陳 政良 說   預計 下週 14 日請 消防局 研擬 消防 設施 修繕 細節   至於 地層下陷 疑慮 將在 15 日請 廠商 鑑定 評估   盡 全力 讓 泳池 盡快 恢 復 營運  ', '〔 記者 黃 旭磊 ／ 台中 報導 〕 烏日 溫水 游泳池 蓋 烏日 焚化廠 旁   由 於 地下水 井積沙 淤泥 嚴重   去年 起 停止 對外 開放   地方 民眾 認為 未 於 本月 如期 開館 營運   通報 市議員 曾威 查出 泳池 前後地層 落差 約 十四 公分   疑有 地層下陷 疑慮   環保局 強調   立即 通報 土木 技師 會勘 釐 清 下陷 疑慮       泳道 南側 比北側 低 了 約 十四 公分     環保局 技士 本週 前往 烏日 溫水 游泳池 測量   查出 五十 公尺 泳道 平面 傾斜 約 十四 公分   南側 地勢 明顯 較 低   疑似 地層下陷   緊急 通報 台中市 土木 技師 公會 複 驗     曾威 說   泳池 蓋 慶 光路 焚化 爐旁   運用 焚化 爐 回饋 金設 置   當初 建造 是 因空 污影響 社區 回饋 鄉親   營運 十年 來 陸續 發生 池底 積沙   頂棚 消防 設備 被 消防局 要求 改善 等 問題   且 沒水 狀況 下   泳池 兩端 落差 十四 公分   疑似 後 方有 地層下陷   相當 危險     烏日 溫水 游泳池 於 二 一 六年 起營運   設有 十道 五十 公尺 長 泳道   兒童池   spa 池   烤箱 蒸氣室   今年 起 由 體育局 移交 給環 保局 列管     會勘 團隊 查出   泳池 北側 地勢 最高 處   水面 距 泳池 頂約 廿 公分   南側 地勢 最低 處 水面 距 泳池 頂僅 約 六 公分   結構 明顯 出 問題   土木 技師 初 勘 認定 複 雜 程度 估價   再 進行後續 評估 結構 補強 作業     環保局 副 局長 陳 政良 說   預計 下週 十四日 請 消防局 研擬 消防 設施 修繕 細節   至於 地層下陷 疑慮 也將 於 十五日 請廠 商鑑定 評估   讓 泳池 儘 快 恢 復 營 運  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>17</v>
-      </c>
-      <c r="B20" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>17_雲林縣_村_鄉鎮_電場</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>['雲林縣', '村', '鄉鎮', '電場', '光電業者', '屏東', '種電', '光電場', '枋寮', '鄉']</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>['陳 安邦 等 表示   種電 可以 村外   村內 緊鄰 民宅   不要 說 危害   打 開家門   窗戶 看到 就是 太陽 能板   叫 8   90 歲 老人 情 何以堪   尤其 庄內 種電 作為   請問 哪個 村 可以 接受   所以 村民 大團 結堅 決展 現反 對 到底 決心   任何 回饋 都 不用 說   打死 都 反 對 庄內 種電   任何 法律 問題 他 一個 人承擔   甚至 為 了 爭取 縣長 張麗善 村民 主持公道   特別 今天 前來 向 張縣 長 陳 情   唯一 要求 光場 業者 退出 瓦 磘 村     縣長 張麗善 接下 陳 情書 後 指出   地方 政府 跟 中央政府 都 各自 權責   公務人員 需要 配合 行政 程序   目前 法令 規定   若 是 建地 就 可以 百分之百 種電   雲林縣 農地 很多   地層下陷   易 淹水   不利 耕作 土地   已經 被 中央 核定 為 合法 種電 範圍   為 了 保護 我們 農地   特別 提出 三不三要   就是 不 希望 農地 上面 一直 種電   破壞 農地 未來 發展 跟 價值   光電業者 聚落 裡面 種電   已經 影響 鄉親 生活 起居 跟 品質   大家 不安 焦慮 我們 都 能 感同身受   縣府 透過 各種 協調 溝通   希望 能 保障 地 鄉親 權益  ', '屏東 是 光電場 熱區 之一   正 上演 光電板 與 農民 搶 地爭 奪戰   光電業者 挨家 挨戶 以 誘人 租金 勸 說 地主 租地 種電   租地 種蓮霧 果農 只能 忍痛 看著 心血 被毀   斬斷 兒子 想 當青農 接班 願望   青農 自嘲 說   政府 寧可 把 地租 給業者 種電   不給 老 農一畝 田維生   青年 若當   漂鳥   回農村   肯定 變走 投無路   落翅仔         五十六 歲 鄭明偉 林邊   佳冬 鄉 租下 三座 蓮霧園   他 說   兩座 花 了 十多年 整理   收成 正漸 入 佳境   地主 竟 收回 種電   他 只能 忍痛 放棄   由 於 種蓮霧 要 手把手 長 期培養 技術   正在 念農校 兒子 雖 有心 接手   但 他 勸 兒子 算了   最好 另謀 出路                             農民控 國產署   為 賺 更 多 租金     屏東 沿海 不少 國有 財產 署名 下 新生 地   被 農 民用 於 種田   六十三 歲 楊寶秀 枋寮 寮 段種 芭樂   無奈說   種芭樂近 四十年   也繳 用地 補償 金給 國產署   一直 相安 無事   近年 數度 送件 申請 合法 承租 都 被 拒絕   後 來 光電業者 芭樂園 貼 告示 已 承租 種電   要 農民 及早 搬離   國產 署則 回覆 因 地層下陷 不利 耕作   要 轉作光 電場       六十多 歲 呂姓 老農 靠 這片 三分 地 蓮霧 園維生   他 說   國產署 明知 老農靠 種蓮霧 養家   寧可租 給光 電業者 賺 更 多   如果 沒地 可種     我 不但 要 吃 土   連農保 都 沒 了         面對 農民 控訴   國產署 南區 分署 屏東 辦 公室 指出   光電業者 依法 種電   並願意 取得 承租人 或 使用 人 同意 書 後 清理 地上 物   占用 者 繳 使用 補償 金   但 他們 本 就 沒 合法 使用 權       林邊   佳冬 枋寮   蓮霧 之 鄉   美名   四十八 歲 陳 呈祥 八八 風災後回 鄉 接手 父親 蓮霧園   他 感嘆   近年 光電大舉 入侵   正 侵蝕 果農 維 繫 傳 統 產 業 所 努力       他 說   蓮霧 老農因 子女 無意 接手   只好 租地 給光 電商   果園 地主 刻意 抬高 租金 逼退 承租 農   一塊 塊 果園 被 光電場 取代   包圍   整體 產量 正持續 下降   衝擊 採收   包裝   運銷 等 產業 鏈   未來 工人 更難 找   材料 更貴   務農條件 就 更 差       農地 租金 上漲   加速 產業 衰退     陳 呈祥 說   蓮霧 產業 衰退 人口老化   缺工 等 有關   雖 不能 全歸責 光電   但 確實 造成 農地 租金 上漲 問題   間接 加速 產業 衰退   政府 對 這些 衝突視 若 無睹   苦果 只 由 農民吞       枋寮 農會 總幹事 鄭晏昕   林邊 農會 總幹事 黃 金順 都 慨嘆   原盼 農電能 共生   如今 衝突 嚴重   地 驕傲 半世 紀的 蓮霧 產業   正因 光電 面臨 式微 危機       黃 金順 說   光電場 租金 一分 地四萬元   承租 農民頂 多出 得起 一萬元   相差 四倍   到 處 都 聽 到 地 主要 改 種電   年 輕人 想 返 鄉務農   無 低 租金 農地 可種     蓮霧 故鄉   金字招牌 正在 褪色       台大 農經 碩士 張靜玉 是 枋寮 蓮霧 農   眼看 鄰近 農民 被 光電 搶 地   忿忿不平   直指 當年 農委會 主委 蘇嘉全 還推 漂鳥 計畫   要 青年 返鄉務農   現在 連地 都 租 不到     這 不是 迫遷 青農去 都市 討 生活   漂鳥 回農村   恐怕 走 投無路 變 落翅仔    ', '聯合 報陽光 行動 專題 報導光 電進 駐 屏東   種電 範圍 遍及 農地   山區 到 文資 價值 二戰 遺跡   造成 家園 地景 地貌 變遷   衝擊 老 農生計   變相迫 遷青農   更 被 地方 形容 為   惡鄰     產生 蛇 鼠 與 害蟲   提升 鄰田 管理 困難度   還潛藏 糧食 危機     縣府 環保局 長 顏幸苑 表示   光電不會 無限 擴張   目前 種電 專區 仍 約 3 千公頃 可 耕作 並專案 輔導業者 除草   一定 會 兼顧 農業 永續 發展       顏幸苑 表示   台電饋 線 上限 規定   目前 既有 電力 設施 併 網 上限 下   限度 推動 光電 專區   不會 無 限制 使用 農地 種電   而 東港鎮   林邊   佳冬   枋寮 鄉 等 4 鄉鎮 專案 截至 去年底   共 併 網約 3 百 兆瓦 光電   該區 農地 總面 積約 3800 公頃   至少 還有 約 3 千公頃 面積 可 農作   使用 農地 比例 不到 4 鄉鎮 農地 總面積 一成                             強調   從 未 要求 廠商 提供   不利 耕作 同意 書   或 其他 不 平等 條約 相關 文件   針對 部分 地區 爭議 案件   未 取得 居民 同意 之前   皆 已 要求 業者 停止 施工   另太陽能 案場 內並 無 食物 來源   應非屬 引來 老鼠 主因   目前 已 要求 專案 輔導業者 定期 進行 除草   維護 周遭 環境 整潔       指出   屏東 綠能 推動 政策 以   專案 專區 計畫       土地 複 合式 利用   等 2 大 策略 為 優先   限度 使用 相對 不 適合 耕種 土地 發展 綠能   提供 給 地主   農民階段 性 活化 土地 新選擇   對 於 無力 管理 田間 工作   又 土地 鹽化 等 不利因素 無法 耕作 年 邁老農   則 可以 穩定 收入 過 退休 生活   至於 非 專案 專區 鄉鎮   則優先 鼓勵 廠 商以   土地 複 合式 利用   方式   利用 既有 設施 結合 太陽光 電設施   有效 利用 公共 空間       屏縣 府 綠能 辦 公室 表示   尊重 私有 地主 處置 自家 土地 財產   及業者 依法 申請 案件 權利   相關 審查 過程將 審慎 關注 山坡地   耕作 農地   歷史 遺跡   生態 保育 或 重要 觀 光景 點聯絡 道路 沿線 等 議題   並 要求 廠商 提出 因應 作為   以 避免 衍生 爭議性 問題   兼顧 開發 合理性 及維護 本縣 農民 耕作 權益       生利 能源 表示   屏東 枋寮 案場 是 合法 開發   於 2020 年 9 月 於 案場 發現 碉堡 等 歷史 遺構 後   隨即 保留 並主動展 開一連串 文資 保護作 為   並無二戰 槍堡 被 挖除 等 情事  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>18</v>
-      </c>
-      <c r="B21" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>18_水資源_水源_地下水_水利</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>['水資源', '水源', '地下水', '水利', '用水量', '阻水層', '缺水', '供水', '用水', '水庫']</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>['〔 記者 顏宏駿 ／ 彰化 報導 〕 彰化縣 沒有 水庫   多年 以來 不 缺水   民生 用水   原因 係 倚賴 全縣 200 多口 地下水 井   但 已 造成 地層下陷 問題   惟鳥 嘴潭 人工湖 淨水廠 完工 後 將可 改變 現今 抽 地下水 窘境   目前 台一線 南 彰化 段 正 進行 大型 管路 埋設 工程   2026 年 完工 後   這條 管路 成為 彰化縣 給水大動脈   透過 管路 連結   達到 鳥 嘴潭 人工湖   湖山 水庫   鯉魚 潭 水庫 水源 靈活 調度 目的     台水 公司 指出   目前 鳥 嘴潭淨 水廠 工程 進行 中   埋管 工程 多線 展開   直徑 1.2 公尺 幹管 埋設 工程   為 避免 影響 交通   採 分段 施工   預計 2026 年 全部 完工   最後可達 到 北水南 送   南 水北 送   靈活 供水 目標     台水 公司 表示   目前 彰化縣 每日 用水量 約 為 40 萬公噸   地面水 部分   彰化市 與 美   花壇 部分 地區 每日 用水量 約 為 8 萬公噸   主要 靠 台中 支援   鯉魚 潭 水庫     南 彰化 北斗   二林 與 溪湖 一帶   則由 雲林   湖山 水庫   每日 支援 約 5 萬公噸   烏嘴潭淨 水廠 完工 送水 後   彰化縣 每年 可減 抽 6100 萬噸 地下水   解決 農民 枯水期 經常 抽 不到 地下水 窘境     台水 公司 說   未來 鳥 嘴潭淨 水廠 每天 可供 應 彰化 地區 21 萬噸 水量   加上 現有 每日 來 自 雲林 湖山 水庫 5 萬公噸   而 透過 台 一線 埋設 幹管   南   北 水路 相通   增加 水資源 調度 彈性   上游 採 一般 水庫 採高 水位 操作   依循   蓄豐濟 枯   邏輯   趁 豐水期 盡量 蓄滿   枯水期 才 水 可用   包含 中水 局轄區 鯉 魚潭   湖山 水庫   目前 處 於 枯水期 階段   卻 仍 持續 滿水 溢流   未來 能 應付 極端 氣候 或 突發 供水 危機     台水 公司 第十一 處長 曾 盛一說   水資源 運用 已 不 像 過去   單一 水庫 供水 區 固定   水利 署力 拚 打造 西部 廊道 供水管 網   強化 區域 調度 同時   鳥 嘴潭 雖 不是 直接 參與 管網   但 透過 減少 中部 水庫 支援 彰化 水量     其實 達 到 調度 功能    ', '旗 山溪 與 荖 濃溪 交會 匯流 進入 高屏溪   是 大 高雄 地區 民生 用水 主動脈   是 枯水期 間 地下水 主要 供水 區域   如何 永續 地下水 資源   是 當前 重要 課題   經濟部 水利 署 規劃 高屏溪 跟 荖 濃溪 上游   設置 地下水 補注區   112 年 已 設置 約 11 處   總計 460 公頃   評估 一年 補注 將近 1400 萬噸 補 注量   地下水 補注區 利用 疏浚 砂石 河床 蓋 微型 土堤   讓 水流 受阻   流速 變慢   增加 滯水範圍 讓 更 多水 滲入 地下   當 抽取 完 地下水 後   透過 自然 入 滲補注   就 能 讓 地下水位 快速 回 復 平常 水位 以上   使 地下水 源 得以 永續   1960 年代 起   台灣 引進 地下水 鑿井技術   台灣 西 半部 沿海 養殖 漁業 盛行   大量 地超 抽 地下水   使得 地層下陷   海水倒灌   土壤 鹽化 等 問題 層出 不窮   有關 高雄 運用 地下水 資源 是否 會 造成 地層下陷   水利 署透 過長 期 監控 做出 釋疑   經濟部 水利 署 水文 技術 組科長 吳 明哲 表示   高屏溪 沿岸 屏東 平原 地下水 區   主要 以砂礫 石層 為 主   礫石 跟 礫 石之間 顆粒 地下水 時候   不會 壓密行 為   地下水 一旦 下降   因顆 粒 與 顆粒 支撐   不會產生 壓密 沉陷   另 根據 屏東 科技 大學 名譽 教授 丁澈士 老師 實驗   模擬 高雄 地區 砂礫 石層 抽水 情況   證明 砂礫 石層 比較 不會 出現 地層下陷   民眾 不必 過度 擔心   經濟部 水利 署南區 水資源局 副 局長 何達夫 說明   軟礫 石層 跟 粘土 層 不 一樣   粘土 層 抽水 後 會 下陷   但 軟礫 石層 是 一個 石頭 接著 一個 石頭   把 石頭間 水 抽掉   抽走 得 很快 補充 非常 快   不會 地層下陷 問題   專家 強調   只要 不過度 超 抽   加上 嚴密 監測   就 不必 擔心 地層下陷   學者 呼籲   豐水期 應多加 利用 地下水   不僅 能夠 避免 水資源 浪費   還能夠 防洪 減災   高屏溪 擁有 豐沛 地下水 資源   從 鑿 井 取水 到 地下水 補注   不僅 讓 水資源 得以 永續   成為 高雄 地區 對 抗旱 象 關鍵 利器  ', '2023 年 9 月 海葵 颱 風 登陸前   南部 地區 一度 超過 600 天沒有 下雨   高雄 爆發 旱象   雖然 高雄 地表 缺水   但 地面 下 卻 蘊藏 豐富 水源   根據 統計   高雄 高達 8 成到 9 成的備 援用 水   都 能 取自 地下水 及伏 流水   但 大規模 鑿 井 是否 會 剝奪 農業 用水   甚至 造成 地層下陷   時序 來 到 年底   全 台 各地 開始 進入 枯水期   加上 氣候變遷   南北 降雨 不均   不少 人憂心   南 台灣 今年 是否 會 再度 面臨 缺水 危機   幸好 高雄 地區 地表 之下   蘊藏 了 神 祕 巨大 水庫   靠 著伏 流水 資源   度過 缺水 危機   高雄 大泉 伏 流水 取水 站   內徑 15 公尺   深 19 公尺 集 水井 裡頭   有著 11 個 粗大 管線 負責 抽水   將伏 流水 運到 淨水廠   供 民生 用水   所謂 伏 流水   就是 流動 或是 儲 存在 河床 底下   砂礫 石層 當中 水源   透過 自然 過濾 或是 滲透   流入 地面 之下   包括 了 由 粗顆 粒 土壤 組成 含水 層   以及 由細顆 粒 粘土 組成 阻水層   伏 流水 大約 落 地面 下 15 到 20 公尺   反觀 如果 滲透到 了 20 到 40 公尺 深   稱為 淺層 地下水   如果 繼續 滲透到 了 50 公尺 以下 到 150 公尺 處   則稱 為 深層 地下水   屏東 科技 大學 名譽 教授 丁澈士 表示   伏 流水 變成現 救命 水   尤其 是 汛期 時候   它 非常 乾淨   外面 河川 裡面 濁度 甚至 於 飆到 10 萬個 NTU   根本 就 沒 辦法 後 製 沉 沙   沉 澱 處理   但是 伏 流水   因為 河水 跟 井水 是 相通   所以 伏 流水 就 可以 發揮 它 這段 時間 裡面 作用   所以 就 變成 所 說 救命 水   同樣 被 視為 救命 水源   還有 這 一根 根 打入 地底下 抗旱 水井   別 小看 這些 不起眼 水井   它們 可是 解決 高雄 缺水 危機 抗旱 英雄   類 似的 抗旱 水井   已經 3 年間 高雄 陸續 開鑿 了 110 座   每日 供水量 將近 35 萬噸   雖然 穩定 水情   但是 大規模 鑿 井   卻 讓 當地 農民相 當憂心 是否 會 剝奪 農業 用水   對此 專家 解釋   抗旱 水井 是 取用 深度 達 100 到 150 公尺 深層 地下水   與 一般 深 20 到 40 公尺 間   淺層 地下水 農業 灌溉 井   含水 層 不同   而且 兩者 間 還有 阻水層 相互 阻隔   因此 開鑿 抗旱 水井   對 於 農業 用水 並不會 產生 影響   高雄市 水利局 長 蔡長 展 表示   抗旱 水井 其實 是 一個備 援用 水   它 使用 時間 大概 每年 3 月 到 5 月   到 了 下雨 時候   我們 就 沒 再 用   就是 藉由 下雨 時候   會 地下水 補注   所以 對 整個 地下水位 來講   跟 市民 用 一些 農業 灌溉 用水   是 安全   神 祕 地下水 補注區   其實 就 隱身 高屏溪 河床 底下   從 空中 俯瞰   這些 不起眼 灰色 土石   全都 扮演 關鍵 角色   所謂 地下水 補注區   就是 利用 疏濬 砂石   河床 蓋 微型 土堤   讓 水流 受阻   流速 變慢   增加 滯水範圍   讓 更 多水 滲入 地下   藉此 增加 地下水 量   使得 地下水 源 得以 永續   大量 運用 地下水 資源   不免 讓 人 憂心 抽取 地下水   是否 會 造成 地層下陷   水利 專 家丁 澈士 教授 解釋   因為 這 一些 土壤 裡面   一些 礫石 跟 比 較 粗 沙子   所以 說 放釋 水 時候   它 比 較 不會產生 所謂 壓密 沉陷   因為 它 骨架 會 互相 地支 撐   實驗 還原 了 高雄 地層 下 狀況   清楚 證明 了 砂礫 石層 確實 比較 不會 出現 地層下陷 情形   因此 民眾 不必 過度 擔心   南區 水資源 分署 副 分署 長 何達夫 表示   軟礫 石層 跟 粘土 層 不 一樣   粘土 層 抽 了 水之後它 是 會 下陷   但是 軟礫 石層   是 一個 石頭 接著 一個 石頭   是 把 石頭間 水 抽掉   它 抽走 得 很快   補充 非常 快   那個 地方 抽 地下水   是 不會 地層下陷 問題   極端 氣候 肆虐 全球   缺水 危機 恐將 一再 重演   無論 是 伏 流水 還是 地下水   都 是 抗旱 時期 救命 水源   唯有 善加利用   才能 讓 危機 成為 轉機  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>19</v>
-      </c>
-      <c r="B22" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>19_新竹市_地下水位_新竹_巷道</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>['新竹市', '地下水位', '新竹', '巷道', '地下水', '市府', '水井', '巷', '地下', '高雄']</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>['順著 高屏溪 右岸 來 到 高雄 大樹區 九曲堂 工作站   從 空中 俯瞰 一個 個 用圍 欄圍 起 方形 區塊   排列 整齊   錯落 其中   靠近 一看 才 發現 這是 一根 根 打入 地底下 水管   稱為 抗旱 水井   高雄市 政府 水利局 表示   所謂 抗旱 水井 是 抽取 深層 地下水   從 地表 往下 150 米 深   透過 抽水 設備   將深層 地下水 經由 抗旱 水井 取出   相較 於 海淡廠   再生 水 等等   取水 更為 快速   成本 更 低   供水量 更 大 地下水   成為 抗旱 期間 關鍵 水源   類 似的 抗旱 水井 已 高雄 陸續 開鑿 110 座   每日 供水量 將近 35 萬噸   雖然 穩定 水情   但是 大規模 鑿 井 卻 讓 當地 農民相 當憂心   是否 會 剝奪 農業 用水   對此 專家 解釋   抗旱 水井 是 取用 深度 達 100 到 150 公尺 深層 地下水   與 一般 深 20 到 40 公尺 間 淺層 地下水 農業 灌溉 井   含水 層 不同   且 兩者 間 還有 阻水層 相互 阻隔   因此 開鑿 抗旱 水井 對 於 農業 用水 並不會 產生 影響   水利局 局長 蔡長 展 指出   抗旱 水井 是備 援用 水   使用 時間 大約 每年 3 月 至 5 月   藉由 雨水 對 地下水 進行 補注   對 農業 灌溉 用水 不受 影響   根據 地下水位 監測 資料 顯示   112 年 1 月份 地下水位 高點 落 14 公尺   接著 隨著 枯水期 到 來   地下水位 5 月份 降到 了 大約 6 公尺   隨後迅 期到 來 開始 降雨   加上 高雄市 政府 與 水利 署 合作   推動 高屏溪 流域 河道 疏濬 補注 地下水 計畫   增加 地下水 量   使得 9 月份 地下水位 上升 到 16 公尺   足足 比 枯水期 高出 了 10 公尺   甚至 高 於 1 月份 水位   枯水期 嚴密 監控   視情況 抽用   豐水期 加強 地下水 補注   能夠 達 到 水資源 永續 發展 目標   經濟部 水利 署 副署 長 林元鵬 說明   高雄 地區 總 共有 11 口 觀測 水井   所有 水井 都 會 進行 管控   只要 是 有效 地去 管控 數據   地下水 高雄 地區 是 可以 當作 一個 安全 用水   嚴密監 控確 保不會 造成 地層下陷 影響 水源 保育 情況 之下   短期 備援 抗旱 水井 不僅成 了 抗旱 功臣   賦予 地下水 資源 更 多元 運用 可能  ', '新竹市 和平 路竹 慶建設   筑光   建案 工地 下 挖 地下室   未料 前天 發生 基地 旁 道路 下方 自來 水管 線   瓦斯 管線 洩漏   連帶 造成 和平路 20 巷 地層下陷   由 於   天坑   填平 後   今天 又 他 處 塌陷   竹 市府 下午 成立 前進 指揮 所   市長 高虹安 提出 8 點 指示   包括 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置 並即 時 回報   確保當 地 安全       和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   前天 竟釀 緊鄰 巷弄 道路 下陷 後   被 市府 勒令停工   不過   因為 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 對 道路 持續 下沉 塌陷 狀況 相當 擔憂   市府 今天下午 請來 4 大技師 公會 到場 會勘                             高虹安 今天 中午 下令 於 竹光國 中旁 成立 災害 應變 前進 指揮 所   並 要求 廠商 與 消防局   警察局   都 發處   民政 處   產發處   區 公所 立即 派員進 駐   下午 4 點半   高虹安 會 同 土木 技師 等 四大 專業 技師 公會 民富 里 沈朝 旺里長 聽取 簡報   並 了解 居民 訴求       高虹安 今晚 臉書 發文 說明   針對 此案 已下 達 8 項 指示   包含 責成 消防局   工務處 與 產發處 聯 繫 自 來 水 與 瓦斯 公司 明天 立即 進場 全面 開 挖汰 換成 最新 管線   因無法 同 時汰換 兩種 管線   將 依序 先後汰換 自來 水 與 瓦斯 管線       由 於 傾斜計 監測 數值 逼近 警戒 值   高虹安 要求 廠商以 最快 速度 完成 對 周邊 民宅 自動 傾斜 偵測 設備 裝置   並即 時 回報   要求 消防局 會同 民政 處   社會處 研擬 若事態 進 一步 擴大時   緊急 撤離 與 安置 措施   並預 準備       明天 開始 於 管線汰換 與 相關 改善 工程 期間   要求 廠商 每日 提供 足量 飲 用水 與 水車 供 停水 住戶 使用   要求 交通 處開放 周邊 停車場 供 居民 暫時 停放 車輛   竹光 國民運動 中心 免費 開放 居民 盥洗 使用       高虹安 說   確認 改善 完成 前   要求 災害 應變 前進 指揮 所 全天候 開設   隨時 提供 居民 諮 詢 與 處理 居民 回報 相關 問題   於 管線汰換 與 相關 改善 工程 期間   要求 警察局 做好 周邊 交通管制   確保 對 當地 交通 衝擊 降到 最低       高虹安說   今天 現場 與 當地 居民 溝通 與 聆 聽 心聲   並 一一 記錄   要求 廠商 與 局處 盡 全力 處理   強調 市府 團隊 一定 是 各位 最大 靠山   不僅會 要求 廠商 負起 責任   完成 改善 並經 確認 安全 無虞 之前   不得 進行 除了 安全工程 以外 其他 工程   新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影 新竹 市長 高虹安 今天下午 到 和平路 20 巷 了解 居民 心聲   圖 ／ 竹 市府 提供 新竹 市長 高虹安 今天下午 進入 建案 基地 勘查 狀況   圖 ／ 竹 市府 提供 新竹市 和平 路竹 慶建設   筑光   建案 工地 旁 和平路 20 巷 地層下陷   連日來 都 搶 修處理   記者 張裕珍 ／ 攝影', '新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   還有 自來 水洩漏   瓦斯 異味 飄散 情形   引起 住戶 疑慮   雖然 天坑 處緊 急 回填   但 仍 持續 他 處 下陷   建物 傾斜計 監測 數值 逼近 警戒 值   自來 水 公司 將於 明天 起汰換 上百 公尺 老舊 自來 水塑膠 管線   市長 高虹安 下午 赴 前進 指揮 所 了解 應變 情形       新竹市 和平路 該 建案 工地 規畫 地上 14 層   地下 3 層 建物   正在 下 挖 地下 3 層   未料 前天 竟釀 緊鄰 巷弄 道路 下陷   由 於 一旁 住家 距離 建案 基地 只有 3 公尺   將近 40 戶住 戶 相當 擔憂   市府 今天下午 請 來 4 大技師 公會 到場 了解   確認 工地 與 道路 下陷 情形                             據 了解   前天 發生 和平路 20 巷   天坑   事件 後   建商 取得 住戶 同意 20 巷前   中   後 段 設置 建物 傾斜計 監測 傾斜 情形   今天 最新 測得 最大值 每秒 387   已經 接近 每秒 413 警戒 值   由 於 和平路 20 巷 仍 道路 下陷   漏水 情形   今天 緊急 加裝 關水閥 處理       建案 營造 商工 務經理 黃 姓 經理 說   建案 地質 為 砂質 帶土   下 挖 施工 採鑽掘 方式 進行   強度 類似 連續 壁 工法   但蔽 體開 挖 壓力 造成 基地 外側 道路 內部 土壤 位移   加上 巷內 老舊 自來 水管 線 破裂   漏水 導致 土壤 泥沙 流失   進而 造成 地層下陷   水 流入 基地       由 於 和平路 20 巷內 約 3   40 戶 民宅   民富 里里長 沈朝旺 說   住戶 都 擔心 房子 會 塌陷   不要 等到 真正 傾斜 就 來 不及 了   希望 相關 單位 公告 監測 數據   並 加快 自來 水 與 瓦斯 管線汰換   自來 水 公司 明天 將進場 開 挖   汰換 鑄鐵管   盼 建商 同步 處理 好 地基         各項 資訊要 更 透明   讓 住 戶們 安心     楊姓 住戶 說   他 巷 住 了 20 年   其他 老住 戶 更 住 了 40 多年   大家 都 擔心 道路 下陷 擴大   希望 檢測 資訊 更加 透明   因為 他們 肉眼 看不到 傾斜 程度   很 需要 科技 儀器 來 幫忙 監測   數據 要 公開 讓 住 戶 都 了解       由 於 建案 工地 旁不斷 道路 下陷   建案 自行 組成 應變 中心   應變 中心 代表 允諾   已經 協調 明天 自來 水 公司 進場 換管   加派 人力 前   後 分頭 施工 情形 下   能 7 天汰管 完成   預計 10 月初 再換 瓦斯 管線   若 傾斜計 監測 到 了 警戒 值   將 安置 住戶 入住 旅館       新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   造成 緊鄰 和平路 20 巷道 路 下陷   明天 將進 場汰換 老舊 自來 水管 線   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室 造成 緊鄰 和平路 20 巷道 路 下陷   市府 今天 設置 前進 指揮 所   市長 高虹安 下午 到場 了解 應變 情形   記者 張裕珍 ／ 攝影 新竹市 和平路 某建案 工地 下 挖 地下室   前天 發生 緊鄰 和平路 20 巷道 路 下陷   市府 今天 邀集 技師 公會 進入 工地 會勘   記者 張裕珍 ／ 攝影']</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>20</v>
-      </c>
-      <c r="B23" t="n">
-        <v>4</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>20_新竹市_道路_市公所_路面</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>['新竹市', '道路', '市公所', '路面', '市府', '新竹', '坍塌', '巷', '台北', '施工']</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>['疑因   豐采 520   建案 導致 竹 北市 莊敬 六街 發生 道路 坍塌   一輛 特斯拉 還掉 進去   新竹縣 長 楊 文科 今天 表示   已 與 竹北 市長 鄭 朝方 協議   市公所 將 全力 配合 相關 作業   並 要求 建商以 透地雷達 設備   預防性 檢測 建案 四周 道路 土質 情形   預防 再次 坍塌   工務處 表示   目前 初判 造成 此次 坍塌   原因 是 建商開 挖 地下室 抽取 地下水   導致 土砂 層 部分 帶 走 地層下陷   為 防止 附近 道路 再次 發生 坍塌   已 要求 建商以 透地雷達 設備 詳實 檢測 建案 四周 勝利 二路   勝利 一路   莊敬 六街 自強 北路   確認 是否 仍有 土質 流失 造成 坑洞   由 於 該 路段 路權 為 竹北 市公所 權責   縣長 楊 文科 與 竹北 市長 鄭 朝方 達 成共識   市公所 將 全力 配合 周邊 道路 封鎖 透地雷達 監測 等   展開 全面 檢測   縣府 已 與 市公所 研議 相關 作業   確保 附近 住戶 安全 無虞   工務處 指出   縣府 已 要求 建商 於 維生 管線   自來 水   電力   瓦斯 等 檢測 維修 完成 後   會同 竹北 市公所 同意   以低 強度 混凝土 灌漿 補強   針對 承造 監造 人   縣府 希望 加重 懲罰 機制   將 蒐集 近幾次 相關 違 失事 證   移送 新竹縣 營造業 審議 委員會 建築師 懲戒 委員會 審議   另外   縣府 也將 此次 工安 事件 提列 為 建築 爭議 損鄰 事件   立案 列管   通知 起造   承造 監造 人 改善 鄰房 損害 情況   並 於 完成 安全 改善 修 復 後   檢具 相關 證明 文件 與 同意 書 報府 核備   後 續 建商 必須 與 受 損戶 達成 和解   縣府 才 會 核發 使用 執照   工務處 說   縣府 將持續 配合 新竹 地檢署 調查   後 續 該 工地 建商 如 欲 復工   縣府將 與 竹檢 取得 共識   要求 工地 完善 工地 安全   確定 鑑定 報告 結果 無 虞   舉辦 施工 說 明會   繳清 所有 罰 鍰   以 嚴格 標準 檢視 改善 結果 後   再 評估 是否 辦理 復工  ', '新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     凹陷 面積 約 1 公尺 見方   雖然 緊急 灌漿 回填   但 今天 又 發現 巷 另 處 凹陷 下沉   由 於 一旁 不到 3 公尺 緊鄰 20 多戶 住戶   引發 住戶 擔憂   整夜 睡不著     民代質疑 工法 問題   未來 恐繼續 塌陷       市府 都 發處 指出   昨天 已 勒令 建案 停工   裁罰   並 要求 廠商 進行 加固 支撐 灌漿 作業   自來 水 公司 今天 派員現 勘 要汰換 道路 下方 自來 水管 線   之後將 觀察 管線 狀況 再 重鋪 路面   現場 將加裝 傾斜儀 24 小時 檢測   預警   以確 保住 戶 安全 為 最大 前提                             據 了解   該 建案 基地 正下 挖 到 地下 3 層   頻繁 重車 進出   先前 就 有人 發現 建案 基地 旁 道路 與 民宅 出現 裂縫   昨天 則開始 出現 道路 地層下陷   還伴 隨 瓦斯 異味   讓 周邊 住戶 相當 害怕   就 怕 上演 基泰 大直 工地 事件       竹 市府 指出   地層下陷 疑似 為 建案 基地 內側 開 挖 後   造成 基地 外側 道路 內部 土壤 位移   連帶 造成 自來 水管 線 破裂   沖 刷 土壤 泥沙 後 再 造成 地層下陷   瓦斯 管線 破裂       市議員陳慶齡 熟悉 建築 營造 工程   他 說 該 建案工 地位 於 沙地   正在 下 挖 地下室   懷疑 打 基樁 過程 不夠 密實   導致 基地 旁 道路 沙土 不斷 流失 流進 地下室   才 會 造成 道路 沈陷   如果 沒有 妥善 處理   未來 還是 會 發生 道路 沈陷 可能       和平路 20 巷 住 戶 約 20 多戶   居民 無奈   不敢 休息     擔心 瓦斯 味 很重   萬一 爆炸 怎麼 辦   平常 只有 兩老住 這 而已   半夜 已經 沒法 入睡   眼看 住家 旁建案 工地 才 剛蓋   未來 至少 還要 辛苦 兩   三年   希望 做好 偵測   事先 預防   否則 出事 就 麻煩 了   新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     今天 還有 另處 塌陷   記者 張裕珍 ／ 攝影 新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     雖然 已經 回填   但 仍 可見 到 住家 前方 有裂 縫   記者 張裕珍 ／ 攝影 新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     雖然 已經 回填   但 仍 可見 到 住家 前方 有裂 縫   記者 張裕珍 ／ 攝影 新竹市 和平路 20 巷 某建案 工地 旁 道路 昨天 驚見   天坑     今天 還有 另處 塌陷   記者 張裕珍 ／ 攝影', '新竹市 和平路 20 巷 昨 下午 驚見   天坑     市府 獲報 到場   確認 是 和平路 某建案 工地 施工 造成 緊鄰 道路 下方 自來 水管 線   瓦斯 管線 洩漏   導致 地層下陷   多名 民代 要求 強化 安全 檢測   市長 高虹安 昨 要求 建商務必 盡速 完成 改善   市府 並 勒令 承造 人 立即 停工   依法 裁處   改善 完成 無虞 才能 復工       市府 表示   昨 下午 13 時 35 分多 消防局 受理 和平路 出現 道路 地基 下陷   還伴 隨 瓦斯 異味   相關 單位 都 獲報 搶修   由 於 近期 接連 發生 竹北 天坑   基泰 大直 工地 事故   和平路 附近 居民 人心惶惶                             時代 力量 立委 邱顯智   市議員林彥 甫 說   要求 建商確 保相關 支撐   才能 復工   希望 安全 檢測 頻率 從 1 周 2 次 至 每天 1 次   國民黨 市議員 黃 美慧 認為   未來須 全面 將 瓦斯 自來 水管 線 更新   同時須 工地 周邊 建築安裝 警示 裝置   確保 居民 安全       市府 指出   該 建案 工地 下 挖 到 地下 3 樓   依規 有施 打 預壘 樁 擋 水樁   但 疑似 為 基地 內側 開 挖 後   造成 基地 外側 道路 內部 土壤 位移   連帶 造成 自來 水管 線 破裂   沖 刷 土壤 泥沙 後 再 造成 地層下陷   瓦斯 管線 破裂       市府 指出   已 要求 建商 改善 期間 每日 需以 儀器 監測 周邊 民宅 無 傾斜 情形   後 續 將持續 觀察 自來 水管 是否 還有 造成 洩漏       由 於 施工 造成 地層下陷   都 發處將 依建築法 89 條 勒令停工   並針 對 起造 人   承造 人   監造 人先 進行 裁罰 各 3 萬元   並視後續 情況 再行 論處  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>21</v>
-      </c>
-      <c r="B24" t="n">
-        <v>4</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>21_水資源_水源_水利_蓄水量</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>['水資源', '水源', '水利', '蓄水量', '淨水場', '供水量', '水場', '供水', '用水', '地下水']</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>['〔 記者 李容萍 ／ 桃園 報導 〕 桃園市 石門 水庫 水情 吃緊   截至 今   21 日   中午   蓄水量 7131 萬噸   蓄水 率 34.75 ％   經濟部 水利 署自 19 日起 調整 桃竹苗 地區 水情 燈號 為   水情 提醒   綠燈   提醒 各界 節約 用水   國立 中央 大學 研究 團隊 今 發表 於 新屋 綠色 隧道 海岸 線 TaiCOAST 臨海 工作站   發現 地下水 出流 現象 非常 強勁   每年 出 流量 達 1 億公噸   相當 半座 石門 水庫 容量   這項 成果 刊載 於 新一期   水文 學雜誌   Journal   of   Hydrology     Regional   Studies 頂尖 期刊   未來 可進 一步 研究 探討 如何 適度 使用 不會 造成 環境 危害     中央 大學應 用地 質 研究所 教授 倪春發 表示   海岸 帶 地下水 出流   Submarine   Groundwater   Discharge     SGD   為 地下水 直接 流進 海洋 自然 現象   普遍存在 於 世界各地   中央 大學 TaiCOAST 臨海 工作站 自 2021 年 開始 進行 新屋 海岸 帶 地下水 出 流量 調查   發現 即使 2021 年 大旱 期間   遭遇 台灣 56 年 來 最 嚴重 缺水 危機   出 流量 仍 相當 豐沛     研究 團隊 透過 鑽井   深入 地下 100 公尺   發現 打出 仍 是 淡水   透過 數學 模型 計算 流速 面積 累加   發現 新屋 地區 海岸 帶 地下水 出 流量 每天 可達 30 萬噸   1 年 高達 1 億噸   相當 半座 石門 水庫 容量   近年 來 調查 結果 更 發現   新屋 區往 北 海岸 出 流量 更 高潛勢   顯示 桃園 海岸 帶 整體 地下水 出 流量 更為 可觀     研究 團隊 指出   台灣 年 降雨量 約 2500 毫米   約 為 全球 平均 3 倍   但 因 台灣 地形 梯度 較大   60 ％ 流入 海洋   只有 5 ％ 含水 層   儘 管 台灣 降水量 高   但 水資源 有限   雖然 發現 地下水 出 流量 資源 豐沛   但 如何 汲水 開發   不致 造成 海水 入侵 地層下陷   涉及 政策   科學 工程 等 多重 挑戰   還需 兼顧 出海口 生態 平衡   才能 造福 國家 社會     此 研究 團隊 涵蓋 中央 大學 地球 科學學院 各系所 老師   包括 應 用地 質 研究所 教授 倪春發   副教授 王士榮   水文 與 海洋 科學 研究所 教授 李明旭   錢樺   副教授 黃 志 誠   以及 地球 科學學系 教授 顏宏元   陳 建志 等 人   各自 發揮 所長   追求 科學 卓越   期許 對 人類 社會 有所 貢獻  ', '因應 極端 氣候   水利 署 投入 123.6 億元展 開   鳥 嘴潭 人工湖 下游 自來 水 供水 工程 計畫     包括 6 座 人工 蓄水池 草屯   鳥 嘴潭 2 座淨 水場   鳥 嘴潭 人工湖 自 2022 年 11 月 起 每日 供水 9 萬噸   其中 彰化 7 萬噸   南投 2 萬噸   草屯 淨水場 今年 3 月 27 日 正式 完工 出水   總 供水量 提升 到 每日 14 萬噸   並持續 推動 鳥 嘴潭淨 水場 工程   預計 2025 年底 可達 日供 25 萬噸 目標   4 萬噸 供 草屯   21 萬噸 供 彰化 地區 使用     陳 建仁 與 經濟 部長 王美花 視察 草屯 淨水場 新建 工程   立委 馬 文君   游顥 等 均 到場   王 瑞德 當場 向 陳 建仁 爭取 補助 延管 或 增加 簡易 自來 水經費 補助   盼 讓 偏鄉 地區 鄉親 能 同享 量 好質 優 水資源   他 並建議   鳥 嘴潭 人工湖 周遭 可 執行 綠毯 計畫   持續 綠 美化   取得 民眾 對 水庫 建設 喜 愛     陳 建仁 說   烏溪 鳥 嘴潭 人工湖 計畫 是 政府 核定   雲彰 地區 地層下陷 具體 解決 方案 暨 行動 計畫   中 重大 建設 之一   草屯 淨水場 為 其中 一環   3 月 已 達 最大 設計 出水 功能   通過 5 萬 CMD   立方公尺 ／ 每日   能力 測試   比 原訂 期程 提早 3 個 月   相信 未來 完工 後   定能 穩定 供 應質 優   量 足 水資源   進 一步 帶動 地方 發展     游顥會 後 指出   南投縣 水源 長 期不斷 供給 外縣 市 居民 使用   但 南投縣 自來 水 普及率 水管 汰 舊換 新 都 需要 中央 支持   草屯 淨水廠 應 優先 滿足 南投縣 用水 需求   剩餘 供水量 再 調度 給外 縣市   才能 實際 解決 南投縣 用水 問題  ', '烏溪 鳥 嘴潭 人工湖 是 中部 地區 最 重要 水利 計畫   總 蓄水量 1450 萬 立方公尺   目前 透過 草屯 淨水場 5 月 起 每日 供水 14 萬噸   等 彰化 鳥 嘴潭淨 水場 明年 12 月 完工   可達 到 最大 每日 25 萬噸 供水量     陳 建 仁和 經濟 部長 王美花 今天 視察 草屯 淨水場   自來 水 公司 董事 長 李嘉榮 簡報   中部 地區 供水 面臨 極端 氣候 影響 產業 發展區   整體 需水量 不斷 增加   造成 雲彰 地區 超 抽 地下水   地層下陷   鳥 嘴潭 人工湖 可 增加 供水   並 改善 地層下陷 問題     人工湖 已蓄 滿 5 個 湖區   C 湖區 預計 5 月底 蓄滿   台水 負責 下游 自來 水 供水 計畫   包含 草屯   鳥 嘴潭 兩座 淨水場   10 公里 原水 導 水管 工程 已 完工   總長 85 公里 送 水管   聯絡管 工程 已 完成 54 公里   草屯 淨水場 可供 應 草屯 鄰 近地 區 15 萬人 用水     王 瑞德 說   南投縣 集集 攔河堰   湖山 水庫   鳥 嘴潭 人工湖   都 是 供應 下游 彰化   雲林 使用   南投縣 民 配合 政府 政策   但 南投縣 偏鄉 沒有 自來 水   且 自來 水延長 管線 成本 高   南投縣 政府 每次 提 競爭 型 計畫 都 沒 被 選上   只能 開闢 簡易 自來 水   影響 鄉親 健康   希望 中央 能 重視 南投 自來 水管 線延管 工程   或 加大 簡易 自來 水補助   讓 南投 鄉親 能 喝 到 量 好質 優 自來 水     陳 建仁 說   北從 翡翠 水庫   石門 水庫 一路下 來   這些 水庫 形成 一粒 粒   珍珠 串     讓 台灣 水資源 調度 更好   顯示 台灣 人民 慈悲 善良   願意 彼此 幫忙   互相 援助   鳥 嘴潭 人工湖 除了 供應 民生 用水   會 持續 綠 美化   變成 南投 新 觀光 地標     立委 游顥 說   南投縣 水源 供應 彰化   雲林 地區 使用   但 行政院 對 南投 回饋 協助 不足   王 瑞德 副 縣長 當場 反映 自來 水 普及率 水管 汰 舊 換性   草屯 地區 東 八里 4800 戶水員供 應 不足   但 陳 院長 沒有 回應   他會 立法院 繼續 爭取   希望 行政院 重視 南投 用水 問題  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>22</v>
-      </c>
-      <c r="B25" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>22_灌區_水稻_灌溉_農田</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>['灌區', '水稻', '灌溉', '農田', '水利', '水源', '農業', '地面水', '農委會', '平方公里']</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>['雲林縣 高鐵 沿線 區域 近年 來 因為 地層下陷 嚴重   恐影響 高鐵行車 安全   農委會 從 2013 年 祭 出節 水獎勵 鼓勵 稻農 轉作   但 卻 從 去年 暫停 獎助   雲縣 府 為 了 鼓勵 稻農 轉作 減少 抽取 地下水   持續 向 中央 爭取 獲得 核定 復 辦   將在明   2023   年 起 恢 復 實施 節水 獎勵 措施   雲林 高鐵 沿線 地區 是 地層下陷 嚴重 區域   其中 雲林 土庫 段 一年 下陷 6.5 公分 最 嚴重   恐 危及 高鐵 安全   農委會 2013 年針 對雲縣 虎尾   土庫   元長 北港 高鐵 沿線 左右 1.5 公里   提出 節水 獎勵 鼓勵 稻農 轉作   但 卻 去年 暫停 辦理   雲林 農民 表示     只要 不是 種 水稻 類   其實 它 吸 水量 會 真的 會差 很多   這是 實在 話   雲林 這邊 就是 水稻 需求   地下水 需求量 是 最 多     為 了 鼓勵 高鐵 沿線 農民能 一期 稻 休耕 或 轉作 低耗 水性 作物   雲縣 府 持續 向 中央 爭取 復 辦獎勵 補助 近期 通過 核定   除了 領取 綠色 獎勵 金外   還能 領轉 作金 3 萬元 或 生產 環境 維護金 4 萬 2 至 5 萬 2 不 等   雲林縣 農業 處 副 處長 蔡耿宇 指出     高鐵 沿線 周邊 1.5 公里 它針 對 綠肥 部分   原本 是 大概 每公頃   補助   4 萬 5   這次會 加碼   如果 一期 作去 推動 話 可以 加碼 4 萬 2000 元   所以 一公頃 可以 領到 8 萬 7000 元     雲林 農民 指出     成本 還有 包括 肥料   噴灑 農藥 至少 都 要 花 2 萬元 成本 超過     當地 農民 表示   面對 近期 人工   肥料 成本 提高   若 獎勵 補助 增加 會 讓 農民 提高 轉作 意願   而 農業 處 說   縣內 高鐵 沿線 四鄉鎮 農地 大約 4 千公頃   希望 能 透過 推動 農地 轉旱 作物 獎勵   3 年 達 到 稻作 1700 公頃 轉出 目標  ', '根據 水利 署 監測 資料   雲林縣 水稻 最大 種植 地區 大 埤 鄉   近 5 年 地層下陷 面積 與 深度 惡化 現象   為 了 避免 極端 氣候 造成 水情 吃緊   地層下陷 持續   雲縣 府 建議 引 北港溪 水源   新建 給 水管 路供 應 灌溉   經費 約 3.3 億餘元   並提報 中央 等待 核准 辦理 中   2 期稻 收割 後 農民忙 著 整地   雲林 大 埤 鄉 是 雲林 種植 水稻 面積 最大 地區   但 卻 時常 面臨 灌溉 水源 不足 問題   當地 農民 就 說   為 灌溉 農田田區 同時 要 用 2 至 3 口井 放水   才能 夠來 因應   雲林 大 埤 鄉 農民 表示     就是 都 沒 水   如果 有人 耕田 廣一點   就 用 大 井水   比較 深層   我 這個 都 是 小 井水   就 很 難 去 灌溉   有時 要 放水 1 天 1 夜 才能 全部 都 讓 水覆蓋     雲縣 府 表示   根據 水利 署 監測 資料   大 埤 鄉 下陷 面積 深度 持續 擴大   主要 就是 因為 農田 水利 事業 區域 灌溉 系統 末端 或區 外   包括 北鎮   西鎮 怡然 等 村   若 要 一年 兩作 無水 可 灌溉   一定 要 抽取 地下水 使用   雲縣 府 水利 處處長 許 宏博 表示     非灌區 地方   去 想 辦法 怎麼 用 地面 水源 來 補充   我們 研究 是 以 大 埤 附近 北港溪   去 引 北港溪 水源   作為 1 期 稻作 灌溉 水源     雲縣 府 水利 處 表示   為 改善 大 埤 鄉 地層下陷 惡化 問題   縣府 完成 大 埤 非 灌區 灌溉 水源 改善 工程 前期 規劃   希望 引 北港溪 地面水 到 高灘 地 設置 調 蓄水池 等   供給 農田 灌溉 使用   但 概估 工程 經費 約 3.3 億   目前 已經報 請 中央 等待 核定 中  ', '經濟部 水利 署 監測 雲林縣 地層下陷   去年 雲林 顯著 下陷 面積 247.7 平方公里   較 前年 略增   全 台面 積 最大 稻作 鄉鎮 大 埤 鄉 因 部分 地區 非 灌區   僅能 抽取 地下水   近年 下陷 面積 逐漸 擴大   縣府 提出 大 埤 鄉 非 灌區 灌溉 水源 改善 工程   提報 中央 爭取 專案 經費   並建請 農田 水利 署將 該區 納入 擴大 灌溉 服務範圍       根據 水利 署 監測 資料 顯示   雲林縣 去年 顯著 下陷 面積 為 247.7 平方公里   較 前年 239.5 公里 增加   年 下陷 速度 約 7 公分   土庫 及元長 水位 仍有 持續 下降 趨勢   枯水期 間 各 監測 站 地下水位 最大 洩降 約 4 至 15 公尺   其中 又 以 大 埤 監測 站 洩降 15 公尺 最 嚴重   為 雲林縣 近年 地層下陷 顯著 農業 重點 鄉鎮                             縣府 水利 處長 許 宏博 表示   過去 雲林縣 地層下陷 以高鐵 沿線 虎尾   土庫   元長 北港 較 為 嚴重   但 近年 大 埤 鄉 地層下陷 惡化 趨勢   主因 為 大 埤 鄉 為 全台 稻作 面積 最大 鄉鎮   種植 面積 逾 5 千公頃   但 部分 地區 非 灌區   需仰賴 地表水 或 抽取 地下水 灌溉   導致 近 5 年 地層下陷 面積 深度 都 惡化       為 改善 地層下陷   縣府 已針 對 該 區域 取水 灌溉 進行 初步 規畫   擬在 北港溪 高灘 地 設置 調蓄 池及 臨時性 滯水 設施   透過 貯蓄 北港溪 水源   新建 給 水管 路供 給非 灌區 農田 使用   經費 約 3.32 億元   將向 中央 提報   並建議 農業部 農田 水利 署 擴大非 灌區 灌溉 服務範圍       雲林縣 長 張麗善 說   極端 氣候 越來 越 嚴峻   地面水 資源 無法 支持 產業 所 需   農田 水利 署 如 未能 綜合 考量 水資源 供 應量   農民因 耕作 生計 所 需   勢必 尋求 抽取 地下水 因應   導致 地層下陷 問題   對 於 行經 高鐵行車 安全 亦 可能 造成 嚴重 威脅       許 宏博 表示   針對 高鐵 沿線 虎尾   土庫   元長 北港 四鄉鎮 地區   縣府 將持續 加強 查察 水井 用水 情形   並檢討 與 研議 增設 調蓄 設施   增供 地表水   以 限制 溉 地下水 抽取   自來 水可到 達 水井 將 逐年 核減 水權   以 減少 地下水 抽取 造成 地層下陷   雲林縣 大 埤 鄉 為 全 台面 積 最大 稻作 鄉鎮   因 部分 地區 非 灌區   僅能 抽取 地下水   近年 地層下陷 面積 逐漸 擴大   記者 陳 雅玲 ／ 攝影']</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>23</v>
-      </c>
-      <c r="B26" t="n">
-        <v>3</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>23_北極_冰河_坑洞_大陸</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>['北極', '冰河', '坑洞', '大陸', '平方公里', '坑', '冬季', '全球', '土', '區域']</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>['地球 南北 兩極 這兩天 都 重要 科學 發現 發表 媒體 上   其中 北極 方面   科學家 發現 加拿大 北邊 海底 出現 地層下陷   最大 坑洞 長 200 公尺   寬 74 公尺   深度 達 24 公尺   而 南極 方面   向 來 被 認為 氣溫 較 低   冰層 較 穩定 南極 大陸 東邊   3 月初 到 3 月 中 發生 冰河 快速 消退   導致 面積 144 平方公里 冰架 崩解   相當 於 半個 台北市 大小   科學家 藉 著美國 太空 總署 NASA 衛星   拍 攝到 南極 大陸 東邊   格連澤 冰河     瀕臨 南 印度洋 冰架   2 月底 還狀況 良好   但 3 月初 到 3 月 中 卻 開始 快速 消退   崩解   令科學家 相當 憂心   南極 過去數 十年 來   冰架 崩解 現象   絕 大多 數出現 西邊 南極 半島   就是 與 南美洲 阿根廷 遙遙 相望 所在   而且 過去 冰架 崩解 面積 與 規模 相 對 較 小   同時當 南半球 冬季 來臨   南極 冰雪 增厚   對 全球 海平面 衝擊 有限   從 2020 年 開始 南極 東邊 冰河 開始 縮小面積   但 是 以 每天 1 平方公里 速度 減少   被 認為 是 自然 現象   直到 3 月初 情況 開始 了 改變   美國伍 茲 霍爾 海洋 研究所 研究 員凱瑟琳 沃克 表示   過去 發生 算是 相當 緩慢 變化   原因 包括 海洋 暖化 與 冰 河流 動   凱瑟琳 沃克 指出     但 上星期 我們 發現 快速 氣候 現象   這也許 不足以 說明 事情 全貌   但 確對 冰架 造成 前 所 未 見 壓力     研究 人員 所 說 氣候 現象   是 指 發生 3 月 15 日 大氣 河流   這種 氣候 現 象是 指   高濃度 水蒸 氣沿 著 狹窄 區域 快速 前進   對 於 已經 消退 中 冰架 造成 致命 一擊   而大面積 冰架 崩解 進而 消失   科學家 擔心 未來 海平面 將明顯 上升   另外   美國 蒙特 瑞爾灣 海洋 研究所 加拿大 北邊 北極 海域   發現 大面積 地層下陷   最大 坑洞 長 約 220 公尺   寬 74 公尺   深度 達 24 公尺   研究 團隊 懷疑   除了 氣候 暖化   溫度 上升 地下水 緩慢 流動   是 北極海 地層下陷 原因  ', '路透 報導   一段 無人機 影片 揭露 巴塔 蓋卡 坑洞   Batagaika   crater   近況   這道 長 1 公里 塌陷 區域 位 於 俄羅斯遠 東地區   是 世上 最大 永凍土 巨坑   俄羅斯薩哈 共和 國的 當地 人稱 之 為   地獄 之門         影片 中   兩名 探險者 爬過 巨坑 底部 凹凸不平 地形   這種 高低 起伏 地表 1960 年代 周圍 森林 整地 後 開始 形成   因 地下 永凍土 融化 導致 地層下陷                             當地 居民 兼 探險 家史 特魯奇 科夫   Erel   Struchkov   表示     當地 人稱 之 為 塌陷   1970 年代 形成   最初 是 條溝 壑   然後在 晴天 高溫 下 解凍   開始 擴大         科學家 說   俄國暖化 速度 比 世界 其他 地區 至少 快 2.5 倍   占 俄國國 土面 積達 65% 苔原 因此 融化   釋出 溫室 氣體       位 於 亞庫 次克 梅爾 尼科夫 永凍土 研究所 首席 研究 員尼塔納 納耶夫   Nikita   Tananayev   表示   雖然 這 可能 吸引 遊客   但 坑洞 擴大是   危險訊號       今 後   隨著 氣溫 升高 人 為 壓力 增加   我們將 看到 越來 越 多 這種 巨型 塌陷 形成   直到 所有 永凍土 都 消失 為止         永凍土 融化 已威脅 到 俄國 北部 與 東 北部 城鎮   導致 道路 坍塌   房屋 崩裂   管線 中斷   最近 幾季 愈演愈烈 大規模 野火 使 問題 更加 嚴重       薩哈 共和 國當 地人 注意 到 巨坑 迅速 擴大   史特魯奇 科夫 說       兩 年前   巨坑 邊緣   距離 這條 小路 大約 20 到 30 公尺   現在 它 顯然 離 我們 更 近 了         科學家 不 確定 巴塔 蓋卡 坑洞 擴大 確切 速度   但是 塔納納 耶夫 說   巨坑 下面 土地   有些 地方 深約 100 公尺   含有   大量   有機 碳   隨著永凍 土 融化   這些 機碳 將釋 放到 大氣 中   加劇 全球 暖化     隨著 氣溫 升高   我們 可以 預計   巨坑   將以 更 快 速度 擴大   這將 導致 未來 幾年 氣候 更加 暖化             路透 報導   一段 無人機 影片 揭露 巴塔 蓋卡 坑洞 近況   這道 長 1 公里 塌陷 區域 位 於 俄羅斯遠 東地區   是 世上 最大 永凍土 巨坑   俄羅斯薩哈 共和 國的 當地 人稱 之 為   地獄 之門     路透', '俄羅斯遠 東薩哈 共和 國有 一個 全球 最大 永凍土 塌陷 坑   當地 人 把 它 稱作   冥界 之門     隨著 全球 暖化 加劇   這個 巨型 天坑 正持續 擴大   科學家 警告   永凍土 融化 會 把 更 多 機碳釋 放到 大氣 中   讓 溫室 效應 跟 全球 暖化 加劇   俄羅斯遠 東薩哈 共和 國境   巴塔 蓋卡大融 洞     是 全世界 最大 永凍土 塌陷 坑   當地 人 把 它 稱作   冥界 之門     當地 居民 斯特 魯奇 科夫 表示     這是 1970 年代 形成   最初 是 條溝 壑   然後在 晴天 高溫 下 解凍 開始 擴大     當地 1960 年代 開始 砍伐森林   造成 地下 永凍土 融化   進而導致 地層下陷   氣候 暖化 更 加速 永凍土 流失   讓 融洞 越來 越大   梅爾 尼科夫 永凍土 研究所 首席 研究 員尼塔納 納耶夫 指出     這是 個 危險 跡象   因為 這是 高氣溫   氣候 暖化 跟 人 為 活動 壓力 造成   我們 會 看到 愈來 愈 多 這種 巨大 融洞 形成   直到 所有 永凍土 都 消失     更 糟糕 是   隨著永凍 土 消失   封存 裡頭 機碳會 被釋 放到 大氣 中   加劇 全球 暖化   塔納納 耶夫 表示     永凍 土內 碳 存量 是 大氣 中 兩倍   它將 漸漸 被 釋出 跟 大氣 接觸 後 被 細菌 攝取   導致 更 高 甲烷 跟 二氧化碳 排放   加速 溫室 效應     科學家 說   俄國國 土有 六成 五 都 是 苔原   當地 暖化 速度 比 世界 其他 地方 快 2.5 倍 以上   永凍土 融化 已經 俄國 北部 與 東 北部 許多 城鎮   造成 道路 坍塌   房屋 崩裂 並阻礙 管線 運作   對民眾 生活 構成 威脅  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>24</v>
-      </c>
-      <c r="B27" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>24_綠電_電業_種電_光電場</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>['綠電', '電業', '種電', '光電場', '綠能', '光電', '環境', '全台', '地層下陷區', '光電板']</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>['原來 同一 個 新能源 市場   同時 這麼 多 幫人 市場 上 探索   開發     圖片 來源 ／ Pixabay  ', '從國道 三號 林邊 交流 道 下來   光電場 廣告 映入 眼簾   從大馬 路旁 到 鄉間 農田   光電板 無 所 不   這是 屏東 沿海 地區 這幾年 興起 違 景致   是 全台 種電 縮影   地 青農批 政府   業者 聯手 種電 種到 失心 瘋   從 農地   山區 到 文資 價值 二戰 遺跡 都 不放過   不僅家園 變貌   迫使 老農離 農   變相迫 遷青農       屏東 農地 種光 電原 是 全台 濫觴 典範   二 九年 八月 莫 拉克 風災 挾帶 破紀錄 雨量   造成 中南部 嚴 重水 災   重創 屏東 南部 沿海 鄉鎮   不少 魚塭   果園 被 沖 毀   時任 屏東縣 長 曹啟 鴻 提出   養水 種電   計畫   縣府 媒合 魚塭   農地 租給 光電業者   地主 負責 管理   地主 按 月 收 地租 管理 費   綠電賣給 台電   能 涵養 地下水   減緩 下陷   一舉 數得                           屏東 種電   侵蝕 農地   製 表 ／ 都 會 地方 中心   農業部 前身 農委會 二 一 三年 修法   允許 不適 耕作 農地 種電   大開 種電 之門   但 農地 非農用 罵 聲不斷   二 一 八年 十月 起   屏縣 府 公告 實施   嚴重 地層下陷地區 土地 活化 暨 太陽光 電發 電業 整體 規劃 發展 計畫     開放 下陷區 農地 可 變更 種電       二 二 年 七月   農委會 加嚴 農地 變更 種電 門檻   二到卅公頃 農地 變更 要 由 中央 審查   兩公頃 以下 原則 不 同意 變更 種電   但 早 二 一 八年 屏東縣 長 潘孟安任   報請 行政院 同意 把 東港   林邊   佳冬   枋寮 四鄉鎮   畫為 嚴重 地層下陷區 作光電 專區   成為 特例       四年 多來   屏東 種電 發展 快速   原本 立意 良善 光電   如今 變成 農民 陰霾   枋寮 女青農 張靜玉 說   為衝 高綠電 占 比   種電 已種 到 失心 瘋   不該 種電 地方 都 被 光電板 占領   很多 農民 被 業者 遊說簽   不利 耕作 聲明書     離農 坐收 光電場 租金   但 這些 農地 都種 著蓮霧   水稻   芭樂   何來 不利 耕作         沿海 四鄉 鎮美麗 鄉間 景致 丕 變   綠地 逐漸 蒸發     屏東縣 環境 保護 聯盟 理事 長 洪輝祥 說   綠地   果園 被 一塊 塊 光電板 取代   像 貼 狗皮 膏藥般 醜陋   不但 壓縮 農業 空間   光電板 遮陽 廿年   農地 將 失去 地 力   衝擊 農產業 服務鏈   受益 是 少數 地主   受影響 是 多數 農民   整體 農業將 衰退   屆 時 想 回頭 搶 救 就 難 了       屏東縣 府 綠能 辦 公室 表示   沿海 四鄉 鎮持續 下陷   列 第一   二級 地下水 管制 區   縣府 把 四 鄉鎮 部分 農地 轉作光 電場   搭配 上游 補注 地下水   減緩 地層下陷   創造 地主   業者   政府   全民 與 綠能   五贏     前年 已達成 綠電供 應 全縣 民生 用電 階段 性 目標  ', '光電亂象 已久   從 之前 良田 種電   砍樹 種電   近來 變本 加厲   光電板 不僅 征服 山頭   占 領有 文資 價值 遺跡   更 一步步 裂解 農漁村 產業 鏈   恐阻斷 青農返 鄉 之路   地面 型 光電 社會 衝擊 比 預期 更大且 深   講求 氣候 正義和   企業 Ｅ Ｓ Ｇ   環境 保護   社會責任   公司 治理     國際 主流 下   政府 企業須 警覺   若綠電來 自迫 遷   危害 生態 與 地產業   恐埋 隱憂       屏東縣 沿海 四鄉鎮 被 縣府 以 嚴重 地層下陷區 之名 畫為 光電 專區   本可 接軌 屏東縣 前縣 長 曹啟 鴻   養水 種電   政策   但 實際 推行 結果   鄉間 景觀 破碎   光電場 蛇 鼠 為 患   離農者 漸增 等 負面 效應 逐漸 浮現   加上 光電助 漲 農地 租金   無異將 返鄉 青年 拒 於 農漁村 之外   被 批評 與   養水 種電   初衷 漸行 漸遠                             屏東 只是 全 台 種電 爭議 縮影   更 多 生態   景觀 敏感 地   追 趕綠能 目標 下 可割 可棄   面對 爭議 與 衝擊   政策 把關 工具 遲未 發揮 效能   及早 阻止 種電 副作用   甚至 正向 引導 與 地 共生 共榮   實難辭 其咎   與 執政黨   愛鄉 土   理念 背道 而 馳       開發行 為 必須 堅守 環境 正義底 線   綠能 不 例外   猶記 得 台積 電在 被 徵收 用地 拆 遷戶 激烈 抗爭 下   突然 宣布 放棄 進 駐龍科 三期   不無環境 正義與 企業 Ｅ Ｓ Ｇ 考慮   民進 黨 種電 國策 若 如   失速 列車     無情 地衝 撞 純樸 農漁村   把 青農   老農 都 當成   農村 最軟 一塊     這種 綠電 還是 國際 認可   符合 Ｅ Ｓ Ｇ 綠電  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>25</v>
-      </c>
-      <c r="B28" t="n">
-        <v>3</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>25_坑洞_建管處_破洞_地下</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>['坑洞', '建管處', '破洞', '地下', '台北市', '巷道', '信義區', '街', '坍陷', '道路']</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>['台北市 信義區 一處 新建 工地 旁 道路 地層下陷   崇德 街 60 巷 路面 今天下午 3 點 13 分出 現長 15 公尺   寬 3 公尺   約 2 至 3 公尺 深 大 天坑   台北市 建管處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   目前 了解 是 連續 壁 滲水   工地 正在 止水 當中   消防局 現場 協助 鄰 房民眾 疏散   台北市 建管處 表示   該案 因連續 壁施作   已 派員至 現場 了解 處理 中   工地 正在 止水 當中   圖 ／ 讀者 提供 台北市 信義區 一處 新建 工地 旁 道路 地層下陷   崇德 街 60 巷 路面 出現 大 天坑   圖 ／ 讀者 提供', '〔 記者 楊 心慧 ／ 台北 報導 〕 台北市 信義區 崇德 街 60 巷華熊 營造 建案 工地 旁 巷道   昨   13   日 下午 發生 地層下陷   出現 長 15 公尺   寬 3 公尺   深 3 公尺 巨大 坑洞   昨晚 灌漿 填補 坑洞 與 建案 基地   坑洞 初步 填平 完成   但 目前 為將 土水壓 平衡   仍 基地 內持續 灌水   台北市 都 發局 長 王玉芬 今   14   日 上午 說明   灌水 作業 預計 今 下午 完成   至於 住戶 回家 需達 3 條件   估計 作業 需 1 至 2 週     王玉芬 今 上午 抵達 現場 說明 進度   並 表示 造成 道路 塌陷 初步 判斷 是 工地 地下 連續 壁 約 11   12 公尺 處有 破洞   造成 水 與 砂往 工地 內流   產生 破洞 原因   疑似 為 連續 壁 施工 時有 包土 狀況   目前 已 坑洞 進行 灌漿 回填   基地 內則 採填砂 灌水 以 平衡 水壓     至於 安置 在外 住戶   王玉芬 指出   住戶 回到 家 需有 3 個 條件   包含 透過 雷達 探測 檢查 無 孔洞 或 軟弱 土層   監測 建築物 無 傾斜   由 專業 技術 人員 進入 屋內 檢查 無 毀損 或 裂縫   預計 時間 需 1 至 2 週   希望 可盡 早 完成   讓 住戶 回到 家園   安置 費用則 由 廠商 全部 負擔     針對 現場 作業 進度   王玉芬 說   目前 基地 水位 地下 5.5 公尺   大約 下午 會 灌到 地下 3 公尺   雖然 昨晚 已 初步 判斷   狀況 趨 於 穩定   但 北市 府 要求 持續 灌水 至 地下 3 公尺 處   預計 灌水 作業 今 下午 可 完成     台北市 信義區 長 陳 冠伶今 受訪 表示   調查 結果 撤出 有七戶   需要 安置 住戶 一共 5 戶 10 人   目前 都 安置 信義區 旅館   按照 規定 發生 緊急 災害 補助 可 申請 安置 補助   每人 一天 1600 元   最多 可 申請 七天   超過 部分   廠 商承諾 超出 部分 可 負擔  ', '首次 上稿   00   04 更新 時間   06   09   〔 記者 蔡亞樺 ／ 台北 報導 〕 台北市 信義區 崇德 街 60 巷一處 華熊 營造 建案 工地 旁 巷道   13 日 下午 3 點多 發生 地層下陷   出現 長 15 公尺   寬 3 公尺   深 3 公尺 巨大 坑洞   台北市 政府 與 建 商展 開搶 救   灌漿 填補 坑洞 與 建案 基地   晚間 11 點 坑洞 初步 填平 完成   北市 府 啟動 預防性 疏散   疏散 安置 11 名住 戶到 旅館 住宿     台北市 建管處 指出   崇德 街 60 巷華熊 營造 建築 工地 旁發生 道路 坍陷   建管處 收到 訊息 立刻 派員 現場 了解   工地 正 進行 地下室 開挖   因連續 壁體 滲水 造成 地下水 湧入 引發 道路 坍陷   立即 指揮 承造 人 進行 緊急 處置   要求 基地 外 道路 下陷 處 進行 灌漿 回填   基地 內採 填砂 灌水 以 平衡 水壓   至 13 日 晚間 11 點 道路 下陷 處 已 初步 填補 完成   趨 於 穩定   基地 仍 監督持續 進行 填砂 灌漿     台北市 建管處 長 虞 積學 表示   經 建管處 緊急 聯 繫   台北市 土木 技師 公會莊 理事 長 結構 技師 公會 徐 理事 長   均 第一 時間 趕 現場 協助 緊急 處置 事宜 確認 疏散 範圍   目前 採預 防性 疏散 措施   疏散 12   24 號計 5 戶 需 安置 11 名住 戶   均 已 安排 至 旅館 住宿     虞積學 強調   該 建案 違反   建築法   部分 現場 已 立即 勒令停工   並處 以 18 萬元罰 鍰   建管處 將持續 現場 指揮 搶 救   現場 並已 要求 承商 加強 設置 周遭 鄰房 安全 觀測   提高 觀測 頻率   直到 確認 安全 無虞   該 工地 目前 已 勒令停工   後 續須 確認 週邊 地質 鄰房 安全 無虞   並檢具 改善 計畫 經相關 公會 審 查核 可 後   始得 復工  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>26</v>
-      </c>
-      <c r="B29" t="n">
-        <v>3</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>26_萬華區_台北市_新竹_新北</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>['萬華區', '台北市', '新竹', '新北', '台北', '向', '〔', '〕', '鄰', '建路']</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>['〔 記者 吳昇儒 ／ 新北 報導 〕 受   尼莎   颱 風共伴 效應 影響   新北市 汐止 地區 降下 豪 大雨   不 只 發生 土石 流   就 連工 建路 出現 地層下陷 情形   工務人員 初步 搶 修後工 建路 一度 恢 復 通行   但 昨日 夜間 卻 發現 地基 仍須 補強   必須 再次 施工   警方 獲報 後   立刻 派員 前往 進行 交通管制   全線 封閉 該 路段   為 加快 搶救 速度   警方 還 徒手 協助 搬運 30 多輛 機車   讓 工程 能 順利 進行     汐止 區工 建路 地層下陷 後   經工務 人員 搶 救   暫時將 凹陷 地基 填補 起來   未料 這兩天 又 因受 豪雨 影響   再此 下陷   汐止 警 分局 接獲 通報 後   即刻 拉起 封鎖線   並連夜 將規劃 好 改 道路 線 公告 各 臉書 地方 集團 供民眾 參考     深夜 中   員警手 拿 指揮棒   持續 管制 車流   柏油路 面上 出現 許多道 裂痕   除了 用 交通 錐 警示 阻擋   立起 告示牌   請行經 車輛 改道 行駛   經過 徹夜 管制 後   施工 單位 評估 現場 完畢 於 今早 6 點準備 開工   卻 發現 許多 機車 車主未 依 通知 移置 車輛   造成 施工 路段 周圍 停滿 機車   負責 交通管制 社后 派出所 2 名員警   見狀 趕緊 上前 幫忙   短短 10 幾分鐘 就 徒手 移 了 3   40 台機車   讓 搶 救 工程 得以 順利 進行     新北 市長 侯友宜 上午 特別 到工 建路 了解 現場 狀況   並感謝 汐止 警 分局   區 公所 施工 單位   連夜 辛苦 進行 管制 勘查   並 指示 相關 單位務 必 儘 速 完成 搶修 並維持 交通 順暢   全力 協助民眾 解決 問題     民進 黨籍 市議員 張錦豪 請 助理 前往 工 建路 現場   向 周邊 住戶 詢問 是否 需要 協助 之處   並與 施工 單位 保持 聯 繫   希望 能 早日 恢 復 正常 通行  ', '〔 記者 黃 美珠 ／ 新竹 報導 〕 新竹縣 竹 北市 房市 熱絡   集合 式 住宅 大樓 如雨後春 筍般 不斷 冒出   然而 今天 竹北 勝利 15 街 卻 傳出 某 集合 式 住宅 大樓 工地   疑似 開挖 地下室 後 導致 隔鄰 一戶 鐘姓 民宅 地基 下陷   牆面 牆角 龜裂 等   屋主 向 北興里長 田慶 順陳情   擔憂 價值 數千萬 透天 厝 會 不會 一夕 傾倒 危險   希望 相關 單位 幫忙 出面 解決     被 指控 工地 陳 姓 現場 負責人 說   經實 勘 發現   該 民宅 應該 之前 就 原因 不明 下陷   龜裂 問題   看起 來 災害 確實 持續 進行 中   但導致 持續 龜裂 擴大 原因 有待 鑑定 釐 清   但基 於 敦親 睦 鄰   他 允諾會 天氣 放晴 後 協助 維修 處理     陳 講   鍾 姓 住戶 主要 是 拿 自家 建物 背 後 另 1 間 民宅 比 對   鍾 認為 2 宅   沒有 一直 線     所以 認定 傾斜   但 他 實勘 評估 鍾 宅 並無傾 斜 之 虞   不過 未來 他們 施工 會 再 注意 加強 整體 安全 維護     縣府 工務處 長江 良淵 說   鄉親 若 發現 自宅 可能 因 他人 施工 導致 毀損 疑慮 時   可以 向 該 處建 管科 陳 情   由 他們 立案 追 蹤   同時 可 要求 工地 原設 計建築師 或 技師 到場 無 立即 性 危險 判斷   因為 一般 工地 開工前 都 會針 對 緊鄰 建物 現況 鑑定   就是 供 一旦 發生 鄰 損爭 議時 比 對 參考     北興里長 田慶順 說   鍾 姓 住 戶 是 縣治 3 期 被 徵收 戶   3 樓半 住家 就是 蓋 約 3   40 坪 配回 地上   10 年前 要蓋 這樣 透天 厝 少 說 要 1000 萬   現在 當地 房價 被 建商 炒作 到 每坪 80 萬   以現 新建 工程款 每坪 約 15 萬元 等 換算   鍾 宅少 說 4   5000 萬   由 於 鍾 家 1 家 5   6 口人 就 住 其中   如果 房子 真的 不安   影響 非常 大     鍾 說   隔鄰 新建 工地 約 是 2 個 多月 前開 挖 地下室   不久 後 他 就察覺 自宅 車庫 原本 平整 地面   竟 自己 車位 處 開始 出現 下陷   一旁 區隔 鄰宅 用 牆面 了 龜裂 狀況   牆角 跟 地面 磁磚 裂開   且 前述 下陷 裂縫 都 不斷 加大     田慶 順聞言 實際 測量   發現 鍾 宅 車位 下陷 處 最高 已有 他 1 片 手指甲 寬   至於 牆角 地面 磁磚裂 縫 最大 可以 塞下 2 根竹 筷子   確實 讓 人 擔憂  ', '〔 記者 蔡思培 ／ 台北 報導 〕 台北市 近來 天坑 事件 頻傳   萬華區 一處 建案 工地 旁 道路 日前 發生 地層下陷   坑洞 面積 約 一輛 汽車 車身   所幸 無人 受傷   不過當 地里 長 蔡岳樺 表示   工地 已 二度 出包   天坑 修補 後 又 出現 積水   北市 議員 應曉薇 質疑   建案 若 未 側溝   未來 仍 可能 天坑 事件   台北市 建管處 表示   會 要求 將 排水 系統 完   已將個 案列 為 重點 稽查 個案     應曉薇 今天 與 多位 萬華里 長 前往 萬華 工地 會勘   應曉薇 質疑 建案 是否 側溝   若側 溝都 沒有   未來 仍 可能 天坑   若 再有 大雨   台北市 衛工處 又 要 幫忙 清砂   發現   坑洞 日前 雖已 填補   但現 又 出現 積水   對 於 台北市 副 市長 李 四川 認為 路 塌 與 極端 氣候 溫室 效應 有關   她則 稱 這 就是 沒有 側溝 造成 人 為 疏失     蔡岳樺 說   福音 里 3 個 工程   每次 都 是 這個 建案 出事   他 對 於 都市 更新 樂觀 其成   但 不 希望 影響民眾 安全   他 呼籲 建商 出事 要 負責   不要 什麼 就 推給 別人   蔡 表示   天坑 意外 當天 建案 負責人 推 託 說 下雨   地基 掏空   又 說 沒 危險 沒什麼   讓 他 相當 憤怒   難道 要 出事 才 算 問題   呼籲 建商要 把 事情 做好     萬華區 全 德里 里長 趙 素美 認為   這個 問題 應該 可以 提前 處理   不能 發生 事情 才 處理   里長 都 為 里 民保護 身家 財產   建商 與 里 長 應該 互相 尊重     建管處 表示   此 都 更案 採用 是 舊 法令   本案 涉有 公有   私有土地   法令 上不會 要求 現在 就 按照 使用 執照 竣工 時 排水 系統 完   但 目前 排水 系統 不 完整 才 導致 大雨 後 排水 不順 地基 下陷   現行 法令 對 於 打通 道路   區域 排水 沒 規範   但 建管處 會 要求 將 排水 系統 完   改善 區域 排水     建管處 說   已將 此案 列為 重點 稽查 個案   未來會 加強 稽查   目前 坑洞 已 填好   初步 安全 無虞   並將 安全 疑慮 地方 阻隔  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>27</v>
-      </c>
-      <c r="B30" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>27_新竹市_台北市_坑洞_坑中</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>['新竹市', '台北市', '坑洞', '坑中', '街', '信義區', '消防局', '市府', '道路', '鄰近']</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>['先前 才 發生 竹北 天坑 事件   新竹市 和平路 20 巷今   21   天 下午 突然 出現 天坑   大約 一輛車 面積   根據 了解   天坑 旁有 一個 建案   目前 已經 挖 到 地下 三樓   新竹市 府 說明   今日 下午 13 時 35 分許   消防局 受理 和平路 出現 道路 地基 下陷 情形   消防局 派員到 場後發現 道路 明顯 傾斜   並伴 隨 瓦斯 異味   隨即 通報 都 發處   工務處   自來 水 公司   瓦斯 公司 等 單位 前來 搶 修及 勘查   市長 高虹安 隨後也親 自到 場關 心及 了解 狀況   聆 聽 周邊民眾 心聲   要求 廠商必 須 儘 速 完成 改善   並確 保 居民 居住 安全   市府 指出   現場 工地 依規 有施 打 預壘 樁 擋 水樁   工法 沒有 問題   疑似 是 基地 內側 開 挖 後   造成 基地 外側 道路 內部 土壤 位移   連帶 造成 自來 水管 線 破裂   沖 刷 土壤 泥沙 後 再 造成 地層下陷   瓦斯 管線 破裂   市府 已 要求 建商 改善 期間 每日 需以 儀器 監測 周邊 民宅 無 傾斜 情形   如 民宅 開始 傾斜 情形   應 進行 預防性 撤離   另 已確 認自來 水破管 位置   並 完成 修 復 回填   將持續 觀察 是否 還有 造成 洩漏 情形   避免 地層 再次 下陷   市府 進 一步 指出   本案 因違 反建築法 第 63 條   都 發處 依建築法 89 條 勒令停工   並針 對 起造 人   承造 人   監造 人先 進行 裁罰 各三萬元   並視後續 情況 再行 論處  ', '台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶   並劃 設緊 戒線   並 通知 府 相關 單位 到場 處理   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   記者 廖炳棋 翻攝 台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   緊急 救援 住戶   圖 ／ 讀者 提供', '台北市 出現 天坑   今天下午 15 時許   台北市 信義區 崇德 街 60 巷 22 號 附近   一處 新建 工地 旁 道路 地層下陷   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   目視 可 看到 機車   自行 車 陷落 坑中   同時 坑洞 波及 一旁 民宅 地基   目前 台北市 消防局 已經 疏散 鄰近 住戶 10 多人   並劃 設緊 戒線   並 通知 市府 相關 單位 到場 處理       天坑 位 於 新建 工地 民宅 中間 巷弄 道路   塌陷 時 發出 聲響   驚動 住戶   但 因為 坑洞 擋 在家 門前   第一 時間 無法 脫困   消防局 緊急 到場   以 爬梯 方式 救援 住戶 出來                             消防局 救出 2 名 女子   疏散 1 男 1 女   人員 已 全數 疏散 完畢   另外 1 名 85 歲 老婦   因長 期行動 不便   雖無外傷   意識 清醒   但家屬 要求 預防性 送醫   由 消防局 送北醫   由 於 天坑 危及 安全   影響 周遭 至少 五戶 民宅   部分 住戶 無法 回家   估計 10 餘人受 影響   將由 台北市 府 處理 安置 問題       台北市 信義區 出現 天坑   目前 市府 新工處   建管處   勞檢處 等 相關 單位 都 已 派 人 到場   現場 設置 指揮 所   初步 懷疑 與 民宅 對面 新建 工地 工程 有關   現以 灌漿 方式 緊急 處置   至於 天坑 出現 原因   將 交由 市府 建管   新工 等 單位 調查   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝 台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 翻攝']</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>28</v>
-      </c>
-      <c r="B31" t="n">
-        <v>2</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>28_公園_步道_水路_坑洞</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>['公園', '步道', '水路', '坑洞', '廣場', '向區', '夯土', '環境', '園', '市府']</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>['嘉義市 35 座公園 是 國內 密度 最高   其中 20 座公園 廁所   曾 議員 勘察 指出 不少 照明 不足   設備 損壞 沒修   衛生 不佳 等 問題   市府 指出   爭取 經費 改善 逐步 翻新   今年 至今 完成 3 處   以往 漏積水 嚴重 番仔 溝公園 廁所   改建 後 光潔 明亮   具設 計感   未來 每年 持續 將老舊 公園 公廁 改善 更新       番仔 溝公園 公廁 已 10 多年   市府 接 獲陳情 反映 多次派 員維修   但 管線   設備 老舊   再 加上 地震   地層下陷 等   造成 漏積 水   尤其 是 男廁 問題 嚴重   去年 獲環 保署 補助 566 萬元   與 南興 公園   228 紀念 公園 共 3 處廁 所 於 今年 4 月底 改善 完工   5 月底 同步 開放                             番仔 溝公園 公廁 更新 男女 廁   無障礙 廁所   包括 廁具   隔間   燈光   造型 壁地磚 等 設備   尤是 無障礙 廁所升級 加入 親子 廁所 功能 設備   有兒 童馬桶   尿布 台   較 低 洗手台   功能 上 更 完善       市府 建設 處 表示   2019 年 起 向 環保署 申請   優質 公廁 美質 環境 推動 計畫   經費 補助   整修 文化   友忠   劉厝   中正   北社 尾及 宣信 公園 公廁   公廁 設施 損毀   潮濕 髒 臭 等 情形   都 修繕   清理   今年 還會針 對 嘉義 公園裡 公廁 陸續 整修   工程 採半半 施工   施工期 間   民眾 還能 使用 其他 公廁  ', '桃園市 蘆竹 區南興 水岸 遊憩 公園 耗資 1 億元 打造   完工 迄今 不到 4 年   近期 被 發現 步道 草 原因 地層下陷   出現 大大小小 坑洞   議員 批評 宛如 成 了   地 雷公 園     市府 工務局 表示   地層下陷 原因 可能 是 夯土 不夠 扎實   水路 沖 刷 造成   將 安排 會勘 改善       南興 水岸 遊憩 公園 2019 年 竣工   市府 特別 引進 共融式 設計   設置 樹屋   人文 廣場   森林 小徑   遊戲 沙坑   自行 車道 等   南 崁 住宅 密集 區營造   都 會 中 綠洲                               市議員 張桂綿 說   公園 步道 近期 嚴重 下陷   包括 法式 滾球區 兒童 奔跑 大 草原 出現 大小不一 坑洞   甚至 掏空 成   無底 洞     推測 是 鄰近 河川 水流 滲透導致 地層下陷 嚴重   土壤 幾乎 全都 流失         這裡 宛如 地雷 區     張桂綿 直言   如果 民眾 或 兒童 沒 注意   一不小心 可能 踩 空 受傷   已 向區 公所 反映   但 仍 無 解方   呼籲 市府 工務 單位 正視   盡速 拆除   地雷     還給 鄉親 安全 遊憩 環境       工務局 長 汪在宙 說   初判 可能 是 施工 時 夯土 不夠 扎實   附近 水流 滲透 加上 行人 重量 造成 壓力   導致 夯土 流失   地層下陷   市府 後 續會 協同 各 單位 現勘   了解 發生 原因 並盡速 改善 施工 缺失  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>29</v>
-      </c>
-      <c r="B32" t="n">
-        <v>2</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>29_新北市_萬里區_致建築物_投溫泉</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>['新北市', '萬里區', '致建築物', '投溫泉', '溫泉', '當地民眾', '地民眾', '公共', '俞肇福', '湯空間']</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>['萬里區 公 所以 訊息 說明   萬里 區加 投溫泉 公共 浴室 於 日據 時代 建造   歷史 悠久   屬 於 海底 溫泉   為 當地 居民 從小到 大泡 湯空間     區 公所 表示   因 2 月底 有民眾 反應 浴室 燈管   溫度 顯示器 不亮 等 問題   於 是 委 託 廠商 勘查 後 發現   疑似 地層下陷 現象   為確 保泡湯 安全   已 封閉 浴室     區長 黃 雱 勉 表示   為 瞭解 確切 原因   找出 有效 改善 方法   將邀 請 專業 技師 進行 檢查 評估   以商 討後續 改善 辦法   期望 安全 前提 下   儘 早 恢 復 提供 民眾 泡 湯空間   提醒 民眾 封閉 期間 勿 擅自 進入 使用   以維護 自身 安全     萬里區 公所 主任 秘書 許明富 向 中央社 記者 表示   當地過 去 地層下陷   並 完成 改善 多年   未影響 溫泉 供給 溫度   加投 溫泉 公共 浴室 經找 技師 以 透地雷達 探測 後   男女 湯室 地下 發現 土壤 流失 現象   未來將 進行 修繕 改善   並確 認無 危險 之 虞   才 會 再行 開放 供民眾 使用     編輯   林恕暉   1130326', '〔 記者 俞肇福 ／ 新北 報導 〕 日治 時代 建造 新北市 萬里 區加 投溫泉 公共 浴室   提供 大眾 免費 泡湯   不僅 受到 當地民眾 喜愛   就連 基隆 人 慕名 前來   日前 發現 疑似 地層下陷   萬里區 公所 立即 封閉 浴室   並邀 請 專業 技師 與 工程 廠商 勘查   將於 完成 改善 並確 認沒有 危險   才 會 重新 開放     新北市 議員 周雅玲 表示   接 獲當 地民眾 反映   加投 溫泉 公共 浴室 屋頂 漏水   排水 不良   牆面 出現 裂縫   廠商 會勘 後 懷疑 是 地層下陷   為確 保民 眾 安全   三月 四日 起先 封閉 浴室   經技師 以 透地雷達 探測   男女 湯室 地底下 發現 土壤 流失 現象     周雅玲 指出   萬 里加 投溫泉 公共 浴室 十多年 前 曾 經修繕   當時 出動 透地雷達 探測   這次 發現 問題 較 嚴重   建議 邀請 土木 技師 參 與 會勘   經濟 發展局 水利局 應針 對 附近 溫泉業者 開發 予以 總量 管制   以利 公共 浴室 永續 發展     萬里區 長 黃 雱 勉 表示   加投 溫泉 公共 浴室 經專業 技師 檢視   發現 下陷 致建築物 傾斜 情形   公所 將再 請 土木 技師 公會 等 專家 進行 檢查 評估   期望 確保 安全 前提 下   儘 早 恢 復 民 眾 泡 湯 空 間  ']</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>30</v>
-      </c>
-      <c r="B33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>30_坑洞_台北市_街巷_坍塌</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>['坑洞', '台北市', '街巷', '坍塌', '信義區', '塌陷', '路面', '小洞', '建管處', '混凝土']</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>['北市 信義區 崇德 街 60 巷 路面 今天下午 出現 大 天坑   坑洞 長 15 公尺   寬 3 公尺   深度 2 到 3 公尺   機車   單車 陷落 坑中   消防局 已 疏散 鄰近 住戶 10 多人   台北市 建管處 表示   路面 坍陷 處以 混凝土 處置   目前 已 勒令停工   將依建築法 開罰 營造廠   監造 人 各 9 萬元       台北市 建管處 表示   事發地 旁為 一處 新建 住宅 大樓 工地   疑似 施作 連續 壁 滲水   導致 道路 塌陷   目前 以 混凝土 處置   工地 現場 緊急 處理 中   將依建築法 第 89 條開罰 承造 人   營造廠     監造 人   建築師   各 9 萬元   目前 已 勒令停工   未來 把 一切 安全 問題 妥善 完成 後 才 會 復工   消防局 已協助 將住 戶 全部 撤離 完畢   人員均 安全   信義區 公所 正在 處理 安置 問題                             北市 議員 許淑華 表示   該處 昨晚 就 灌水   疑似 連續 壁施作 釀禍   事發地 鄰近 住戶 共 30 戶   12 戶住 坍塌 處 附近   約 10 人 安置 飯店   要求 市府 妥善 協助 住戶   台北市 崇德 街 出現 天坑   警消 緊急 疏散 民眾   記者 廖炳棋 ／ 翻攝 北市 信義區 出 現長 15 公尺 深 3 公尺   天坑     圖 ／ 北市 府 提供', '台北市 信義區 崇德 街巷 弄 13 日 下午 發生 路面 塌陷 事故   現場 緊鄰 一旁 建案 工地   中央社   台北市 信義區 一處 建案 旁 巷弄 今天下午 出現 長 15 公尺   深 3 公尺 坑洞   市府 表示   正在 持續 向 坑洞 灌漿   建案 基地 灌水   共 撤離 周遭 16 戶住 戶   其餘住 戶判斷 沒有 危險                           台北市 信義區 崇德 街巷 弄 今天下午 出現 一個 長 15 公尺   寬 3 公尺   深度 3 公尺 坑洞   道路 緊鄰 建築 基地 當時 正在 施作 連續 壁 工程   目前 已 停工 並 疏散 鄰近 住戶   副 市長 李 四川   工務局 長 黃 一平   都 發局 長 王玉芬 皆 到場 了解 狀況     王玉芬 向 中央社 記者 表示   坑洞 正在 持續 灌漿   建築 基地 則用 消防 車 灌水   讓 內外 壓力 平衡   阻止 繼續 塌陷   何時 才能 確認 沒 進 一步 危害 則要 持續 觀察     至於 住戶 部分   王玉芬 說   已經 撤離 16 戶   其中 10 人 需要 安置   這些 開銷 都 會 由 開發 單位 負責   其餘住 戶 雖 由 台北市 結構 技師 公會 判斷 沒有 危險   考量 住戶 仍會 擔心   已 請里長 逐戶 安撫     談到 事發 過程   附近 居民 仍然 餘悸 猶存   鄭 大哥 說   他 姊姊 大概 下午 2 時 50 分 時候 聽 到   砰   聲音   並 看到 門口 出現 一個 小洞   就 喊 他 出去 看   洞 這個 過程 中越 來 越 大   路上 腳踏車   摩托 車等 就 跟 著 掉下去     很 可怕       鄭 大哥 表示   他 住 這裡 3 年 多 了   旁邊 建案 大概 去年 開始 施工   剛開 挖 時候 路面 龜裂   建商 就 來 補好   之 後 雖然 施工 時 住家 總會 感到 地震   無法 睡 午覺   但 沒 什麼 異狀     黃 則說   他 住 這裡 20 多年 了   今天下午 外面 散步   走過 去 時 發現 一個 小洞   這個 洞後來 持續 陷 下去   但 他 沒 聽 到 什麼 聲音     新竹縣 竹北 莊敬 六街 一處 建案 周邊 日前 才 發生 路基 坍塌   導致 一輛 停放 路邊 特斯拉 轎車 直接 掉落  ']</t>
+          <t>['〔 記者 何玉華 ／ 台北 報導 〕 台北市 南港區 昨天 晚間 發生 道路 塌陷   經查 塌陷 原因 是 雨水 連 接管 脫管 造成   南港路 3 段 47 巷雙 向 封閉 施工   原 預計 今   19   晚 10 時 恢 復 通車   水利 處連夜 搶 修下   已 接續 完成 連 接管 脱管 處鋼 鈑 包覆   灌漿 回填 及路 面臨 鋪 作業   提前 於 早上 8 點開放 機車 小型 轎車 通行   預訂 中午 12 點 全面 通行     南港 警方 昨天 晚間 近 6 點 42 分   接獲 南港路 3 段 47 巷 與 昆陽街 60 巷 交叉路口 機車 停等區 地層下陷   下陷 面積長 約 2 公尺   寬約 2 公尺   深度 約 2 公尺   幸無人 受傷   員警劃 設 警戒 線   副 市長 李 四川 指示 區 公所   新工處 調派 重機 具開 挖   確認 坍塌 原因     經設 置 前進 指揮 所   水利 處 擴大開 挖 作業   確認 是 雨水 連 接管 脫管 造成   連夜 搶 修後已 經修 復 完成 並 回填 路面   今天 早上 已經 提前 恢 復 通車   後 續 新 工處 將會 以 透地雷達 檢測 無 其他 路面 下 空洞  ', '4 個 月 5 起 道路 塌陷   工務局 ︰ 多 與 地下 管線 有關   市府 已 要求 總體檢   〔 記者 魏瑾筠   何玉華 ／ 台北 報導 〕 台北市 昨晚 萬華區 昆明 路 一處 建案 工地 旁   又 發生 地層下陷   是 近四個 月 來 第五次 市區 道路 塌陷   昨晚 塌陷 原因 仍 不明   不 排除 是 豪 大雨 所致   台北市 政府 工務局 說   前 四次 塌陷 都 不是 車輛 輾壓 破損   而是 與 地下 管線 有關   已擬定 防範 措施   台北市 副 市長 李 四川 則 提到 都 與 極端 氣候 溫室 效應 有關   呼籲 重視民眾 看不到 基礎 建設   民進 黨 議員林 延鳳   陳 怡 君質疑 是   甩鍋     認為 市府 應積極 研擬 極端 氣候 下   管線 老舊 問題 對策     萬華 昆明 路建案 工地 旁   又 發生 地層下陷   李 四川 回應 議員質疑 說   絕非   甩鍋     氣候變遷 造成 豪 大雨 並 沖 刷 排水管 涵   導致 有些 本來 就 破裂 老舊 排水管 損裂 更 嚴重   民生 東路 管線 就是 超過 廿年   而 上次 南京 西路 塌陷 後   他 已 要求 衛工處 總體 檢老舊 管線 箱涵   若 需要 維修 或 更 換會 立即 處理     萬華 昨晚 塌陷 地點 在建 案 工地 旁   下陷 面積 約 長 三 公尺   寬 兩 公尺   深度 一 ． 五 公尺   晚間 已經 完成 回填   十九日 民生 東路 塌陷 處   完成 回填   水利 處 勘查 是 側溝 破 損導致 地層 被 掏空   將進 行側 溝修 復     豪 大雨 沖 刷   導致 破裂 排水管 損害 更 嚴重   工務局 說明   這幾起 道路 塌陷 都 不是 車輛 輾壓 造成   五月 十三日 崇德 街是 因建案 開 挖 地下 基礎   連續 壁 滲水 造成 地下水 湧入 基地   帶 走 周邊 道路 沙土 而 出現 坑洞   七月 十日 南京 西路 是 軟弱 地層 長 期受 潮汐 影響 地下水位   土壤 承載力 不佳   導致 污水 管接 頭 鬆 脫 錯 位   土沙 沿管線 破 損處 流失     而 南港路 許多 建案 施工   四 七巷 道路 狹小   排水 箱涵 接側 溝的連 接管 無法 深埋   疑似 重車 來 往 頻繁 造成 連 接管 間 縫隙   地下水 帶 走 土沙 而 地層下陷   民生 東路 是 道路 側溝 溝體 老舊 破損   加上 近期 下雨 排水 掏 涮 所致     李 四川 臉書 有感 而 發說   近來 國內外 天災 不斷   包含 國內 南投 豪 大雨   高雄 積 淹水   北市 路面 塌陷 等   都 與 極端 氣候 溫室 效應 有關   希望 每 一位 在位者 都 能 對 百姓 看不到 基礎 建設 工程   多用 一點心     議員 ︰ 應 研擬 極端 氣候 管線 老舊 對策   林延鳳 認為 李 四川 說 法 是 甩鍋   卸責   有失 專業   直指 四起 道路 塌陷   都 是 疏 於 督管 工程 品質   人禍     不應 歸咎 於 天災   陳 怡君 說   極端 氣候 不能 成為 推卸 市政 理由 與 藉口   市府 應針 對 路面 總體檢   更換 或 整修 老舊 管線 箱涵   積極 研擬 因應 極端 氣候 公共 管線 老舊 對策  ']</t>
         </is>
       </c>
     </row>

</xml_diff>